<commit_message>
Ajout d'un identifiant pour chaque contrôle, et modification de l'ordre
</commit_message>
<xml_diff>
--- a/Documentation/Controleur.xlsx
+++ b/Documentation/Controleur.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="52">
   <si>
     <t>Famille</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>Mauvaise version de la C3A</t>
+  </si>
+  <si>
+    <t>Numéro de Contrôle</t>
   </si>
 </sst>
 </file>
@@ -748,595 +751,674 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="41.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="41.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
-      <c r="B2" s="16"/>
+      <c r="B2" s="15"/>
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
-      <c r="G2" s="12"/>
-    </row>
-    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="G2" s="16"/>
+      <c r="H2" s="12"/>
+    </row>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="E4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="G4" s="19" t="s">
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="7" t="s">
+    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>8</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="7" t="s">
+      <c r="B10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="8"/>
+      <c r="H10" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>9</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="B11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="8"/>
+      <c r="H11" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="8"/>
+      <c r="H12" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="8"/>
+      <c r="H13" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="8"/>
+      <c r="H16" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>15</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="8" t="s">
+      <c r="B17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="8"/>
+      <c r="H17" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>16</v>
       </c>
-      <c r="F6" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="8" t="s">
+      <c r="B18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="8"/>
+      <c r="H18" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" s="8"/>
+      <c r="H19" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>18</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="8" t="s">
+      <c r="B20" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="8"/>
+      <c r="H20" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>19</v>
       </c>
-      <c r="F8" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" s="9" t="s">
+      <c r="B21" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G21" s="8"/>
+      <c r="H21" s="9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="8" t="s">
+    <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="F9" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="8" t="s">
+      <c r="B22" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G22" s="7"/>
+      <c r="H22" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>21</v>
       </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="8" t="s">
+      <c r="B23" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" s="8"/>
+      <c r="H23" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>22</v>
       </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="9" t="s">
+      <c r="B24" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G24" s="8"/>
+      <c r="H24" s="9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="7" t="s">
+    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>23</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="B25" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G25" s="8"/>
+      <c r="H25" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>24</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="8" t="s">
+      <c r="B26" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26" s="8"/>
+      <c r="H26" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>25</v>
       </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F19" s="8"/>
-      <c r="G19" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F20" s="8"/>
-      <c r="G20" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F21" s="8"/>
-      <c r="G21" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F22" s="7"/>
-      <c r="G22" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F23" s="8"/>
-      <c r="G23" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F24" s="8"/>
-      <c r="G24" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="F25" s="8"/>
-      <c r="G25" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F26" s="8"/>
-      <c r="G26" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>17</v>
+      <c r="B27" s="13" t="s">
+        <v>7</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E27" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F27" s="10"/>
-      <c r="G27" s="9" t="s">
+      <c r="G27" s="10"/>
+      <c r="H27" s="9" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- Ajout des commentaires - Correction de bug dans contrôle 2: mauvaise variable - Amélioration de code - Ajout de la gestion d'un dictionnaire permettant de selectionner ou non un controle (ce dictionnaire sera, à terme, une extraction d'un fichier xls) - Correction d'un bug du contrôle 4, les données étaient mal extraites
</commit_message>
<xml_diff>
--- a/Documentation/Controleur.xlsx
+++ b/Documentation/Controleur.xlsx
@@ -770,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
- Ajout des contrôles 13 et 14 - Mise à jour du fichier controlleur.xlsx avec de nouveaux libellés et formats d'erreur - Correction du controle 1 - Quand il y a la C3A dans les deux sources, on affiche que dans source A - Dans contrôle 7, une seule ligne par troncon même si point A ET point B sont incorrects - Mise à jour de la première ligne du C3A puisqu'elle est différente dans la dernière version - Simplification du modele d'erreur en fonction, pour les C3A - Eviter de charger des XLSX temporaires ou invisibles - On vérifie maintenant 2 colonnes pour savoir si la ligne est vide ou non
</commit_message>
<xml_diff>
--- a/Documentation/Controleur.xlsx
+++ b/Documentation/Controleur.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="72">
   <si>
     <t>Famille</t>
   </si>
@@ -102,18 +102,12 @@
     <t>Incohérence du type de point technique [Colonne D ou Colonne F]entre la C3A et QGIS</t>
   </si>
   <si>
-    <t>Information de sous tubage incomplète pour le tronçon [Colonne D - Colonne F]. La colonne I doit être renseigné</t>
-  </si>
-  <si>
     <t>Vérifier que le couple (colonne C, colonne E) ne forme pas une combinaison dans la liste suivante : [CT – CT], [C – CT], [CT – C], [CT– P], [CT – A], [A – CT], [P-CT]</t>
   </si>
   <si>
     <t>Dans le cas d'une liaison [C - C], la colonne H doit prendre les valeurs contenues dans cette liste : ["28","32","45","60","80","100","150","Sous-tubage existant","caniveau","galerie"]</t>
   </si>
   <si>
-    <t>Information de diamètre de l'alvéole est mal renseigné pour la liaison [Colonne D - Colonne F]</t>
-  </si>
-  <si>
     <t>Dans le cas d'une liaison [C - IMB], la colonne F doit être vide</t>
   </si>
   <si>
@@ -150,9 +144,6 @@
     <t>Mineure</t>
   </si>
   <si>
-    <t>Mauvaise con</t>
-  </si>
-  <si>
     <t>version</t>
   </si>
   <si>
@@ -223,6 +214,27 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Format de nommage incorrect</t>
+  </si>
+  <si>
+    <t>Information de sous tubage incomplète pour le tronçon. La colonne I doit être renseigné</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [Colonne D - Colonne F]</t>
+  </si>
+  <si>
+    <t>[Colonne D - Colonne F]</t>
+  </si>
+  <si>
+    <t>Information de diamètre de l'alvéole mal renseigné</t>
+  </si>
+  <si>
+    <t>Longueur de tronçon / portée incorrect</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [Colonne D]</t>
   </si>
 </sst>
 </file>
@@ -829,10 +841,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -853,7 +866,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>0</v>
@@ -871,7 +884,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H1" s="9" t="s">
         <v>5</v>
@@ -880,34 +893,34 @@
         <v>6</v>
       </c>
       <c r="J1" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="O1" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="P1" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="Q1" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="R1" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="S1" s="21" t="s">
         <v>57</v>
-      </c>
-      <c r="N1" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="O1" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="P1" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q1" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="R1" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="S1" s="21" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="30" x14ac:dyDescent="0.25">
@@ -918,46 +931,46 @@
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I2" s="14" t="s">
         <v>10</v>
       </c>
       <c r="J2" s="23"/>
       <c r="K2" s="22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="L2" s="23"/>
       <c r="M2" s="22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="N2" s="23"/>
       <c r="O2" s="22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="P2" s="22"/>
       <c r="Q2" s="22"/>
       <c r="R2" s="23"/>
       <c r="S2" s="22" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19">
         <v>2</v>
       </c>
@@ -971,16 +984,16 @@
         <v>9</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>10</v>
@@ -996,7 +1009,7 @@
       <c r="R3" s="23"/>
       <c r="S3" s="22"/>
     </row>
-    <row r="4" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19">
         <v>3</v>
       </c>
@@ -1007,7 +1020,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>9</v>
@@ -1016,13 +1029,13 @@
         <v>14</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J4" s="23"/>
       <c r="K4" s="22"/>
@@ -1046,7 +1059,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>12</v>
@@ -1054,7 +1067,9 @@
       <c r="F5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="6"/>
+      <c r="G5" s="6" t="s">
+        <v>71</v>
+      </c>
       <c r="H5" s="6" t="s">
         <v>25</v>
       </c>
@@ -1063,24 +1078,24 @@
       </c>
       <c r="J5" s="23"/>
       <c r="K5" s="22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="L5" s="23"/>
       <c r="M5" s="22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="N5" s="23"/>
       <c r="O5" s="22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="P5" s="22"/>
       <c r="Q5" s="22"/>
       <c r="R5" s="23"/>
       <c r="S5" s="22" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="19">
         <v>5</v>
       </c>
@@ -1094,7 +1109,7 @@
         <v>9</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>17</v>
@@ -1104,7 +1119,7 @@
         <v>26</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J6" s="23"/>
       <c r="K6" s="22"/>
@@ -1117,7 +1132,7 @@
       <c r="R6" s="23"/>
       <c r="S6" s="22"/>
     </row>
-    <row r="7" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="19">
         <v>6</v>
       </c>
@@ -1128,20 +1143,22 @@
         <v>16</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="6"/>
+      <c r="G7" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="H7" s="6" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J7" s="23"/>
       <c r="K7" s="22"/>
@@ -1165,38 +1182,40 @@
         <v>16</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="6"/>
+      <c r="G8" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="H8" s="6" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J8" s="23"/>
       <c r="K8" s="22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="L8" s="23"/>
       <c r="M8" s="22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="N8" s="23"/>
       <c r="O8" s="22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="P8" s="22"/>
       <c r="Q8" s="22"/>
       <c r="R8" s="23"/>
       <c r="S8" s="22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="30" x14ac:dyDescent="0.25">
@@ -1210,36 +1229,40 @@
         <v>16</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+      <c r="G9" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>70</v>
+      </c>
       <c r="I9" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J9" s="23"/>
       <c r="K9" s="22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="L9" s="23"/>
       <c r="M9" s="22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="N9" s="23"/>
       <c r="O9" s="22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="P9" s="22"/>
       <c r="Q9" s="22"/>
       <c r="R9" s="23"/>
       <c r="S9" s="22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="45" x14ac:dyDescent="0.25">
@@ -1253,10 +1276,10 @@
         <v>16</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>21</v>
@@ -1264,7 +1287,7 @@
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J10" s="23"/>
       <c r="K10" s="22"/>
@@ -1288,10 +1311,10 @@
         <v>16</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>22</v>
@@ -1299,7 +1322,7 @@
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J11" s="23"/>
       <c r="K11" s="22"/>
@@ -1323,10 +1346,10 @@
         <v>16</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>23</v>
@@ -1334,7 +1357,7 @@
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J12" s="23"/>
       <c r="K12" s="22"/>
@@ -1358,38 +1381,40 @@
         <v>16</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G13" s="6"/>
+        <v>27</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="H13" s="6" t="s">
         <v>24</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J13" s="23"/>
       <c r="K13" s="22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="L13" s="23"/>
       <c r="M13" s="22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="N13" s="23"/>
       <c r="O13" s="22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="P13" s="22"/>
       <c r="Q13" s="22"/>
       <c r="R13" s="23"/>
       <c r="S13" s="22" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="90" x14ac:dyDescent="0.25">
@@ -1403,20 +1428,22 @@
         <v>16</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="G14" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="H14" s="6" t="s">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J14" s="23"/>
       <c r="K14" s="22"/>
@@ -1440,18 +1467,18 @@
         <v>16</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J15" s="23"/>
       <c r="K15" s="22"/>
@@ -1475,18 +1502,18 @@
         <v>16</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J16" s="23"/>
       <c r="K16" s="22"/>
@@ -1510,18 +1537,18 @@
         <v>16</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J17" s="23"/>
       <c r="K17" s="22"/>
@@ -1545,18 +1572,18 @@
         <v>16</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J18" s="23"/>
       <c r="K18" s="22"/>
@@ -1580,18 +1607,18 @@
         <v>16</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J19" s="23"/>
       <c r="K19" s="22"/>
@@ -1615,18 +1642,18 @@
         <v>16</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J20" s="23"/>
       <c r="K20" s="22"/>
@@ -1650,18 +1677,18 @@
         <v>16</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G21" s="6"/>
       <c r="H21" s="5"/>
       <c r="I21" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J21" s="23"/>
       <c r="K21" s="22"/>
@@ -1685,18 +1712,18 @@
         <v>16</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
       <c r="I22" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J22" s="23"/>
       <c r="K22" s="22"/>
@@ -1720,18 +1747,18 @@
         <v>16</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
       <c r="I23" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J23" s="23"/>
       <c r="K23" s="22"/>
@@ -1755,18 +1782,18 @@
         <v>16</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
       <c r="I24" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J24" s="23"/>
       <c r="K24" s="22"/>
@@ -1790,18 +1817,18 @@
         <v>16</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
       <c r="I25" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J25" s="23"/>
       <c r="K25" s="22"/>
@@ -1825,18 +1852,18 @@
         <v>16</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
       <c r="I26" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J26" s="23"/>
       <c r="K26" s="22"/>
@@ -1850,7 +1877,20 @@
       <c r="S26" s="22"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I26"/>
+  <autoFilter ref="A1:I26">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="[Fichier C3A]"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="4">
+      <filters>
+        <filter val="[Fichier C3A]"/>
+        <filter val="[Fichier C7]"/>
+        <filter val="Dossier poteaux"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
- Mise à jour Controleur.xlsx des champs concernés et sources puis suppression d'une ligne doublon - Dans le contrôle 7, vérifier le champ seulement s'il n'est pas vider - Mise à jour du programme en tenant compte du contrôle supprimé dans le xlsx - Pour contrôle 13, Les valeurs numériques des excels sont casté en int puis str pour avoir un format comparable facilement - Ajout des contrôles 15,16,17,18,19,20,21,22,23,24 - Mise à jour des messages - Ajout de la fonction permettant d'avoir l'indice selon la lettre, pour Excel
</commit_message>
<xml_diff>
--- a/Documentation/Controleur.xlsx
+++ b/Documentation/Controleur.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Controleur CA'!$A$1:$I$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Controleur CA'!$A$1:$I$25</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="73">
   <si>
     <t>Famille</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t xml:space="preserve"> [Colonne D]</t>
+  </si>
+  <si>
+    <t>[Vide]</t>
   </si>
 </sst>
 </file>
@@ -842,10 +845,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:S26"/>
+  <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -937,7 +940,7 @@
         <v>49</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>42</v>
@@ -1146,7 +1149,7 @@
         <v>49</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>18</v>
@@ -1185,7 +1188,7 @@
         <v>49</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>19</v>
@@ -1232,7 +1235,7 @@
         <v>49</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>20</v>
@@ -1279,12 +1282,14 @@
         <v>49</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="6"/>
+      <c r="G10" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="H10" s="6"/>
       <c r="I10" s="7" t="s">
         <v>40</v>
@@ -1384,7 +1389,7 @@
         <v>49</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>27</v>
@@ -1431,7 +1436,7 @@
         <v>49</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>28</v>
@@ -1470,12 +1475,14 @@
         <v>49</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="6"/>
+      <c r="G15" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="H15" s="6"/>
       <c r="I15" s="7" t="s">
         <v>40</v>
@@ -1505,12 +1512,14 @@
         <v>49</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="6"/>
+      <c r="G16" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="H16" s="6"/>
       <c r="I16" s="7" t="s">
         <v>40</v>
@@ -1540,12 +1549,14 @@
         <v>49</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="6"/>
+      <c r="G17" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="H17" s="6"/>
       <c r="I17" s="7" t="s">
         <v>40</v>
@@ -1575,12 +1586,14 @@
         <v>49</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G18" s="6"/>
+        <v>33</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="H18" s="6"/>
       <c r="I18" s="7" t="s">
         <v>40</v>
@@ -1596,7 +1609,7 @@
       <c r="R18" s="23"/>
       <c r="S18" s="22"/>
     </row>
-    <row r="19" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="19">
         <v>18</v>
       </c>
@@ -1610,12 +1623,14 @@
         <v>49</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" s="6"/>
+        <v>31</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="H19" s="6"/>
       <c r="I19" s="7" t="s">
         <v>40</v>
@@ -1631,7 +1646,7 @@
       <c r="R19" s="23"/>
       <c r="S19" s="22"/>
     </row>
-    <row r="20" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="19">
         <v>19</v>
       </c>
@@ -1645,13 +1660,15 @@
         <v>49</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H20" s="5"/>
       <c r="I20" s="7" t="s">
         <v>40</v>
       </c>
@@ -1680,13 +1697,15 @@
         <v>49</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G21" s="6"/>
-      <c r="H21" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H21" s="6"/>
       <c r="I21" s="7" t="s">
         <v>40</v>
       </c>
@@ -1715,12 +1734,14 @@
         <v>49</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G22" s="6"/>
+        <v>35</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="H22" s="6"/>
       <c r="I22" s="7" t="s">
         <v>40</v>
@@ -1736,7 +1757,7 @@
       <c r="R22" s="23"/>
       <c r="S22" s="22"/>
     </row>
-    <row r="23" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="19">
         <v>22</v>
       </c>
@@ -1750,12 +1771,14 @@
         <v>49</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G23" s="6"/>
+        <v>36</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="H23" s="6"/>
       <c r="I23" s="7" t="s">
         <v>40</v>
@@ -1785,12 +1808,14 @@
         <v>49</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G24" s="6"/>
+        <v>37</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="H24" s="6"/>
       <c r="I24" s="7" t="s">
         <v>40</v>
@@ -1806,27 +1831,29 @@
       <c r="R24" s="23"/>
       <c r="S24" s="22"/>
     </row>
-    <row r="25" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="19">
+    <row r="25" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="20">
         <v>24</v>
       </c>
-      <c r="B25" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" s="5" t="s">
+      <c r="B25" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
+        <v>72</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H25" s="8"/>
       <c r="I25" s="7" t="s">
         <v>40</v>
       </c>
@@ -1841,43 +1868,8 @@
       <c r="R25" s="23"/>
       <c r="S25" s="22"/>
     </row>
-    <row r="26" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="20">
-        <v>25</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="J26" s="23"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="23"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="23"/>
-      <c r="O26" s="22"/>
-      <c r="P26" s="22"/>
-      <c r="Q26" s="22"/>
-      <c r="R26" s="23"/>
-      <c r="S26" s="22"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:I26">
+  <autoFilter ref="A1:I25">
     <filterColumn colId="3">
       <filters>
         <filter val="[Fichier C3A]"/>
@@ -1892,7 +1884,7 @@
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
- Ajout du contrôle 9 - Correction du contrôle 13 - Ajout du libellé d'erreur dans le Controleur.xlsx
</commit_message>
<xml_diff>
--- a/Documentation/Controleur.xlsx
+++ b/Documentation/Controleur.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="74">
   <si>
     <t>Famille</t>
   </si>
@@ -238,6 +238,9 @@
   </si>
   <si>
     <t>[Vide]</t>
+  </si>
+  <si>
+    <t>Les valeurs ne respectent pas les listes déroulantes</t>
   </si>
 </sst>
 </file>
@@ -847,8 +850,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1290,7 +1293,9 @@
       <c r="G10" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="H10" s="6"/>
+      <c r="H10" s="6" t="s">
+        <v>73</v>
+      </c>
       <c r="I10" s="7" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
- Remplissage de tous les libellés dans le programme et l'excel - Remplissage des champs concernés dans l'excel et suppression d'une ligne doublon (contrôle 14) - Suppression du contrôle 14 dans le programme - Réactivation de tous les tests dans contrôle 9 - Ajout des contrôles 10 et 11 pour la C7 - modele_erreur_c3a a été complexifié pour être utilisé par + de cas
</commit_message>
<xml_diff>
--- a/Documentation/Controleur.xlsx
+++ b/Documentation/Controleur.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Controleur CA'!$A$1:$I$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Controleur CA'!$A$1:$I$24</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="81">
   <si>
     <t>Famille</t>
   </si>
@@ -234,13 +234,34 @@
     <t>Longueur de tronçon / portée incorrect</t>
   </si>
   <si>
-    <t xml:space="preserve"> [Colonne D]</t>
-  </si>
-  <si>
     <t>[Vide]</t>
   </si>
   <si>
     <t>Les valeurs ne respectent pas les listes déroulantes</t>
+  </si>
+  <si>
+    <t>Fichier C7 manquant</t>
+  </si>
+  <si>
+    <t>Appui manquant dans la C7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [Colonne D ou Colonne F]</t>
+  </si>
+  <si>
+    <t>La colonne F doit être vide</t>
+  </si>
+  <si>
+    <t>La colonne G doit contenir la valeur "7"</t>
+  </si>
+  <si>
+    <t>La colonne H doit contenir la valeur "transition"</t>
+  </si>
+  <si>
+    <t>La colonne H doit contenir la valeur "adduction"</t>
+  </si>
+  <si>
+    <t>Les colonne B et D doivent être vide</t>
   </si>
 </sst>
 </file>
@@ -848,10 +869,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:S25"/>
+  <dimension ref="A1:S24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -943,7 +964,7 @@
         <v>49</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>42</v>
@@ -1074,7 +1095,7 @@
         <v>15</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>25</v>
@@ -1152,7 +1173,7 @@
         <v>49</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>18</v>
@@ -1191,7 +1212,7 @@
         <v>49</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>19</v>
@@ -1238,7 +1259,7 @@
         <v>49</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>20</v>
@@ -1285,7 +1306,7 @@
         <v>49</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>21</v>
@@ -1294,7 +1315,7 @@
         <v>67</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I10" s="7" t="s">
         <v>40</v>
@@ -1329,8 +1350,12 @@
       <c r="F11" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="G11" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>73</v>
+      </c>
       <c r="I11" s="7" t="s">
         <v>39</v>
       </c>
@@ -1364,8 +1389,12 @@
       <c r="F12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
+      <c r="G12" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>74</v>
+      </c>
       <c r="I12" s="7" t="s">
         <v>39</v>
       </c>
@@ -1394,7 +1423,7 @@
         <v>49</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>27</v>
@@ -1441,7 +1470,7 @@
         <v>49</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>28</v>
@@ -1466,9 +1495,9 @@
       <c r="R14" s="23"/>
       <c r="S14" s="22"/>
     </row>
-    <row r="15" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="19">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" s="16" t="s">
         <v>7</v>
@@ -1480,15 +1509,17 @@
         <v>49</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="H15" s="6"/>
+      <c r="H15" s="6" t="s">
+        <v>79</v>
+      </c>
       <c r="I15" s="7" t="s">
         <v>40</v>
       </c>
@@ -1503,9 +1534,9 @@
       <c r="R15" s="23"/>
       <c r="S15" s="22"/>
     </row>
-    <row r="16" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="19">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>7</v>
@@ -1517,15 +1548,17 @@
         <v>49</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="H16" s="6"/>
+      <c r="H16" s="6" t="s">
+        <v>76</v>
+      </c>
       <c r="I16" s="7" t="s">
         <v>40</v>
       </c>
@@ -1540,9 +1573,9 @@
       <c r="R16" s="23"/>
       <c r="S16" s="22"/>
     </row>
-    <row r="17" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>7</v>
@@ -1554,15 +1587,17 @@
         <v>49</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G17" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="H17" s="6"/>
+      <c r="H17" s="6" t="s">
+        <v>77</v>
+      </c>
       <c r="I17" s="7" t="s">
         <v>40</v>
       </c>
@@ -1577,9 +1612,9 @@
       <c r="R17" s="23"/>
       <c r="S17" s="22"/>
     </row>
-    <row r="18" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="19">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" s="16" t="s">
         <v>7</v>
@@ -1591,15 +1626,17 @@
         <v>49</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="H18" s="6"/>
+      <c r="H18" s="6" t="s">
+        <v>76</v>
+      </c>
       <c r="I18" s="7" t="s">
         <v>40</v>
       </c>
@@ -1614,9 +1651,9 @@
       <c r="R18" s="23"/>
       <c r="S18" s="22"/>
     </row>
-    <row r="19" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="19">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" s="16" t="s">
         <v>7</v>
@@ -1628,15 +1665,17 @@
         <v>49</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="H19" s="6"/>
+      <c r="H19" s="5" t="s">
+        <v>78</v>
+      </c>
       <c r="I19" s="7" t="s">
         <v>40</v>
       </c>
@@ -1653,7 +1692,7 @@
     </row>
     <row r="20" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="19">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20" s="16" t="s">
         <v>7</v>
@@ -1665,15 +1704,17 @@
         <v>49</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G20" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="H20" s="5"/>
+      <c r="H20" s="6" t="s">
+        <v>77</v>
+      </c>
       <c r="I20" s="7" t="s">
         <v>40</v>
       </c>
@@ -1690,7 +1731,7 @@
     </row>
     <row r="21" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="19">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>7</v>
@@ -1702,15 +1743,17 @@
         <v>49</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G21" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="H21" s="6"/>
+      <c r="H21" s="6" t="s">
+        <v>78</v>
+      </c>
       <c r="I21" s="7" t="s">
         <v>40</v>
       </c>
@@ -1725,9 +1768,9 @@
       <c r="R21" s="23"/>
       <c r="S21" s="22"/>
     </row>
-    <row r="22" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="19">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" s="16" t="s">
         <v>7</v>
@@ -1739,15 +1782,17 @@
         <v>49</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="H22" s="6"/>
+      <c r="H22" s="6" t="s">
+        <v>76</v>
+      </c>
       <c r="I22" s="7" t="s">
         <v>40</v>
       </c>
@@ -1764,7 +1809,7 @@
     </row>
     <row r="23" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="19">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" s="16" t="s">
         <v>7</v>
@@ -1776,15 +1821,17 @@
         <v>49</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="H23" s="6"/>
+      <c r="H23" s="6" t="s">
+        <v>80</v>
+      </c>
       <c r="I23" s="7" t="s">
         <v>40</v>
       </c>
@@ -1799,29 +1846,31 @@
       <c r="R23" s="23"/>
       <c r="S23" s="22"/>
     </row>
-    <row r="24" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="19">
-        <v>23</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="5" t="s">
+    <row r="24" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="20">
+        <v>24</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>37</v>
+        <v>71</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="H24" s="6"/>
+      <c r="H24" s="6" t="s">
+        <v>78</v>
+      </c>
       <c r="I24" s="7" t="s">
         <v>40</v>
       </c>
@@ -1836,45 +1885,8 @@
       <c r="R24" s="23"/>
       <c r="S24" s="22"/>
     </row>
-    <row r="25" spans="1:19" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="20">
-        <v>24</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="H25" s="8"/>
-      <c r="I25" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="J25" s="23"/>
-      <c r="K25" s="22"/>
-      <c r="L25" s="23"/>
-      <c r="M25" s="22"/>
-      <c r="N25" s="23"/>
-      <c r="O25" s="22"/>
-      <c r="P25" s="22"/>
-      <c r="Q25" s="22"/>
-      <c r="R25" s="23"/>
-      <c r="S25" s="22"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:I25">
+  <autoFilter ref="A1:I24">
     <filterColumn colId="3">
       <filters>
         <filter val="[Fichier C3A]"/>

</xml_diff>

<commit_message>
** Version v4 ** - Renommer Commande d'accès en Commande - Suppression des fichiers d'installation inutiles - Forcer les contrôles à être effectué par le dpt testv1 pour l'instant - Suppression des messages sur terminal - contrôles sélectionnés en lisant le fichier controleur.xlsx - Possibilité d'arrêter les contrôles si la c3a n'a pas la bonne version (commenté) - message de succès mis sous fonction - Correction de bug de configuration (suite à la modification massive des variables avec le nouveau système de dictionnaire pour les variables spécifiques au département) - Réorganisation de definitions.py au niveau de l'ordre, pour gérer l'existance de la fonction log au moment des erreurs - Ajout du point technique dans la configuration par département - Commenter certaines variables de config par département en attendant de trouver comment les gérer - log sans extension txt - Dans le dossier installation, ajout du script permettant de créer l'installateur
</commit_message>
<xml_diff>
--- a/Documentation/Controleur.xlsx
+++ b/Documentation/Controleur.xlsx
@@ -96,9 +96,6 @@
     <t>Combinaison interdite</t>
   </si>
   <si>
-    <t>Fiche poteaux [Colonne D ou Colonne F] manquante</t>
-  </si>
-  <si>
     <t>Vérifier que le couple (colonne C, colonne E) ne forme pas une combinaison dans la liste suivante : [CT – CT], [C – CT], [CT – C], [CT– P], [CT – A], [A – CT], [P-CT]</t>
   </si>
   <si>
@@ -268,6 +265,9 @@
   </si>
   <si>
     <t>Incohérence du type de point technique entre la C3A et QGIS</t>
+  </si>
+  <si>
+    <t>Fiche poteaux manquante</t>
   </si>
 </sst>
 </file>
@@ -871,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,7 +893,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -911,7 +911,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>5</v>
@@ -920,34 +920,34 @@
         <v>6</v>
       </c>
       <c r="J1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -958,45 +958,45 @@
         <v>7</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>41</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>42</v>
       </c>
       <c r="I2" s="9" t="s">
         <v>10</v>
       </c>
       <c r="J2" s="10"/>
       <c r="K2" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L2" s="10"/>
       <c r="M2" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N2" s="10"/>
       <c r="O2" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P2" s="11"/>
       <c r="Q2" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R2" s="10"/>
       <c r="S2" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:19" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -1013,16 +1013,16 @@
         <v>9</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F3" s="21" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="21" t="s">
         <v>50</v>
-      </c>
-      <c r="H3" s="21" t="s">
-        <v>51</v>
       </c>
       <c r="I3" s="22" t="s">
         <v>10</v>
@@ -1049,7 +1049,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>9</v>
@@ -1058,13 +1058,13 @@
         <v>14</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I4" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J4" s="10"/>
       <c r="K4" s="11"/>
@@ -1088,7 +1088,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E5" s="14" t="s">
         <v>12</v>
@@ -1097,33 +1097,33 @@
         <v>15</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>25</v>
+        <v>82</v>
       </c>
       <c r="I5" s="16" t="s">
         <v>10</v>
       </c>
       <c r="J5" s="10"/>
       <c r="K5" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L5" s="10"/>
       <c r="M5" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N5" s="10"/>
       <c r="O5" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R5" s="10"/>
       <c r="S5" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:19" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1140,19 +1140,19 @@
         <v>9</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F6" s="15" t="s">
         <v>17</v>
       </c>
       <c r="G6" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="H6" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="H6" s="15" t="s">
-        <v>82</v>
-      </c>
       <c r="I6" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J6" s="10"/>
       <c r="K6" s="11"/>
@@ -1176,42 +1176,42 @@
         <v>16</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F7" s="15" t="s">
         <v>18</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J7" s="10"/>
       <c r="K7" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L7" s="10"/>
       <c r="M7" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N7" s="10"/>
       <c r="O7" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P7" s="11"/>
       <c r="Q7" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R7" s="10"/>
       <c r="S7" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:19" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -1225,42 +1225,42 @@
         <v>16</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F8" s="15" t="s">
         <v>19</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J8" s="10"/>
       <c r="K8" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L8" s="10"/>
       <c r="M8" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N8" s="10"/>
       <c r="O8" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P8" s="11"/>
       <c r="Q8" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R8" s="10"/>
       <c r="S8" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1274,42 +1274,42 @@
         <v>16</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F9" s="15" t="s">
         <v>20</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J9" s="10"/>
       <c r="K9" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L9" s="10"/>
       <c r="M9" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N9" s="10"/>
       <c r="O9" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P9" s="11"/>
       <c r="Q9" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R9" s="10"/>
       <c r="S9" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:19" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1323,42 +1323,42 @@
         <v>16</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F10" s="15" t="s">
         <v>21</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L10" s="10"/>
       <c r="M10" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N10" s="10"/>
       <c r="O10" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P10" s="11"/>
       <c r="Q10" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R10" s="10"/>
       <c r="S10" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:19" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -1372,42 +1372,42 @@
         <v>16</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F11" s="15" t="s">
         <v>22</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J11" s="10"/>
       <c r="K11" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L11" s="10"/>
       <c r="M11" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N11" s="10"/>
       <c r="O11" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P11" s="11"/>
       <c r="Q11" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R11" s="10"/>
       <c r="S11" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:19" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -1421,42 +1421,42 @@
         <v>16</v>
       </c>
       <c r="D12" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="14" t="s">
         <v>48</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>49</v>
       </c>
       <c r="F12" s="15" t="s">
         <v>23</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J12" s="10"/>
       <c r="K12" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L12" s="10"/>
       <c r="M12" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N12" s="10"/>
       <c r="O12" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P12" s="11"/>
       <c r="Q12" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R12" s="10"/>
       <c r="S12" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:19" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -1470,42 +1470,42 @@
         <v>16</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H13" s="15" t="s">
         <v>24</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J13" s="10"/>
       <c r="K13" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L13" s="10"/>
       <c r="M13" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N13" s="10"/>
       <c r="O13" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P13" s="11"/>
       <c r="Q13" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R13" s="10"/>
       <c r="S13" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:19" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -1519,42 +1519,42 @@
         <v>16</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G14" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="H14" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="H14" s="15" t="s">
-        <v>67</v>
-      </c>
       <c r="I14" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J14" s="10"/>
       <c r="K14" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L14" s="10"/>
       <c r="M14" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N14" s="10"/>
       <c r="O14" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P14" s="11"/>
       <c r="Q14" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R14" s="10"/>
       <c r="S14" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:19" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1568,42 +1568,42 @@
         <v>16</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I15" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J15" s="10"/>
       <c r="K15" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L15" s="10"/>
       <c r="M15" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N15" s="10"/>
       <c r="O15" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P15" s="11"/>
       <c r="Q15" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R15" s="10"/>
       <c r="S15" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1617,42 +1617,42 @@
         <v>16</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I16" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J16" s="10"/>
       <c r="K16" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L16" s="10"/>
       <c r="M16" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N16" s="10"/>
       <c r="O16" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P16" s="11"/>
       <c r="Q16" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R16" s="10"/>
       <c r="S16" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:19" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1666,42 +1666,42 @@
         <v>16</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I17" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J17" s="10"/>
       <c r="K17" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L17" s="10"/>
       <c r="M17" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N17" s="10"/>
       <c r="O17" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P17" s="11"/>
       <c r="Q17" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R17" s="10"/>
       <c r="S17" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1715,42 +1715,42 @@
         <v>16</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I18" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J18" s="10"/>
       <c r="K18" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L18" s="10"/>
       <c r="M18" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N18" s="10"/>
       <c r="O18" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P18" s="11"/>
       <c r="Q18" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R18" s="10"/>
       <c r="S18" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:19" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1764,42 +1764,42 @@
         <v>16</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I19" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J19" s="10"/>
       <c r="K19" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L19" s="10"/>
       <c r="M19" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N19" s="10"/>
       <c r="O19" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P19" s="11"/>
       <c r="Q19" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R19" s="10"/>
       <c r="S19" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:19" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1813,42 +1813,42 @@
         <v>16</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I20" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J20" s="10"/>
       <c r="K20" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L20" s="10"/>
       <c r="M20" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N20" s="10"/>
       <c r="O20" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P20" s="11"/>
       <c r="Q20" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R20" s="10"/>
       <c r="S20" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:19" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1862,42 +1862,42 @@
         <v>16</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I21" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J21" s="10"/>
       <c r="K21" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L21" s="10"/>
       <c r="M21" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N21" s="10"/>
       <c r="O21" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P21" s="11"/>
       <c r="Q21" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R21" s="10"/>
       <c r="S21" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1911,42 +1911,42 @@
         <v>16</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I22" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J22" s="10"/>
       <c r="K22" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L22" s="10"/>
       <c r="M22" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N22" s="10"/>
       <c r="O22" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P22" s="11"/>
       <c r="Q22" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R22" s="10"/>
       <c r="S22" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1960,42 +1960,42 @@
         <v>16</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I23" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J23" s="10"/>
       <c r="K23" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L23" s="10"/>
       <c r="M23" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N23" s="10"/>
       <c r="O23" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P23" s="11"/>
       <c r="Q23" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R23" s="10"/>
       <c r="S23" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:19" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -2009,42 +2009,42 @@
         <v>16</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F24" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I24" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J24" s="10"/>
       <c r="K24" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L24" s="10"/>
       <c r="M24" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N24" s="10"/>
       <c r="O24" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P24" s="11"/>
       <c r="Q24" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R24" s="10"/>
       <c r="S24" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -2079,15 +2079,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document Microsoft Word" ma:contentTypeID="0x01010066910ADB61686C45A75A7A744D7D5C8E0022B63E0AEFBB2040BF2A3B1B4BE32EE5" ma:contentTypeVersion="4" ma:contentTypeDescription="Document Microsoft Word vierge." ma:contentTypeScope="" ma:versionID="0a4943d90c7214e3c95a70ccb3c8346b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c97f8e9-86c7-4e99-9925-cc9540b321fe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eeaa8661ba6ba22f90735bcd04aade41" ns2:_="">
     <xsd:import namespace="9c97f8e9-86c7-4e99-9925-cc9540b321fe"/>
@@ -2290,6 +2281,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2305,13 +2305,37 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F02C15CB-09E5-4D58-8C63-77232C75BB18}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8B2112A-C178-4B00-8690-1CA741C188F5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9c97f8e9-86c7-4e99-9925-cc9540b321fe"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8B2112A-C178-4B00-8690-1CA741C188F5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F02C15CB-09E5-4D58-8C63-77232C75BB18}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFD779FF-B039-4DC7-8903-586F168B5B9F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFD779FF-B039-4DC7-8903-586F168B5B9F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9c97f8e9-86c7-4e99-9925-cc9540b321fe"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
- Nouveau design de fenêtre - Menu déroulant à l'écran principal pour selectionner département, type livrable et zone - Gestion du paramétrage dynamique selon les 3 nouveaux critères et le nouveau format de Controleur.xlsx - Nouveau format de Controleur.xlsx pour avoir les contrôles par département, type livrable et zone
</commit_message>
<xml_diff>
--- a/Documentation/Controleur.xlsx
+++ b/Documentation/Controleur.xlsx
@@ -4,12 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="255" windowWidth="6915" windowHeight="6600"/>
+    <workbookView xWindow="480" yWindow="255" windowWidth="6915" windowHeight="6600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Controleur CA" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
+    <sheet name="CD21" sheetId="2" r:id="rId2"/>
+    <sheet name="CD39" sheetId="3" r:id="rId3"/>
+    <sheet name="CD58" sheetId="4" r:id="rId4"/>
+    <sheet name="CD70" sheetId="5" r:id="rId5"/>
+    <sheet name="CD71" sheetId="6" r:id="rId6"/>
+    <sheet name="testv1" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Controleur CA'!$A$1:$I$24</definedName>
@@ -19,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="94">
   <si>
     <t>Famille</t>
   </si>
@@ -96,6 +100,9 @@
     <t>Combinaison interdite</t>
   </si>
   <si>
+    <t>Fiche poteaux [Colonne D ou Colonne F] manquante</t>
+  </si>
+  <si>
     <t>Vérifier que le couple (colonne C, colonne E) ne forme pas une combinaison dans la liste suivante : [CT – CT], [C – CT], [CT – C], [CT– P], [CT – A], [A – CT], [P-CT]</t>
   </si>
   <si>
@@ -267,7 +274,37 @@
     <t>Incohérence du type de point technique entre la C3A et QGIS</t>
   </si>
   <si>
-    <t>Fiche poteaux manquante</t>
+    <t>NRO AVP</t>
+  </si>
+  <si>
+    <t>Numéro de contrôle</t>
+  </si>
+  <si>
+    <t>NRO PRO</t>
+  </si>
+  <si>
+    <t>NRO EXE</t>
+  </si>
+  <si>
+    <t>Transport EXE</t>
+  </si>
+  <si>
+    <t>Transport PRO</t>
+  </si>
+  <si>
+    <t>SRO PRO</t>
+  </si>
+  <si>
+    <t>SRO EXE</t>
+  </si>
+  <si>
+    <t>Distributeur RBAL</t>
+  </si>
+  <si>
+    <t>Distributeur PRO</t>
+  </si>
+  <si>
+    <t>Distributeur EXE</t>
   </si>
 </sst>
 </file>
@@ -520,7 +557,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -562,6 +599,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -871,8 +914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,7 +936,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -911,7 +954,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>5</v>
@@ -920,34 +963,34 @@
         <v>6</v>
       </c>
       <c r="J1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="S1" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -958,45 +1001,45 @@
         <v>7</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>46</v>
-      </c>
       <c r="H2" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I2" s="9" t="s">
         <v>10</v>
       </c>
       <c r="J2" s="10"/>
       <c r="K2" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L2" s="10"/>
       <c r="M2" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N2" s="10"/>
       <c r="O2" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P2" s="11"/>
       <c r="Q2" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R2" s="10"/>
       <c r="S2" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:19" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -1013,16 +1056,16 @@
         <v>9</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F3" s="21" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="21" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H3" s="21" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I3" s="22" t="s">
         <v>10</v>
@@ -1049,7 +1092,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>9</v>
@@ -1058,13 +1101,13 @@
         <v>14</v>
       </c>
       <c r="G4" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="H4" s="15" t="s">
-        <v>43</v>
-      </c>
       <c r="I4" s="16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J4" s="10"/>
       <c r="K4" s="11"/>
@@ -1088,7 +1131,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E5" s="14" t="s">
         <v>12</v>
@@ -1097,33 +1140,33 @@
         <v>15</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>82</v>
+        <v>25</v>
       </c>
       <c r="I5" s="16" t="s">
         <v>10</v>
       </c>
       <c r="J5" s="10"/>
       <c r="K5" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L5" s="10"/>
       <c r="M5" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N5" s="10"/>
       <c r="O5" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R5" s="10"/>
       <c r="S5" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:19" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1140,19 +1183,19 @@
         <v>9</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F6" s="15" t="s">
         <v>17</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J6" s="10"/>
       <c r="K6" s="11"/>
@@ -1176,42 +1219,42 @@
         <v>16</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F7" s="15" t="s">
         <v>18</v>
       </c>
       <c r="G7" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="H7" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="H7" s="15" t="s">
-        <v>63</v>
-      </c>
       <c r="I7" s="16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J7" s="10"/>
       <c r="K7" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L7" s="10"/>
       <c r="M7" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N7" s="10"/>
       <c r="O7" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P7" s="11"/>
       <c r="Q7" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R7" s="10"/>
       <c r="S7" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:19" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -1225,42 +1268,42 @@
         <v>16</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F8" s="15" t="s">
         <v>19</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J8" s="10"/>
       <c r="K8" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L8" s="10"/>
       <c r="M8" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N8" s="10"/>
       <c r="O8" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P8" s="11"/>
       <c r="Q8" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R8" s="10"/>
       <c r="S8" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1274,42 +1317,42 @@
         <v>16</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F9" s="15" t="s">
         <v>20</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J9" s="10"/>
       <c r="K9" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L9" s="10"/>
       <c r="M9" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N9" s="10"/>
       <c r="O9" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P9" s="11"/>
       <c r="Q9" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R9" s="10"/>
       <c r="S9" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:19" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1323,42 +1366,42 @@
         <v>16</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F10" s="15" t="s">
         <v>21</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L10" s="10"/>
       <c r="M10" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N10" s="10"/>
       <c r="O10" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P10" s="11"/>
       <c r="Q10" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R10" s="10"/>
       <c r="S10" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:19" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -1372,42 +1415,42 @@
         <v>16</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F11" s="15" t="s">
         <v>22</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J11" s="10"/>
       <c r="K11" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L11" s="10"/>
       <c r="M11" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N11" s="10"/>
       <c r="O11" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P11" s="11"/>
       <c r="Q11" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R11" s="10"/>
       <c r="S11" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:19" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -1421,42 +1464,42 @@
         <v>16</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F12" s="15" t="s">
         <v>23</v>
       </c>
       <c r="G12" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="H12" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="H12" s="15" t="s">
-        <v>71</v>
-      </c>
       <c r="I12" s="16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J12" s="10"/>
       <c r="K12" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L12" s="10"/>
       <c r="M12" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N12" s="10"/>
       <c r="O12" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P12" s="11"/>
       <c r="Q12" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R12" s="10"/>
       <c r="S12" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:19" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -1470,42 +1513,42 @@
         <v>16</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H13" s="15" t="s">
         <v>24</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J13" s="10"/>
       <c r="K13" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L13" s="10"/>
       <c r="M13" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N13" s="10"/>
       <c r="O13" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P13" s="11"/>
       <c r="Q13" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R13" s="10"/>
       <c r="S13" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:19" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -1519,42 +1562,42 @@
         <v>16</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I14" s="16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J14" s="10"/>
       <c r="K14" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L14" s="10"/>
       <c r="M14" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N14" s="10"/>
       <c r="O14" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P14" s="11"/>
       <c r="Q14" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R14" s="10"/>
       <c r="S14" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:19" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1568,42 +1611,42 @@
         <v>16</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I15" s="16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J15" s="10"/>
       <c r="K15" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L15" s="10"/>
       <c r="M15" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N15" s="10"/>
       <c r="O15" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P15" s="11"/>
       <c r="Q15" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R15" s="10"/>
       <c r="S15" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1617,42 +1660,42 @@
         <v>16</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I16" s="16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J16" s="10"/>
       <c r="K16" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L16" s="10"/>
       <c r="M16" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N16" s="10"/>
       <c r="O16" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P16" s="11"/>
       <c r="Q16" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R16" s="10"/>
       <c r="S16" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:19" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1666,42 +1709,42 @@
         <v>16</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I17" s="16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J17" s="10"/>
       <c r="K17" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L17" s="10"/>
       <c r="M17" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N17" s="10"/>
       <c r="O17" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P17" s="11"/>
       <c r="Q17" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R17" s="10"/>
       <c r="S17" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1715,42 +1758,42 @@
         <v>16</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I18" s="16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J18" s="10"/>
       <c r="K18" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L18" s="10"/>
       <c r="M18" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N18" s="10"/>
       <c r="O18" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P18" s="11"/>
       <c r="Q18" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R18" s="10"/>
       <c r="S18" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:19" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1764,42 +1807,42 @@
         <v>16</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I19" s="16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J19" s="10"/>
       <c r="K19" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L19" s="10"/>
       <c r="M19" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N19" s="10"/>
       <c r="O19" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P19" s="11"/>
       <c r="Q19" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R19" s="10"/>
       <c r="S19" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:19" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1813,42 +1856,42 @@
         <v>16</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I20" s="16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J20" s="10"/>
       <c r="K20" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L20" s="10"/>
       <c r="M20" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N20" s="10"/>
       <c r="O20" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P20" s="11"/>
       <c r="Q20" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R20" s="10"/>
       <c r="S20" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:19" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1862,42 +1905,42 @@
         <v>16</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I21" s="16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J21" s="10"/>
       <c r="K21" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L21" s="10"/>
       <c r="M21" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N21" s="10"/>
       <c r="O21" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P21" s="11"/>
       <c r="Q21" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R21" s="10"/>
       <c r="S21" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1911,42 +1954,42 @@
         <v>16</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I22" s="16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J22" s="10"/>
       <c r="K22" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L22" s="10"/>
       <c r="M22" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N22" s="10"/>
       <c r="O22" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P22" s="11"/>
       <c r="Q22" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R22" s="10"/>
       <c r="S22" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1960,42 +2003,42 @@
         <v>16</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I23" s="16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J23" s="10"/>
       <c r="K23" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L23" s="10"/>
       <c r="M23" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N23" s="10"/>
       <c r="O23" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P23" s="11"/>
       <c r="Q23" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R23" s="10"/>
       <c r="S23" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:19" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -2009,42 +2052,42 @@
         <v>16</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F24" s="19" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I24" s="16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J24" s="10"/>
       <c r="K24" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L24" s="10"/>
       <c r="M24" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N24" s="10"/>
       <c r="O24" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P24" s="11"/>
       <c r="Q24" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R24" s="10"/>
       <c r="S24" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2056,24 +2099,2760 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="24">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="24">
+        <v>2</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="24">
+        <v>3</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="24">
+        <v>4</v>
+      </c>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="24">
+        <v>5</v>
+      </c>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="24">
+        <v>6</v>
+      </c>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="24">
+        <v>7</v>
+      </c>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="24">
+        <v>8</v>
+      </c>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="24">
+        <v>9</v>
+      </c>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="24">
+        <v>10</v>
+      </c>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="24">
+        <v>11</v>
+      </c>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="24">
+        <v>12</v>
+      </c>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="24">
+        <v>13</v>
+      </c>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="24">
+        <v>14</v>
+      </c>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="24">
+        <v>15</v>
+      </c>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="24">
+        <v>16</v>
+      </c>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="24">
+        <v>17</v>
+      </c>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="24">
+        <v>18</v>
+      </c>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="24">
+        <v>19</v>
+      </c>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="24">
+        <v>20</v>
+      </c>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="24">
+        <v>21</v>
+      </c>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="24">
+        <v>22</v>
+      </c>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="24">
+        <v>24</v>
+      </c>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="24">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="24">
+        <v>2</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="24">
+        <v>3</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="24">
+        <v>4</v>
+      </c>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="24">
+        <v>5</v>
+      </c>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="24">
+        <v>6</v>
+      </c>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="24">
+        <v>7</v>
+      </c>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="24">
+        <v>8</v>
+      </c>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="24">
+        <v>9</v>
+      </c>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="24">
+        <v>10</v>
+      </c>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="24">
+        <v>11</v>
+      </c>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="24">
+        <v>12</v>
+      </c>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="24">
+        <v>13</v>
+      </c>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="24">
+        <v>14</v>
+      </c>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="24">
+        <v>15</v>
+      </c>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="24">
+        <v>16</v>
+      </c>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="24">
+        <v>17</v>
+      </c>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="24">
+        <v>18</v>
+      </c>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="24">
+        <v>19</v>
+      </c>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="24">
+        <v>20</v>
+      </c>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="24">
+        <v>21</v>
+      </c>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="24">
+        <v>22</v>
+      </c>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="24">
+        <v>24</v>
+      </c>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="5" max="6" width="16.28515625" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" customWidth="1"/>
+    <col min="11" max="11" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="24">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="24">
+        <v>2</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="24">
+        <v>3</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="24">
+        <v>4</v>
+      </c>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="24">
+        <v>5</v>
+      </c>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="24">
+        <v>6</v>
+      </c>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="24">
+        <v>7</v>
+      </c>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="24">
+        <v>8</v>
+      </c>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="24">
+        <v>9</v>
+      </c>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="24">
+        <v>10</v>
+      </c>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="24">
+        <v>11</v>
+      </c>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="24">
+        <v>12</v>
+      </c>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="24">
+        <v>13</v>
+      </c>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="24">
+        <v>14</v>
+      </c>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="24">
+        <v>15</v>
+      </c>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="24">
+        <v>16</v>
+      </c>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="24">
+        <v>17</v>
+      </c>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="24">
+        <v>18</v>
+      </c>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="24">
+        <v>19</v>
+      </c>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="24">
+        <v>20</v>
+      </c>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="24">
+        <v>21</v>
+      </c>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="24">
+        <v>22</v>
+      </c>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="24">
+        <v>24</v>
+      </c>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" customWidth="1"/>
+    <col min="10" max="10" width="19.5703125" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="24">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="24">
+        <v>2</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="24">
+        <v>3</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="24">
+        <v>4</v>
+      </c>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="24">
+        <v>5</v>
+      </c>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="24">
+        <v>6</v>
+      </c>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="24">
+        <v>7</v>
+      </c>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="24">
+        <v>8</v>
+      </c>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="24">
+        <v>9</v>
+      </c>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="24">
+        <v>10</v>
+      </c>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="24">
+        <v>11</v>
+      </c>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="24">
+        <v>12</v>
+      </c>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="24">
+        <v>13</v>
+      </c>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="24">
+        <v>14</v>
+      </c>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="24">
+        <v>15</v>
+      </c>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="24">
+        <v>16</v>
+      </c>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="24">
+        <v>17</v>
+      </c>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="24">
+        <v>18</v>
+      </c>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="24">
+        <v>19</v>
+      </c>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="24">
+        <v>20</v>
+      </c>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="24">
+        <v>21</v>
+      </c>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="24">
+        <v>22</v>
+      </c>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="24">
+        <v>24</v>
+      </c>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" customWidth="1"/>
+    <col min="11" max="11" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="24">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="24">
+        <v>2</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="24">
+        <v>3</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="24">
+        <v>4</v>
+      </c>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="24">
+        <v>5</v>
+      </c>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="24">
+        <v>6</v>
+      </c>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="24">
+        <v>7</v>
+      </c>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="24">
+        <v>8</v>
+      </c>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="24">
+        <v>9</v>
+      </c>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="24">
+        <v>10</v>
+      </c>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="24">
+        <v>11</v>
+      </c>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="24">
+        <v>12</v>
+      </c>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="24">
+        <v>13</v>
+      </c>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="24">
+        <v>14</v>
+      </c>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="24">
+        <v>15</v>
+      </c>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="24">
+        <v>16</v>
+      </c>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="24">
+        <v>17</v>
+      </c>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="24">
+        <v>18</v>
+      </c>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="24">
+        <v>19</v>
+      </c>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="24">
+        <v>20</v>
+      </c>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="24">
+        <v>21</v>
+      </c>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="24">
+        <v>22</v>
+      </c>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="24">
+        <v>24</v>
+      </c>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="24">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="24">
+        <v>2</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="24">
+        <v>3</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="24">
+        <v>4</v>
+      </c>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="24">
+        <v>5</v>
+      </c>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="24">
+        <v>6</v>
+      </c>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="24">
+        <v>7</v>
+      </c>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="24">
+        <v>8</v>
+      </c>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="24">
+        <v>9</v>
+      </c>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="24">
+        <v>10</v>
+      </c>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="24">
+        <v>11</v>
+      </c>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="24">
+        <v>12</v>
+      </c>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="24">
+        <v>13</v>
+      </c>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="24">
+        <v>14</v>
+      </c>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="24">
+        <v>15</v>
+      </c>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="24">
+        <v>16</v>
+      </c>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="24">
+        <v>17</v>
+      </c>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="24">
+        <v>18</v>
+      </c>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="24">
+        <v>19</v>
+      </c>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="24">
+        <v>20</v>
+      </c>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="24">
+        <v>21</v>
+      </c>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="24">
+        <v>22</v>
+      </c>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="24">
+        <v>24</v>
+      </c>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2333,9 +5112,15 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFD779FF-B039-4DC7-8903-586F168B5B9F}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9c97f8e9-86c7-4e99-9925-cc9540b321fe"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9c97f8e9-86c7-4e99-9925-cc9540b321fe"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Gestion du point technique avec et sans INSEE
</commit_message>
<xml_diff>
--- a/Documentation/Controleur.xlsx
+++ b/Documentation/Controleur.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="255" windowWidth="6915" windowHeight="6600" activeTab="6"/>
+    <workbookView xWindow="480" yWindow="255" windowWidth="6915" windowHeight="6600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Controleur CA" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="108">
   <si>
     <t>Famille</t>
   </si>
@@ -2304,8 +2304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5656,8 +5656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5764,7 +5764,9 @@
       <c r="J3" s="23"/>
       <c r="K3" s="23"/>
       <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
+      <c r="M3" s="23" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="25">
@@ -5787,7 +5789,9 @@
       <c r="J4" s="23"/>
       <c r="K4" s="23"/>
       <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
+      <c r="M4" s="23" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="25">
@@ -5835,7 +5839,9 @@
       <c r="J6" s="23"/>
       <c r="K6" s="23"/>
       <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
+      <c r="M6" s="23" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="25">
@@ -6318,15 +6324,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document Microsoft Word" ma:contentTypeID="0x01010066910ADB61686C45A75A7A744D7D5C8E0022B63E0AEFBB2040BF2A3B1B4BE32EE5" ma:contentTypeVersion="4" ma:contentTypeDescription="Document Microsoft Word vierge." ma:contentTypeScope="" ma:versionID="0a4943d90c7214e3c95a70ccb3c8346b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c97f8e9-86c7-4e99-9925-cc9540b321fe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eeaa8661ba6ba22f90735bcd04aade41" ns2:_="">
     <xsd:import namespace="9c97f8e9-86c7-4e99-9925-cc9540b321fe"/>
@@ -6529,6 +6526,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -6544,14 +6550,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F02C15CB-09E5-4D58-8C63-77232C75BB18}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8B2112A-C178-4B00-8690-1CA741C188F5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6565,6 +6563,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F02C15CB-09E5-4D58-8C63-77232C75BB18}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
- Contrôle 5 complété et étendu - Contrôle 26 ajouté
</commit_message>
<xml_diff>
--- a/Documentation/Controleur.xlsx
+++ b/Documentation/Controleur.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="255" windowWidth="6915" windowHeight="6600" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="255" windowWidth="6915" windowHeight="6600"/>
   </bookViews>
   <sheets>
     <sheet name="Controleur CA" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="CD70" sheetId="5" r:id="rId5"/>
     <sheet name="CD71" sheetId="6" r:id="rId6"/>
     <sheet name="testv1" sheetId="7" r:id="rId7"/>
+    <sheet name="testv2" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Controleur CA'!$A$1:$I$24</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="107">
   <si>
     <t>Famille</t>
   </si>
@@ -178,21 +179,6 @@
     <t>Liaison manquant dans la C3A</t>
   </si>
   <si>
-    <t>CD21</t>
-  </si>
-  <si>
-    <t>CD39</t>
-  </si>
-  <si>
-    <t>CD58</t>
-  </si>
-  <si>
-    <t>CD70</t>
-  </si>
-  <si>
-    <t>CD71</t>
-  </si>
-  <si>
     <t>Données d'entrée cd21</t>
   </si>
   <si>
@@ -347,6 +333,18 @@
   </si>
   <si>
     <t>Nom de fiche poteau incorrect</t>
+  </si>
+  <si>
+    <t>Structuration des couches</t>
+  </si>
+  <si>
+    <t>Couche point contrôle</t>
+  </si>
+  <si>
+    <t>Vérifier que la liste des champs de la couche point contrôle correspond aux spécifications QGIS</t>
+  </si>
+  <si>
+    <t>La structuration des champs de la couche point contrôle est incorrecte</t>
   </si>
 </sst>
 </file>
@@ -370,7 +368,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -386,6 +384,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -690,7 +694,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -781,6 +785,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1088,29 +1093,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S25"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" customWidth="1"/>
     <col min="6" max="7" width="33.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="41.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.140625" customWidth="1"/>
-    <col min="10" max="10" width="35.140625" customWidth="1"/>
-    <col min="12" max="12" width="35.140625" customWidth="1"/>
+    <col min="10" max="12" width="35.140625" customWidth="1"/>
+    <col min="13" max="13" width="23" customWidth="1"/>
     <col min="14" max="14" width="35.140625" customWidth="1"/>
-    <col min="16" max="16" width="23" customWidth="1"/>
-    <col min="18" max="18" width="35.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>42</v>
       </c>
@@ -1139,37 +1143,22 @@
         <v>6</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="S1" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="20">
         <v>1</v>
       </c>
@@ -1183,7 +1172,7 @@
         <v>47</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>40</v>
@@ -1198,27 +1187,12 @@
         <v>10</v>
       </c>
       <c r="J2" s="10"/>
-      <c r="K2" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="K2" s="10"/>
       <c r="L2" s="10"/>
-      <c r="M2" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="M2" s="11"/>
       <c r="N2" s="10"/>
-      <c r="O2" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="R2" s="10"/>
-      <c r="S2" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:14" s="42" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="20">
         <v>2</v>
       </c>
@@ -1247,17 +1221,12 @@
         <v>10</v>
       </c>
       <c r="J3" s="10"/>
-      <c r="K3" s="11"/>
+      <c r="K3" s="10"/>
       <c r="L3" s="10"/>
       <c r="M3" s="11"/>
       <c r="N3" s="10"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="11"/>
-    </row>
-    <row r="4" spans="1:19" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:14" s="42" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="20">
         <v>3</v>
       </c>
@@ -1286,17 +1255,12 @@
         <v>37</v>
       </c>
       <c r="J4" s="10"/>
-      <c r="K4" s="11"/>
+      <c r="K4" s="10"/>
       <c r="L4" s="10"/>
       <c r="M4" s="11"/>
       <c r="N4" s="10"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="11"/>
-    </row>
-    <row r="5" spans="1:19" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:14" s="42" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="20">
         <v>4</v>
       </c>
@@ -1316,36 +1280,21 @@
         <v>15</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="I5" s="16" t="s">
         <v>10</v>
       </c>
       <c r="J5" s="10"/>
-      <c r="K5" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="K5" s="10"/>
       <c r="L5" s="10"/>
-      <c r="M5" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="M5" s="11"/>
       <c r="N5" s="10"/>
-      <c r="O5" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="R5" s="10"/>
-      <c r="S5" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:14" s="42" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="20">
         <v>5</v>
       </c>
@@ -1365,26 +1314,21 @@
         <v>17</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="I6" s="16" t="s">
         <v>37</v>
       </c>
       <c r="J6" s="10"/>
-      <c r="K6" s="11"/>
+      <c r="K6" s="10"/>
       <c r="L6" s="10"/>
       <c r="M6" s="11"/>
       <c r="N6" s="10"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="11"/>
-    </row>
-    <row r="7" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:14" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
         <v>6</v>
       </c>
@@ -1398,42 +1342,27 @@
         <v>47</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F7" s="15" t="s">
         <v>18</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I7" s="16" t="s">
         <v>38</v>
       </c>
       <c r="J7" s="10"/>
-      <c r="K7" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="K7" s="10"/>
       <c r="L7" s="10"/>
-      <c r="M7" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="M7" s="11"/>
       <c r="N7" s="10"/>
-      <c r="O7" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="R7" s="10"/>
-      <c r="S7" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:14" s="42" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
         <v>7</v>
       </c>
@@ -1447,42 +1376,27 @@
         <v>47</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F8" s="15" t="s">
         <v>19</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="I8" s="16" t="s">
         <v>37</v>
       </c>
       <c r="J8" s="10"/>
-      <c r="K8" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="K8" s="10"/>
       <c r="L8" s="10"/>
-      <c r="M8" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="M8" s="11"/>
       <c r="N8" s="10"/>
-      <c r="O8" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="R8" s="10"/>
-      <c r="S8" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:14" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="20">
         <v>8</v>
       </c>
@@ -1496,42 +1410,27 @@
         <v>47</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F9" s="15" t="s">
         <v>20</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I9" s="16" t="s">
         <v>37</v>
       </c>
       <c r="J9" s="10"/>
-      <c r="K9" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="K9" s="10"/>
       <c r="L9" s="10"/>
-      <c r="M9" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="M9" s="11"/>
       <c r="N9" s="10"/>
-      <c r="O9" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="R9" s="10"/>
-      <c r="S9" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:14" s="42" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="20">
         <v>9</v>
       </c>
@@ -1545,42 +1444,27 @@
         <v>47</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F10" s="15" t="s">
         <v>21</v>
       </c>
       <c r="G10" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" s="15" t="s">
         <v>64</v>
-      </c>
-      <c r="H10" s="15" t="s">
-        <v>69</v>
       </c>
       <c r="I10" s="16" t="s">
         <v>38</v>
       </c>
       <c r="J10" s="10"/>
-      <c r="K10" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="K10" s="10"/>
       <c r="L10" s="10"/>
-      <c r="M10" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="M10" s="11"/>
       <c r="N10" s="10"/>
-      <c r="O10" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="R10" s="10"/>
-      <c r="S10" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:14" s="42" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="20">
         <v>10</v>
       </c>
@@ -1594,42 +1478,27 @@
         <v>47</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F11" s="15" t="s">
         <v>22</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="I11" s="16" t="s">
         <v>37</v>
       </c>
       <c r="J11" s="10"/>
-      <c r="K11" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="K11" s="10"/>
       <c r="L11" s="10"/>
-      <c r="M11" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="M11" s="11"/>
       <c r="N11" s="10"/>
-      <c r="O11" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="R11" s="10"/>
-      <c r="S11" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:14" s="42" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="20">
         <v>11</v>
       </c>
@@ -1649,36 +1518,21 @@
         <v>23</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I12" s="16" t="s">
         <v>37</v>
       </c>
       <c r="J12" s="10"/>
-      <c r="K12" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="K12" s="10"/>
       <c r="L12" s="10"/>
-      <c r="M12" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="M12" s="11"/>
       <c r="N12" s="10"/>
-      <c r="O12" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="R12" s="10"/>
-      <c r="S12" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:14" s="42" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="20">
         <v>12</v>
       </c>
@@ -1692,13 +1546,13 @@
         <v>47</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F13" s="15" t="s">
         <v>25</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H13" s="15" t="s">
         <v>24</v>
@@ -1707,27 +1561,12 @@
         <v>37</v>
       </c>
       <c r="J13" s="10"/>
-      <c r="K13" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="K13" s="10"/>
       <c r="L13" s="10"/>
-      <c r="M13" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="M13" s="11"/>
       <c r="N13" s="10"/>
-      <c r="O13" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="R13" s="10"/>
-      <c r="S13" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" s="12" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:14" s="42" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="20">
         <v>13</v>
       </c>
@@ -1741,42 +1580,27 @@
         <v>47</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F14" s="15" t="s">
         <v>26</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="I14" s="16" t="s">
         <v>38</v>
       </c>
       <c r="J14" s="10"/>
-      <c r="K14" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="K14" s="10"/>
       <c r="L14" s="10"/>
-      <c r="M14" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="M14" s="11"/>
       <c r="N14" s="10"/>
-      <c r="O14" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="P14" s="11"/>
-      <c r="Q14" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="R14" s="10"/>
-      <c r="S14" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:14" s="42" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="20">
         <v>15</v>
       </c>
@@ -1790,42 +1614,27 @@
         <v>47</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F15" s="15" t="s">
         <v>28</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="I15" s="16" t="s">
         <v>38</v>
       </c>
       <c r="J15" s="10"/>
-      <c r="K15" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="K15" s="10"/>
       <c r="L15" s="10"/>
-      <c r="M15" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="M15" s="11"/>
       <c r="N15" s="10"/>
-      <c r="O15" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="R15" s="10"/>
-      <c r="S15" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:14" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
         <v>16</v>
       </c>
@@ -1839,42 +1648,27 @@
         <v>47</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F16" s="15" t="s">
         <v>27</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I16" s="16" t="s">
         <v>38</v>
       </c>
       <c r="J16" s="10"/>
-      <c r="K16" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="K16" s="10"/>
       <c r="L16" s="10"/>
-      <c r="M16" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="M16" s="11"/>
       <c r="N16" s="10"/>
-      <c r="O16" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="R16" s="10"/>
-      <c r="S16" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:14" s="42" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="20">
         <v>17</v>
       </c>
@@ -1888,42 +1682,27 @@
         <v>47</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F17" s="15" t="s">
         <v>31</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="I17" s="16" t="s">
         <v>38</v>
       </c>
       <c r="J17" s="10"/>
-      <c r="K17" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="K17" s="10"/>
       <c r="L17" s="10"/>
-      <c r="M17" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="M17" s="11"/>
       <c r="N17" s="10"/>
-      <c r="O17" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="R17" s="10"/>
-      <c r="S17" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:14" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="20">
         <v>18</v>
       </c>
@@ -1937,42 +1716,27 @@
         <v>47</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F18" s="15" t="s">
         <v>29</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I18" s="16" t="s">
         <v>38</v>
       </c>
       <c r="J18" s="10"/>
-      <c r="K18" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="K18" s="10"/>
       <c r="L18" s="10"/>
-      <c r="M18" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="M18" s="11"/>
       <c r="N18" s="10"/>
-      <c r="O18" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="R18" s="10"/>
-      <c r="S18" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:14" s="42" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="20">
         <v>19</v>
       </c>
@@ -1986,42 +1750,27 @@
         <v>47</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F19" s="15" t="s">
         <v>30</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="I19" s="16" t="s">
         <v>38</v>
       </c>
       <c r="J19" s="10"/>
-      <c r="K19" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="K19" s="10"/>
       <c r="L19" s="10"/>
-      <c r="M19" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="M19" s="11"/>
       <c r="N19" s="10"/>
-      <c r="O19" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="R19" s="10"/>
-      <c r="S19" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:14" s="42" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="20">
         <v>20</v>
       </c>
@@ -2035,42 +1784,27 @@
         <v>47</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F20" s="15" t="s">
         <v>32</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="I20" s="16" t="s">
         <v>38</v>
       </c>
       <c r="J20" s="10"/>
-      <c r="K20" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="K20" s="10"/>
       <c r="L20" s="10"/>
-      <c r="M20" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="M20" s="11"/>
       <c r="N20" s="10"/>
-      <c r="O20" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="P20" s="11"/>
-      <c r="Q20" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="R20" s="10"/>
-      <c r="S20" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:14" s="42" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="20">
         <v>21</v>
       </c>
@@ -2084,42 +1818,27 @@
         <v>47</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F21" s="15" t="s">
         <v>33</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="I21" s="16" t="s">
         <v>38</v>
       </c>
       <c r="J21" s="10"/>
-      <c r="K21" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="K21" s="10"/>
       <c r="L21" s="10"/>
-      <c r="M21" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="M21" s="11"/>
       <c r="N21" s="10"/>
-      <c r="O21" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="P21" s="11"/>
-      <c r="Q21" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="R21" s="10"/>
-      <c r="S21" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:14" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="20">
         <v>22</v>
       </c>
@@ -2133,42 +1852,27 @@
         <v>47</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F22" s="15" t="s">
         <v>34</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="I22" s="16" t="s">
         <v>38</v>
       </c>
       <c r="J22" s="10"/>
-      <c r="K22" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="K22" s="10"/>
       <c r="L22" s="10"/>
-      <c r="M22" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="M22" s="11"/>
       <c r="N22" s="10"/>
-      <c r="O22" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="P22" s="11"/>
-      <c r="Q22" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="R22" s="10"/>
-      <c r="S22" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:14" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="20">
         <v>23</v>
       </c>
@@ -2182,42 +1886,27 @@
         <v>47</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F23" s="15" t="s">
         <v>35</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="I23" s="16" t="s">
         <v>38</v>
       </c>
       <c r="J23" s="10"/>
-      <c r="K23" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="K23" s="10"/>
       <c r="L23" s="10"/>
-      <c r="M23" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="M23" s="11"/>
       <c r="N23" s="10"/>
-      <c r="O23" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="P23" s="11"/>
-      <c r="Q23" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="R23" s="10"/>
-      <c r="S23" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:14" s="42" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="20">
         <v>24</v>
       </c>
@@ -2231,67 +1920,91 @@
         <v>47</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F24" s="19" t="s">
         <v>36</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="I24" s="16" t="s">
         <v>38</v>
       </c>
       <c r="J24" s="10"/>
-      <c r="K24" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="K24" s="10"/>
       <c r="L24" s="10"/>
-      <c r="M24" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="M24" s="11"/>
       <c r="N24" s="10"/>
-      <c r="O24" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="P24" s="11"/>
-      <c r="Q24" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="R24" s="10"/>
-      <c r="S24" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:14" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="35">
         <v>25</v>
       </c>
       <c r="B25" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="14" t="s">
-        <v>8</v>
+      <c r="C25" s="18" t="s">
+        <v>16</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>12</v>
       </c>
       <c r="E25" s="14"/>
       <c r="F25" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="H25" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="I25" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+    </row>
+    <row r="26" spans="1:14" s="42" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="35">
+        <v>26</v>
+      </c>
+      <c r="B26" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H26" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="G25" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="H25" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="I25" s="16" t="s">
-        <v>105</v>
-      </c>
+      <c r="I26" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I24"/>
@@ -2304,8 +2017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2326,7 +2039,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B1" s="41" t="s">
         <v>0</v>
@@ -2335,34 +2048,34 @@
         <v>3</v>
       </c>
       <c r="D1" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="H1" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="K1" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="L1" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="M1" s="34" t="s">
         <v>87</v>
-      </c>
-      <c r="H1" s="30" t="s">
-        <v>86</v>
-      </c>
-      <c r="I1" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="J1" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="K1" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="L1" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="M1" s="34" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -2387,7 +2100,7 @@
       <c r="K2" s="32"/>
       <c r="L2" s="32"/>
       <c r="M2" s="32" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -2458,7 +2171,7 @@
       <c r="K5" s="23"/>
       <c r="L5" s="23"/>
       <c r="M5" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -2483,7 +2196,7 @@
       <c r="K6" s="23"/>
       <c r="L6" s="23"/>
       <c r="M6" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -2508,7 +2221,7 @@
       <c r="K7" s="23"/>
       <c r="L7" s="23"/>
       <c r="M7" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -2533,7 +2246,7 @@
       <c r="K8" s="23"/>
       <c r="L8" s="23"/>
       <c r="M8" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -2558,7 +2271,7 @@
       <c r="K9" s="23"/>
       <c r="L9" s="23"/>
       <c r="M9" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -2583,7 +2296,7 @@
       <c r="K10" s="23"/>
       <c r="L10" s="23"/>
       <c r="M10" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -2608,7 +2321,7 @@
       <c r="K11" s="23"/>
       <c r="L11" s="23"/>
       <c r="M11" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -2633,7 +2346,7 @@
       <c r="K12" s="23"/>
       <c r="L12" s="23"/>
       <c r="M12" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -2658,7 +2371,7 @@
       <c r="K13" s="23"/>
       <c r="L13" s="23"/>
       <c r="M13" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -2683,12 +2396,12 @@
       <c r="K14" s="23"/>
       <c r="L14" s="23"/>
       <c r="M14" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B15" s="40" t="str">
         <f>'Controleur CA'!B15</f>
@@ -2708,12 +2421,12 @@
       <c r="K15" s="23"/>
       <c r="L15" s="23"/>
       <c r="M15" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B16" s="40" t="str">
         <f>'Controleur CA'!B16</f>
@@ -2733,12 +2446,12 @@
       <c r="K16" s="23"/>
       <c r="L16" s="23"/>
       <c r="M16" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B17" s="40" t="str">
         <f>'Controleur CA'!B17</f>
@@ -2758,12 +2471,12 @@
       <c r="K17" s="23"/>
       <c r="L17" s="23"/>
       <c r="M17" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B18" s="40" t="str">
         <f>'Controleur CA'!B18</f>
@@ -2783,12 +2496,12 @@
       <c r="K18" s="23"/>
       <c r="L18" s="23"/>
       <c r="M18" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B19" s="40" t="str">
         <f>'Controleur CA'!B19</f>
@@ -2808,12 +2521,12 @@
       <c r="K19" s="23"/>
       <c r="L19" s="23"/>
       <c r="M19" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B20" s="40" t="str">
         <f>'Controleur CA'!B20</f>
@@ -2833,12 +2546,12 @@
       <c r="K20" s="23"/>
       <c r="L20" s="23"/>
       <c r="M20" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B21" s="40" t="str">
         <f>'Controleur CA'!B21</f>
@@ -2858,12 +2571,12 @@
       <c r="K21" s="23"/>
       <c r="L21" s="23"/>
       <c r="M21" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B22" s="40" t="str">
         <f>'Controleur CA'!B22</f>
@@ -2883,12 +2596,12 @@
       <c r="K22" s="23"/>
       <c r="L22" s="23"/>
       <c r="M22" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B23" s="40" t="str">
         <f>'Controleur CA'!B23</f>
@@ -2908,12 +2621,12 @@
       <c r="K23" s="23"/>
       <c r="L23" s="23"/>
       <c r="M23" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="37" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B24" s="40" t="str">
         <f>'Controleur CA'!B24</f>
@@ -2933,7 +2646,7 @@
       <c r="K24" s="39"/>
       <c r="L24" s="39"/>
       <c r="M24" s="39" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -2958,12 +2671,33 @@
       <c r="K25" s="40"/>
       <c r="L25" s="40"/>
       <c r="M25" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26"/>
-      <c r="C26"/>
+      <c r="A26" s="23">
+        <v>26</v>
+      </c>
+      <c r="B26" s="40" t="str">
+        <f>'Controleur CA'!B26</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C26" s="26" t="str">
+        <f>'Controleur CA'!F26</f>
+        <v>Vérifier que la liste des champs de la couche point contrôle correspond aux spécifications QGIS</v>
+      </c>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="40"/>
+      <c r="L26" s="40"/>
+      <c r="M26" s="23" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27"/>
@@ -2977,10 +2711,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B25" sqref="B2:B25"/>
+      <selection activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3002,7 +2736,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B1" s="41" t="s">
         <v>0</v>
@@ -3011,34 +2745,34 @@
         <v>3</v>
       </c>
       <c r="D1" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="H1" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="K1" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="L1" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="M1" s="34" t="s">
         <v>87</v>
-      </c>
-      <c r="H1" s="30" t="s">
-        <v>86</v>
-      </c>
-      <c r="I1" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="J1" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="K1" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="L1" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="M1" s="34" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -3063,7 +2797,7 @@
       <c r="K2" s="32"/>
       <c r="L2" s="32"/>
       <c r="M2" s="32" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -3088,7 +2822,7 @@
       <c r="K3" s="23"/>
       <c r="L3" s="23"/>
       <c r="M3" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -3113,7 +2847,7 @@
       <c r="K4" s="23"/>
       <c r="L4" s="23"/>
       <c r="M4" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -3138,7 +2872,7 @@
       <c r="K5" s="23"/>
       <c r="L5" s="23"/>
       <c r="M5" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -3163,7 +2897,7 @@
       <c r="K6" s="23"/>
       <c r="L6" s="23"/>
       <c r="M6" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -3188,7 +2922,7 @@
       <c r="K7" s="23"/>
       <c r="L7" s="23"/>
       <c r="M7" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -3213,7 +2947,7 @@
       <c r="K8" s="23"/>
       <c r="L8" s="23"/>
       <c r="M8" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -3238,7 +2972,7 @@
       <c r="K9" s="23"/>
       <c r="L9" s="23"/>
       <c r="M9" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -3263,7 +2997,7 @@
       <c r="K10" s="23"/>
       <c r="L10" s="23"/>
       <c r="M10" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -3288,7 +3022,7 @@
       <c r="K11" s="23"/>
       <c r="L11" s="23"/>
       <c r="M11" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -3313,7 +3047,7 @@
       <c r="K12" s="23"/>
       <c r="L12" s="23"/>
       <c r="M12" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -3338,7 +3072,7 @@
       <c r="K13" s="23"/>
       <c r="L13" s="23"/>
       <c r="M13" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -3363,12 +3097,12 @@
       <c r="K14" s="23"/>
       <c r="L14" s="23"/>
       <c r="M14" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B15" s="40" t="str">
         <f>'Controleur CA'!B15</f>
@@ -3388,12 +3122,12 @@
       <c r="K15" s="23"/>
       <c r="L15" s="23"/>
       <c r="M15" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B16" s="40" t="str">
         <f>'Controleur CA'!B16</f>
@@ -3413,12 +3147,12 @@
       <c r="K16" s="23"/>
       <c r="L16" s="23"/>
       <c r="M16" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B17" s="40" t="str">
         <f>'Controleur CA'!B17</f>
@@ -3438,12 +3172,12 @@
       <c r="K17" s="23"/>
       <c r="L17" s="23"/>
       <c r="M17" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B18" s="40" t="str">
         <f>'Controleur CA'!B18</f>
@@ -3463,12 +3197,12 @@
       <c r="K18" s="23"/>
       <c r="L18" s="23"/>
       <c r="M18" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B19" s="40" t="str">
         <f>'Controleur CA'!B19</f>
@@ -3488,12 +3222,12 @@
       <c r="K19" s="23"/>
       <c r="L19" s="23"/>
       <c r="M19" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B20" s="40" t="str">
         <f>'Controleur CA'!B20</f>
@@ -3513,12 +3247,12 @@
       <c r="K20" s="23"/>
       <c r="L20" s="23"/>
       <c r="M20" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B21" s="40" t="str">
         <f>'Controleur CA'!B21</f>
@@ -3538,12 +3272,12 @@
       <c r="K21" s="23"/>
       <c r="L21" s="23"/>
       <c r="M21" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B22" s="40" t="str">
         <f>'Controleur CA'!B22</f>
@@ -3563,12 +3297,12 @@
       <c r="K22" s="23"/>
       <c r="L22" s="23"/>
       <c r="M22" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B23" s="40" t="str">
         <f>'Controleur CA'!B23</f>
@@ -3588,12 +3322,12 @@
       <c r="K23" s="23"/>
       <c r="L23" s="23"/>
       <c r="M23" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B24" s="40" t="str">
         <f>'Controleur CA'!B24</f>
@@ -3613,7 +3347,7 @@
       <c r="K24" s="23"/>
       <c r="L24" s="23"/>
       <c r="M24" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -3638,7 +3372,32 @@
       <c r="K25" s="40"/>
       <c r="L25" s="40"/>
       <c r="M25" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="23">
+        <v>26</v>
+      </c>
+      <c r="B26" s="40" t="str">
+        <f>'Controleur CA'!B26</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C26" s="26" t="str">
+        <f>'Controleur CA'!F26</f>
+        <v>Vérifier que la liste des champs de la couche point contrôle correspond aux spécifications QGIS</v>
+      </c>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="40"/>
+      <c r="L26" s="40"/>
+      <c r="M26" s="23" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -3648,10 +3407,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD25"/>
+      <selection activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3673,7 +3432,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B1" s="41" t="s">
         <v>0</v>
@@ -3682,34 +3441,34 @@
         <v>3</v>
       </c>
       <c r="D1" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="H1" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="K1" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="L1" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="M1" s="34" t="s">
         <v>87</v>
-      </c>
-      <c r="H1" s="30" t="s">
-        <v>86</v>
-      </c>
-      <c r="I1" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="J1" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="K1" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="L1" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="M1" s="34" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -3734,7 +3493,7 @@
       <c r="K2" s="32"/>
       <c r="L2" s="32"/>
       <c r="M2" s="32" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -3759,7 +3518,7 @@
       <c r="K3" s="23"/>
       <c r="L3" s="23"/>
       <c r="M3" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -3784,7 +3543,7 @@
       <c r="K4" s="23"/>
       <c r="L4" s="23"/>
       <c r="M4" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -3809,7 +3568,7 @@
       <c r="K5" s="23"/>
       <c r="L5" s="23"/>
       <c r="M5" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -3834,7 +3593,7 @@
       <c r="K6" s="23"/>
       <c r="L6" s="23"/>
       <c r="M6" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -3859,7 +3618,7 @@
       <c r="K7" s="23"/>
       <c r="L7" s="23"/>
       <c r="M7" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -3884,7 +3643,7 @@
       <c r="K8" s="23"/>
       <c r="L8" s="23"/>
       <c r="M8" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -3909,7 +3668,7 @@
       <c r="K9" s="23"/>
       <c r="L9" s="23"/>
       <c r="M9" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -3934,7 +3693,7 @@
       <c r="K10" s="23"/>
       <c r="L10" s="23"/>
       <c r="M10" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -3959,7 +3718,7 @@
       <c r="K11" s="23"/>
       <c r="L11" s="23"/>
       <c r="M11" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -3984,7 +3743,7 @@
       <c r="K12" s="23"/>
       <c r="L12" s="23"/>
       <c r="M12" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -4009,7 +3768,7 @@
       <c r="K13" s="23"/>
       <c r="L13" s="23"/>
       <c r="M13" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -4034,12 +3793,12 @@
       <c r="K14" s="23"/>
       <c r="L14" s="23"/>
       <c r="M14" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B15" s="40" t="str">
         <f>'Controleur CA'!B15</f>
@@ -4059,12 +3818,12 @@
       <c r="K15" s="23"/>
       <c r="L15" s="23"/>
       <c r="M15" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B16" s="40" t="str">
         <f>'Controleur CA'!B16</f>
@@ -4084,12 +3843,12 @@
       <c r="K16" s="23"/>
       <c r="L16" s="23"/>
       <c r="M16" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B17" s="40" t="str">
         <f>'Controleur CA'!B17</f>
@@ -4109,12 +3868,12 @@
       <c r="K17" s="23"/>
       <c r="L17" s="23"/>
       <c r="M17" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B18" s="40" t="str">
         <f>'Controleur CA'!B18</f>
@@ -4134,12 +3893,12 @@
       <c r="K18" s="23"/>
       <c r="L18" s="23"/>
       <c r="M18" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B19" s="40" t="str">
         <f>'Controleur CA'!B19</f>
@@ -4159,12 +3918,12 @@
       <c r="K19" s="23"/>
       <c r="L19" s="23"/>
       <c r="M19" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B20" s="40" t="str">
         <f>'Controleur CA'!B20</f>
@@ -4184,12 +3943,12 @@
       <c r="K20" s="23"/>
       <c r="L20" s="23"/>
       <c r="M20" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B21" s="40" t="str">
         <f>'Controleur CA'!B21</f>
@@ -4209,12 +3968,12 @@
       <c r="K21" s="23"/>
       <c r="L21" s="23"/>
       <c r="M21" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B22" s="40" t="str">
         <f>'Controleur CA'!B22</f>
@@ -4234,12 +3993,12 @@
       <c r="K22" s="23"/>
       <c r="L22" s="23"/>
       <c r="M22" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B23" s="40" t="str">
         <f>'Controleur CA'!B23</f>
@@ -4259,12 +4018,12 @@
       <c r="K23" s="23"/>
       <c r="L23" s="23"/>
       <c r="M23" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B24" s="40" t="str">
         <f>'Controleur CA'!B24</f>
@@ -4284,7 +4043,7 @@
       <c r="K24" s="23"/>
       <c r="L24" s="23"/>
       <c r="M24" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -4309,7 +4068,32 @@
       <c r="K25" s="40"/>
       <c r="L25" s="40"/>
       <c r="M25" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="23">
+        <v>26</v>
+      </c>
+      <c r="B26" s="40" t="str">
+        <f>'Controleur CA'!B26</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C26" s="26" t="str">
+        <f>'Controleur CA'!F26</f>
+        <v>Vérifier que la liste des champs de la couche point contrôle correspond aux spécifications QGIS</v>
+      </c>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="40"/>
+      <c r="L26" s="40"/>
+      <c r="M26" s="23" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -4319,10 +4103,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD25"/>
+      <selection activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4343,7 +4127,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B1" s="30" t="s">
         <v>0</v>
@@ -4352,34 +4136,34 @@
         <v>3</v>
       </c>
       <c r="D1" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="H1" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="K1" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="L1" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="M1" s="34" t="s">
         <v>87</v>
-      </c>
-      <c r="H1" s="30" t="s">
-        <v>86</v>
-      </c>
-      <c r="I1" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="J1" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="K1" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="L1" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="M1" s="34" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -4404,7 +4188,7 @@
       <c r="K2" s="32"/>
       <c r="L2" s="32"/>
       <c r="M2" s="32" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -4429,7 +4213,7 @@
       <c r="K3" s="23"/>
       <c r="L3" s="23"/>
       <c r="M3" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -4454,7 +4238,7 @@
       <c r="K4" s="23"/>
       <c r="L4" s="23"/>
       <c r="M4" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -4479,7 +4263,7 @@
       <c r="K5" s="23"/>
       <c r="L5" s="23"/>
       <c r="M5" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -4504,7 +4288,7 @@
       <c r="K6" s="23"/>
       <c r="L6" s="23"/>
       <c r="M6" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -4529,7 +4313,7 @@
       <c r="K7" s="23"/>
       <c r="L7" s="23"/>
       <c r="M7" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -4554,7 +4338,7 @@
       <c r="K8" s="23"/>
       <c r="L8" s="23"/>
       <c r="M8" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -4579,7 +4363,7 @@
       <c r="K9" s="23"/>
       <c r="L9" s="23"/>
       <c r="M9" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -4604,7 +4388,7 @@
       <c r="K10" s="23"/>
       <c r="L10" s="23"/>
       <c r="M10" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -4629,7 +4413,7 @@
       <c r="K11" s="23"/>
       <c r="L11" s="23"/>
       <c r="M11" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -4654,7 +4438,7 @@
       <c r="K12" s="23"/>
       <c r="L12" s="23"/>
       <c r="M12" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -4679,7 +4463,7 @@
       <c r="K13" s="23"/>
       <c r="L13" s="23"/>
       <c r="M13" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -4704,12 +4488,12 @@
       <c r="K14" s="23"/>
       <c r="L14" s="23"/>
       <c r="M14" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B15" t="str">
         <f>'Controleur CA'!B15</f>
@@ -4729,12 +4513,12 @@
       <c r="K15" s="23"/>
       <c r="L15" s="23"/>
       <c r="M15" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B16" t="str">
         <f>'Controleur CA'!B16</f>
@@ -4754,12 +4538,12 @@
       <c r="K16" s="23"/>
       <c r="L16" s="23"/>
       <c r="M16" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B17" t="str">
         <f>'Controleur CA'!B17</f>
@@ -4779,12 +4563,12 @@
       <c r="K17" s="23"/>
       <c r="L17" s="23"/>
       <c r="M17" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B18" t="str">
         <f>'Controleur CA'!B18</f>
@@ -4804,12 +4588,12 @@
       <c r="K18" s="23"/>
       <c r="L18" s="23"/>
       <c r="M18" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B19" t="str">
         <f>'Controleur CA'!B19</f>
@@ -4829,12 +4613,12 @@
       <c r="K19" s="23"/>
       <c r="L19" s="23"/>
       <c r="M19" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B20" t="str">
         <f>'Controleur CA'!B20</f>
@@ -4854,12 +4638,12 @@
       <c r="K20" s="23"/>
       <c r="L20" s="23"/>
       <c r="M20" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B21" t="str">
         <f>'Controleur CA'!B21</f>
@@ -4879,12 +4663,12 @@
       <c r="K21" s="23"/>
       <c r="L21" s="23"/>
       <c r="M21" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B22" t="str">
         <f>'Controleur CA'!B22</f>
@@ -4904,12 +4688,12 @@
       <c r="K22" s="23"/>
       <c r="L22" s="23"/>
       <c r="M22" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B23" t="str">
         <f>'Controleur CA'!B23</f>
@@ -4929,12 +4713,12 @@
       <c r="K23" s="23"/>
       <c r="L23" s="23"/>
       <c r="M23" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B24" t="str">
         <f>'Controleur CA'!B24</f>
@@ -4954,7 +4738,7 @@
       <c r="K24" s="23"/>
       <c r="L24" s="23"/>
       <c r="M24" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -4979,7 +4763,32 @@
       <c r="K25" s="40"/>
       <c r="L25" s="40"/>
       <c r="M25" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="23">
+        <v>26</v>
+      </c>
+      <c r="B26" s="40" t="str">
+        <f>'Controleur CA'!B26</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C26" s="26" t="str">
+        <f>'Controleur CA'!F26</f>
+        <v>Vérifier que la liste des champs de la couche point contrôle correspond aux spécifications QGIS</v>
+      </c>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="40"/>
+      <c r="L26" s="40"/>
+      <c r="M26" s="23" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -4989,10 +4798,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5014,7 +4823,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B1" s="30" t="s">
         <v>0</v>
@@ -5023,34 +4832,34 @@
         <v>3</v>
       </c>
       <c r="D1" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="H1" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="K1" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="L1" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="M1" s="34" t="s">
         <v>87</v>
-      </c>
-      <c r="H1" s="30" t="s">
-        <v>86</v>
-      </c>
-      <c r="I1" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="J1" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="K1" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="L1" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="M1" s="34" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -5075,7 +4884,7 @@
       <c r="K2" s="32"/>
       <c r="L2" s="32"/>
       <c r="M2" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -5146,7 +4955,7 @@
       <c r="K5" s="23"/>
       <c r="L5" s="23"/>
       <c r="M5" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -5194,7 +5003,7 @@
       <c r="K7" s="23"/>
       <c r="L7" s="23"/>
       <c r="M7" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -5219,7 +5028,7 @@
       <c r="K8" s="23"/>
       <c r="L8" s="23"/>
       <c r="M8" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -5244,7 +5053,7 @@
       <c r="K9" s="23"/>
       <c r="L9" s="23"/>
       <c r="M9" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -5269,7 +5078,7 @@
       <c r="K10" s="23"/>
       <c r="L10" s="23"/>
       <c r="M10" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -5294,7 +5103,7 @@
       <c r="K11" s="23"/>
       <c r="L11" s="23"/>
       <c r="M11" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -5319,7 +5128,7 @@
       <c r="K12" s="23"/>
       <c r="L12" s="23"/>
       <c r="M12" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -5344,7 +5153,7 @@
       <c r="K13" s="23"/>
       <c r="L13" s="23"/>
       <c r="M13" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -5369,12 +5178,12 @@
       <c r="K14" s="23"/>
       <c r="L14" s="23"/>
       <c r="M14" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B15" t="str">
         <f>'Controleur CA'!B15</f>
@@ -5394,12 +5203,12 @@
       <c r="K15" s="23"/>
       <c r="L15" s="23"/>
       <c r="M15" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B16" t="str">
         <f>'Controleur CA'!B16</f>
@@ -5419,12 +5228,12 @@
       <c r="K16" s="23"/>
       <c r="L16" s="23"/>
       <c r="M16" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B17" t="str">
         <f>'Controleur CA'!B17</f>
@@ -5444,12 +5253,12 @@
       <c r="K17" s="23"/>
       <c r="L17" s="23"/>
       <c r="M17" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B18" t="str">
         <f>'Controleur CA'!B18</f>
@@ -5469,12 +5278,12 @@
       <c r="K18" s="23"/>
       <c r="L18" s="23"/>
       <c r="M18" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B19" t="str">
         <f>'Controleur CA'!B19</f>
@@ -5494,12 +5303,12 @@
       <c r="K19" s="23"/>
       <c r="L19" s="23"/>
       <c r="M19" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B20" t="str">
         <f>'Controleur CA'!B20</f>
@@ -5519,12 +5328,12 @@
       <c r="K20" s="23"/>
       <c r="L20" s="23"/>
       <c r="M20" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B21" t="str">
         <f>'Controleur CA'!B21</f>
@@ -5544,12 +5353,12 @@
       <c r="K21" s="23"/>
       <c r="L21" s="23"/>
       <c r="M21" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B22" t="str">
         <f>'Controleur CA'!B22</f>
@@ -5569,12 +5378,12 @@
       <c r="K22" s="23"/>
       <c r="L22" s="23"/>
       <c r="M22" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B23" t="str">
         <f>'Controleur CA'!B23</f>
@@ -5594,12 +5403,12 @@
       <c r="K23" s="23"/>
       <c r="L23" s="23"/>
       <c r="M23" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B24" t="str">
         <f>'Controleur CA'!B24</f>
@@ -5619,7 +5428,7 @@
       <c r="K24" s="23"/>
       <c r="L24" s="23"/>
       <c r="M24" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -5644,7 +5453,32 @@
       <c r="K25" s="40"/>
       <c r="L25" s="40"/>
       <c r="M25" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="23">
+        <v>26</v>
+      </c>
+      <c r="B26" s="40" t="str">
+        <f>'Controleur CA'!B26</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C26" s="26" t="str">
+        <f>'Controleur CA'!F26</f>
+        <v>Vérifier que la liste des champs de la couche point contrôle correspond aux spécifications QGIS</v>
+      </c>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="40"/>
+      <c r="L26" s="40"/>
+      <c r="M26" s="23" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -5654,10 +5488,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView topLeftCell="D12" workbookViewId="0">
+      <selection activeCell="D26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5679,7 +5513,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B1" s="30" t="s">
         <v>0</v>
@@ -5688,34 +5522,34 @@
         <v>3</v>
       </c>
       <c r="D1" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="H1" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="K1" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="L1" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="M1" s="34" t="s">
         <v>87</v>
-      </c>
-      <c r="H1" s="30" t="s">
-        <v>86</v>
-      </c>
-      <c r="I1" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="J1" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="K1" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="L1" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="M1" s="34" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -5740,7 +5574,7 @@
       <c r="K2" s="32"/>
       <c r="L2" s="32"/>
       <c r="M2" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -5765,7 +5599,7 @@
       <c r="K3" s="23"/>
       <c r="L3" s="23"/>
       <c r="M3" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -5790,7 +5624,7 @@
       <c r="K4" s="23"/>
       <c r="L4" s="23"/>
       <c r="M4" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -5815,7 +5649,7 @@
       <c r="K5" s="23"/>
       <c r="L5" s="23"/>
       <c r="M5" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -5840,7 +5674,7 @@
       <c r="K6" s="23"/>
       <c r="L6" s="23"/>
       <c r="M6" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -5865,7 +5699,7 @@
       <c r="K7" s="23"/>
       <c r="L7" s="23"/>
       <c r="M7" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -5890,7 +5724,7 @@
       <c r="K8" s="23"/>
       <c r="L8" s="23"/>
       <c r="M8" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -5915,7 +5749,7 @@
       <c r="K9" s="23"/>
       <c r="L9" s="23"/>
       <c r="M9" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -5940,7 +5774,7 @@
       <c r="K10" s="23"/>
       <c r="L10" s="23"/>
       <c r="M10" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -5965,7 +5799,7 @@
       <c r="K11" s="23"/>
       <c r="L11" s="23"/>
       <c r="M11" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -5990,7 +5824,7 @@
       <c r="K12" s="23"/>
       <c r="L12" s="23"/>
       <c r="M12" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -6015,7 +5849,7 @@
       <c r="K13" s="23"/>
       <c r="L13" s="23"/>
       <c r="M13" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -6040,12 +5874,12 @@
       <c r="K14" s="23"/>
       <c r="L14" s="23"/>
       <c r="M14" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B15" t="str">
         <f>'Controleur CA'!B15</f>
@@ -6065,12 +5899,12 @@
       <c r="K15" s="23"/>
       <c r="L15" s="23"/>
       <c r="M15" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B16" t="str">
         <f>'Controleur CA'!B16</f>
@@ -6090,12 +5924,12 @@
       <c r="K16" s="23"/>
       <c r="L16" s="23"/>
       <c r="M16" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B17" t="str">
         <f>'Controleur CA'!B17</f>
@@ -6115,12 +5949,12 @@
       <c r="K17" s="23"/>
       <c r="L17" s="23"/>
       <c r="M17" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B18" t="str">
         <f>'Controleur CA'!B18</f>
@@ -6140,12 +5974,12 @@
       <c r="K18" s="23"/>
       <c r="L18" s="23"/>
       <c r="M18" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B19" t="str">
         <f>'Controleur CA'!B19</f>
@@ -6165,12 +5999,12 @@
       <c r="K19" s="23"/>
       <c r="L19" s="23"/>
       <c r="M19" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B20" t="str">
         <f>'Controleur CA'!B20</f>
@@ -6190,12 +6024,12 @@
       <c r="K20" s="23"/>
       <c r="L20" s="23"/>
       <c r="M20" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B21" t="str">
         <f>'Controleur CA'!B21</f>
@@ -6215,12 +6049,12 @@
       <c r="K21" s="23"/>
       <c r="L21" s="23"/>
       <c r="M21" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B22" t="str">
         <f>'Controleur CA'!B22</f>
@@ -6240,12 +6074,12 @@
       <c r="K22" s="23"/>
       <c r="L22" s="23"/>
       <c r="M22" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B23" t="str">
         <f>'Controleur CA'!B23</f>
@@ -6265,12 +6099,12 @@
       <c r="K23" s="23"/>
       <c r="L23" s="23"/>
       <c r="M23" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B24" t="str">
         <f>'Controleur CA'!B24</f>
@@ -6290,7 +6124,7 @@
       <c r="K24" s="23"/>
       <c r="L24" s="23"/>
       <c r="M24" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -6315,7 +6149,728 @@
       <c r="K25" s="40"/>
       <c r="L25" s="40"/>
       <c r="M25" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="23">
+        <v>26</v>
+      </c>
+      <c r="B26" s="40" t="str">
+        <f>'Controleur CA'!B26</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C26" s="26" t="str">
+        <f>'Controleur CA'!F26</f>
+        <v>Vérifier que la liste des champs de la couche point contrôle correspond aux spécifications QGIS</v>
+      </c>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="40"/>
+      <c r="L26" s="40"/>
+      <c r="M26" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M26"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:XFD26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="77.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="K1" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="L1" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="M1" s="34" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="27">
+        <v>1</v>
+      </c>
+      <c r="B2" t="str">
+        <f>'Controleur CA'!B2</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C2" s="28" t="str">
+        <f>'Controleur CA'!F2</f>
+        <v>Vérifier que la colonne C6 contient "C3A BLO5"</v>
+      </c>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="25">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <f>'Controleur CA'!B3</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C3" s="26" t="str">
+        <f>'Controleur CA'!F3</f>
+        <v>Parcourir la table cable_infra. Pour chaque objet de la table de type infra_orange, vérifier qu'il existe une correspondance dans la C3A</v>
+      </c>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="25">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <f>'Controleur CA'!B4</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C4" s="26" t="str">
+        <f>'Controleur CA'!F4</f>
+        <v>Parcourir la C3A. Pour chaque ligne, vérifier qu'il existe une correspondance dans la table_infra</v>
+      </c>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="25">
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <f>'Controleur CA'!B5</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C5" s="26" t="str">
+        <f>'Controleur CA'!F5</f>
+        <v>Vérifier qu'il existe une fiche poteaux pour chaque poteaux de la C3A</v>
+      </c>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="25">
+        <v>5</v>
+      </c>
+      <c r="B6" t="str">
+        <f>'Controleur CA'!B6</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C6" s="26" t="str">
+        <f>'Controleur CA'!F6</f>
+        <v>vérifier que le couple (id, type) colonne C-D et E-F est cohérent avec la table point_technique</v>
+      </c>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="25">
+        <v>6</v>
+      </c>
+      <c r="B7" t="str">
+        <f>'Controleur CA'!B7</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C7" s="26" t="str">
+        <f>'Controleur CA'!F7</f>
+        <v>Si la colonne I est vide, la colonne J doit être laissée vide.</v>
+      </c>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="25">
+        <v>7</v>
+      </c>
+      <c r="B8" t="str">
+        <f>'Controleur CA'!B8</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C8" s="26" t="str">
+        <f>'Controleur CA'!F8</f>
+        <v>Vérifier que la colonne C et la colonne F commence par un nombre sur 5 caracteres suivant un "/" sans espace.</v>
+      </c>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="25">
+        <v>8</v>
+      </c>
+      <c r="B9" t="str">
+        <f>'Controleur CA'!B9</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C9" s="26" t="str">
+        <f>'Controleur CA'!F9</f>
+        <v>Vérifier que la colonne G est supérieure ou égal à 1</v>
+      </c>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="25">
+        <v>9</v>
+      </c>
+      <c r="B10" t="str">
+        <f>'Controleur CA'!B10</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C10" s="26" t="str">
+        <f>'Controleur CA'!F10</f>
+        <v>Vérifier que les valeurs sont contenues dans la liste déroulante dans les colonnes où il y en a une</v>
+      </c>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="25">
+        <v>10</v>
+      </c>
+      <c r="B11" t="str">
+        <f>'Controleur CA'!B11</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C11" s="26" t="str">
+        <f>'Controleur CA'!F11</f>
+        <v>Vérifier si le fichier C7 existant dans le cas où la colonne M ou N contient l'une des valeurs suivantes "oui remplacement appui" ou "oui renforcement appui avec commande d'appui"</v>
+      </c>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="25">
+        <v>11</v>
+      </c>
+      <c r="B12" t="str">
+        <f>'Controleur CA'!B12</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C12" s="26" t="str">
+        <f>'Controleur CA'!F12</f>
+        <v>Vérifier que l'appui est présent dans la C7 si la colonne M ou N contient l'une des valeurs suivantes "oui remplacement appui" ou "oui renforcement appui avec commande d'appui"</v>
+      </c>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="25">
+        <v>12</v>
+      </c>
+      <c r="B13" t="str">
+        <f>'Controleur CA'!B13</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C13" s="26" t="str">
+        <f>'Controleur CA'!F13</f>
+        <v>Vérifier que le couple (colonne C, colonne E) ne forme pas une combinaison dans la liste suivante : [CT – CT], [C – CT], [CT – C], [CT– P], [CT – A], [A – CT], [P-CT]</v>
+      </c>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="25">
+        <v>13</v>
+      </c>
+      <c r="B14" t="str">
+        <f>'Controleur CA'!B14</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C14" s="26" t="str">
+        <f>'Controleur CA'!F14</f>
+        <v>Dans le cas d'une liaison [C - C], la colonne H doit prendre les valeurs contenues dans cette liste : ["28","32","45","60","80","100","150","Sous-tubage existant","caniveau","galerie"]</v>
+      </c>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" t="str">
+        <f>'Controleur CA'!B15</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C15" s="26" t="str">
+        <f>'Controleur CA'!F15</f>
+        <v>Dans le cas d'une liaison [C - IMB], la colonne H doit contenir la valeur "adduction"</v>
+      </c>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" t="str">
+        <f>'Controleur CA'!B16</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C16" s="26" t="str">
+        <f>'Controleur CA'!F16</f>
+        <v>Dans le cas d'une liaison [C - IMB], la colonne F doit être vide</v>
+      </c>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" t="str">
+        <f>'Controleur CA'!B17</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C17" s="26" t="str">
+        <f>'Controleur CA'!F17</f>
+        <v>Dans le cas d'une liaison [C - IMB], la colonne G doit contenir la valeur "7"</v>
+      </c>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" t="str">
+        <f>'Controleur CA'!B18</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C18" s="26" t="str">
+        <f>'Controleur CA'!F18</f>
+        <v>Dans le cas d'une liaison [C - F], la colonne F doit être vide</v>
+      </c>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" t="str">
+        <f>'Controleur CA'!B19</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C19" s="26" t="str">
+        <f>'Controleur CA'!F19</f>
+        <v>Dans le cas d'une liaison [C - F], la colonne H doit contenir la valeur "transition"</v>
+      </c>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" t="str">
+        <f>'Controleur CA'!B20</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C20" s="26" t="str">
+        <f>'Controleur CA'!F20</f>
+        <v>Dans le cas d'une liaison [C -F], la colonne G doit contenir la valeur "7"</v>
+      </c>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" t="str">
+        <f>'Controleur CA'!B21</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C21" s="26" t="str">
+        <f>'Controleur CA'!F21</f>
+        <v>Dans le cas d'une liaison [C -P] ou [C-PT], la colonne H doit contenir la valeur "transition"</v>
+      </c>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" t="str">
+        <f>'Controleur CA'!B22</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C22" s="26" t="str">
+        <f>'Controleur CA'!F22</f>
+        <v>Dans le cas d'une liaison [C-PT], la colonne F doit être vide</v>
+      </c>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" t="str">
+        <f>'Controleur CA'!B23</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C23" s="26" t="str">
+        <f>'Controleur CA'!F23</f>
+        <v>Dans le cas d'une liaison [CT-P], les colonne B et D doivent être vide</v>
+      </c>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" t="str">
+        <f>'Controleur CA'!B24</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C24" s="26" t="str">
+        <f>'Controleur CA'!F24</f>
+        <v>Dans le cas d'une liaison [CT-P], la colonne H doit contenir la valeur "transition"</v>
+      </c>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="23">
+        <v>25</v>
+      </c>
+      <c r="B25" s="40" t="str">
+        <f>'Controleur CA'!B25</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C25" s="26" t="str">
+        <f>'Controleur CA'!F25</f>
+        <v>Vérifier que le nom des fiches poteau sont au format insee_nom</v>
+      </c>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="40"/>
+      <c r="L25" s="40"/>
+      <c r="M25" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="23">
+        <v>26</v>
+      </c>
+      <c r="B26" s="40" t="str">
+        <f>'Controleur CA'!B26</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C26" s="26" t="str">
+        <f>'Controleur CA'!F26</f>
+        <v>Vérifier que la liste des champs de la couche point contrôle correspond aux spécifications QGIS</v>
+      </c>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="40"/>
+      <c r="L26" s="40"/>
+      <c r="M26" s="23" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -6324,6 +6879,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document Microsoft Word" ma:contentTypeID="0x01010066910ADB61686C45A75A7A744D7D5C8E0022B63E0AEFBB2040BF2A3B1B4BE32EE5" ma:contentTypeVersion="4" ma:contentTypeDescription="Document Microsoft Word vierge." ma:contentTypeScope="" ma:versionID="0a4943d90c7214e3c95a70ccb3c8346b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c97f8e9-86c7-4e99-9925-cc9540b321fe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eeaa8661ba6ba22f90735bcd04aade41" ns2:_="">
     <xsd:import namespace="9c97f8e9-86c7-4e99-9925-cc9540b321fe"/>
@@ -6526,15 +7090,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -6550,6 +7105,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F02C15CB-09E5-4D58-8C63-77232C75BB18}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8B2112A-C178-4B00-8690-1CA741C188F5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6563,14 +7126,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F02C15CB-09E5-4D58-8C63-77232C75BB18}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
- Dans les controles 14-25, stopper directement si aucun contrôle n'est selectionné - Le traitement général des shapes est sous fonction générique - Les contrôles de champs de shapes (26,27) sont dans une fonction dédiée au controle des champs - Ajout du contrôle 27 - Libellés sous variables afin de centraliser - champs de référence en dictionnaire de tableau plutôt que tableau, avec pour chaque champ les types et reference livrable
</commit_message>
<xml_diff>
--- a/Documentation/Controleur.xlsx
+++ b/Documentation/Controleur.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="110">
   <si>
     <t>Famille</t>
   </si>
@@ -345,6 +345,15 @@
   </si>
   <si>
     <t>La structuration des champs de la couche point contrôle est incorrecte</t>
+  </si>
+  <si>
+    <t>Couche prises</t>
+  </si>
+  <si>
+    <t>Vérifier que la liste des champs de la couche prises correspond aux spécifications QGIS</t>
+  </si>
+  <si>
+    <t>La structuration des champs de la couche prises est incorrecte</t>
   </si>
 </sst>
 </file>
@@ -1093,10 +1102,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1114,7 +1123,7 @@
     <col min="14" max="14" width="35.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>42</v>
       </c>
@@ -2005,6 +2014,40 @@
       <c r="L26" s="12"/>
       <c r="M26" s="12"/>
       <c r="N26" s="12"/>
+    </row>
+    <row r="27" spans="1:14" s="42" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="35">
+        <v>27</v>
+      </c>
+      <c r="B27" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="I27" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I24"/>
@@ -2018,7 +2061,7 @@
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2674,7 +2717,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="23">
         <v>26</v>
       </c>
@@ -2699,9 +2742,30 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27"/>
-      <c r="C27"/>
+    <row r="27" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="23">
+        <v>27</v>
+      </c>
+      <c r="B27" s="40" t="str">
+        <f>'Controleur CA'!B27</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C27" s="26" t="str">
+        <f>'Controleur CA'!F27</f>
+        <v>Vérifier que la liste des champs de la couche prises correspond aux spécifications QGIS</v>
+      </c>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="40"/>
+      <c r="L27" s="40"/>
+      <c r="M27" s="23" t="s">
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2711,10 +2775,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
+      <selection activeCell="A27" sqref="A27:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3400,6 +3464,31 @@
         <v>56</v>
       </c>
     </row>
+    <row r="27" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="23">
+        <v>27</v>
+      </c>
+      <c r="B27" s="40" t="str">
+        <f>'Controleur CA'!B27</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C27" s="26" t="str">
+        <f>'Controleur CA'!F27</f>
+        <v>Vérifier que la liste des champs de la couche prises correspond aux spécifications QGIS</v>
+      </c>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="40"/>
+      <c r="L27" s="40"/>
+      <c r="M27" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3407,10 +3496,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
+      <selection activeCell="A27" sqref="A27:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4096,6 +4185,31 @@
         <v>56</v>
       </c>
     </row>
+    <row r="27" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="23">
+        <v>27</v>
+      </c>
+      <c r="B27" s="40" t="str">
+        <f>'Controleur CA'!B27</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C27" s="26" t="str">
+        <f>'Controleur CA'!F27</f>
+        <v>Vérifier que la liste des champs de la couche prises correspond aux spécifications QGIS</v>
+      </c>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="40"/>
+      <c r="L27" s="40"/>
+      <c r="M27" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4103,10 +4217,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
+      <selection activeCell="A27" sqref="A27:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4791,6 +4905,31 @@
         <v>56</v>
       </c>
     </row>
+    <row r="27" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="23">
+        <v>27</v>
+      </c>
+      <c r="B27" s="40" t="str">
+        <f>'Controleur CA'!B27</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C27" s="26" t="str">
+        <f>'Controleur CA'!F27</f>
+        <v>Vérifier que la liste des champs de la couche prises correspond aux spécifications QGIS</v>
+      </c>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="40"/>
+      <c r="L27" s="40"/>
+      <c r="M27" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4798,10 +4937,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
+      <selection activeCell="A27" sqref="A27:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5481,6 +5620,31 @@
         <v>56</v>
       </c>
     </row>
+    <row r="27" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="23">
+        <v>27</v>
+      </c>
+      <c r="B27" s="40" t="str">
+        <f>'Controleur CA'!B27</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C27" s="26" t="str">
+        <f>'Controleur CA'!F27</f>
+        <v>Vérifier que la liste des champs de la couche prises correspond aux spécifications QGIS</v>
+      </c>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="40"/>
+      <c r="L27" s="40"/>
+      <c r="M27" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5488,10 +5652,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView topLeftCell="D12" workbookViewId="0">
-      <selection activeCell="D26" sqref="A26:XFD26"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6177,6 +6341,31 @@
         <v>56</v>
       </c>
     </row>
+    <row r="27" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="23">
+        <v>27</v>
+      </c>
+      <c r="B27" s="40" t="str">
+        <f>'Controleur CA'!B27</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C27" s="26" t="str">
+        <f>'Controleur CA'!F27</f>
+        <v>Vérifier que la liste des champs de la couche prises correspond aux spécifications QGIS</v>
+      </c>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="40"/>
+      <c r="L27" s="40"/>
+      <c r="M27" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6184,10 +6373,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6873,6 +7062,31 @@
         <v>56</v>
       </c>
     </row>
+    <row r="27" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="23">
+        <v>27</v>
+      </c>
+      <c r="B27" s="40" t="str">
+        <f>'Controleur CA'!B27</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C27" s="26" t="str">
+        <f>'Controleur CA'!F27</f>
+        <v>Vérifier que la liste des champs de la couche prises correspond aux spécifications QGIS</v>
+      </c>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="40"/>
+      <c r="L27" s="40"/>
+      <c r="M27" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6888,6 +7102,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <DocSource xmlns="9c97f8e9-86c7-4e99-9925-cc9540b321fe">Interne</DocSource>
+    <Language xmlns="9c97f8e9-86c7-4e99-9925-cc9540b321fe">Français</Language>
+    <DocType xmlns="9c97f8e9-86c7-4e99-9925-cc9540b321fe">Méthode / Qualité / Organisation / Procédure</DocType>
+    <DocState xmlns="9c97f8e9-86c7-4e99-9925-cc9540b321fe">Finalisé</DocState>
+    <Author0 xmlns="9c97f8e9-86c7-4e99-9925-cc9540b321fe" xsi:nil="true"/>
+    <Description0 xmlns="9c97f8e9-86c7-4e99-9925-cc9540b321fe" xsi:nil="true"/>
+    <DocConf xmlns="9c97f8e9-86c7-4e99-9925-cc9540b321fe">Interne</DocConf>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document Microsoft Word" ma:contentTypeID="0x01010066910ADB61686C45A75A7A744D7D5C8E0022B63E0AEFBB2040BF2A3B1B4BE32EE5" ma:contentTypeVersion="4" ma:contentTypeDescription="Document Microsoft Word vierge." ma:contentTypeScope="" ma:versionID="0a4943d90c7214e3c95a70ccb3c8346b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c97f8e9-86c7-4e99-9925-cc9540b321fe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eeaa8661ba6ba22f90735bcd04aade41" ns2:_="">
     <xsd:import namespace="9c97f8e9-86c7-4e99-9925-cc9540b321fe"/>
@@ -7090,20 +7318,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <DocSource xmlns="9c97f8e9-86c7-4e99-9925-cc9540b321fe">Interne</DocSource>
-    <Language xmlns="9c97f8e9-86c7-4e99-9925-cc9540b321fe">Français</Language>
-    <DocType xmlns="9c97f8e9-86c7-4e99-9925-cc9540b321fe">Autre</DocType>
-    <DocState xmlns="9c97f8e9-86c7-4e99-9925-cc9540b321fe">Finalisé</DocState>
-    <Author0 xmlns="9c97f8e9-86c7-4e99-9925-cc9540b321fe" xsi:nil="true"/>
-    <Description0 xmlns="9c97f8e9-86c7-4e99-9925-cc9540b321fe" xsi:nil="true"/>
-    <DocConf xmlns="9c97f8e9-86c7-4e99-9925-cc9540b321fe">Interne</DocConf>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F02C15CB-09E5-4D58-8C63-77232C75BB18}">
   <ds:schemaRefs>
@@ -7113,6 +7327,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFD779FF-B039-4DC7-8903-586F168B5B9F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9c97f8e9-86c7-4e99-9925-cc9540b321fe"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8B2112A-C178-4B00-8690-1CA741C188F5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7128,20 +7358,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFD779FF-B039-4DC7-8903-586F168B5B9F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9c97f8e9-86c7-4e99-9925-cc9540b321fe"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
*** Version 7 *** - Meilleure mise en forme du XML - Ajout des contrôles 39,47,48 - Ajout du prefixpath de Qgis, variable selon si c'est executé en executable ou avec le .bat - La progress bar est 100% variable, n'ayant plus un 100% forcé au dernier contrôle mais detecté automatiquement - get_shape permet maintenant aussi de vérifier l'existance d'une shape selon un paramètre à activer
</commit_message>
<xml_diff>
--- a/Documentation/Controleur.xlsx
+++ b/Documentation/Controleur.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="315" windowWidth="6915" windowHeight="6540"/>
+    <workbookView xWindow="480" yWindow="315" windowWidth="6915" windowHeight="6540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Controleur CA" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1643" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1681" uniqueCount="188">
   <si>
     <t>Famille</t>
   </si>
@@ -610,7 +610,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -632,18 +632,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -779,7 +767,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -861,12 +849,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1177,8 +1159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1289,7 +1271,9 @@
       <c r="I3" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="26"/>
+      <c r="J3" s="26" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="4" spans="1:10" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="25">
@@ -1319,7 +1303,9 @@
       <c r="I4" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="26"/>
+      <c r="J4" s="26" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="5" spans="1:10" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="25">
@@ -1349,7 +1335,9 @@
       <c r="I5" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="26"/>
+      <c r="J5" s="26" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="6" spans="1:10" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="25">
@@ -1379,7 +1367,9 @@
       <c r="I6" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="J6" s="26"/>
+      <c r="J6" s="26" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="7" spans="1:10" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="25">
@@ -1409,7 +1399,9 @@
       <c r="I7" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="26"/>
+      <c r="J7" s="26" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="8" spans="1:10" s="18" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="25">
@@ -1439,7 +1431,9 @@
       <c r="I8" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="J8" s="26"/>
+      <c r="J8" s="26" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="9" spans="1:10" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="25">
@@ -1469,7 +1463,9 @@
       <c r="I9" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="26"/>
+      <c r="J9" s="26" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="10" spans="1:10" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="25">
@@ -1499,7 +1495,9 @@
       <c r="I10" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="J10" s="26"/>
+      <c r="J10" s="26" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="11" spans="1:10" s="18" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="25">
@@ -1529,7 +1527,9 @@
       <c r="I11" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="J11" s="26"/>
+      <c r="J11" s="26" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="12" spans="1:10" s="18" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="25">
@@ -1559,7 +1559,9 @@
       <c r="I12" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="J12" s="26"/>
+      <c r="J12" s="26" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="13" spans="1:10" s="18" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="25">
@@ -1589,7 +1591,9 @@
       <c r="I13" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="J13" s="26"/>
+      <c r="J13" s="26" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="14" spans="1:10" s="18" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="25">
@@ -1619,7 +1623,9 @@
       <c r="I14" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="J14" s="26"/>
+      <c r="J14" s="26" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="15" spans="1:10" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="25">
@@ -1649,7 +1655,9 @@
       <c r="I15" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="J15" s="26"/>
+      <c r="J15" s="26" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="16" spans="1:10" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="25">
@@ -1679,7 +1687,9 @@
       <c r="I16" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="J16" s="26"/>
+      <c r="J16" s="26" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="17" spans="1:18" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="25">
@@ -1709,7 +1719,9 @@
       <c r="I17" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="J17" s="26"/>
+      <c r="J17" s="26" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="18" spans="1:18" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="25">
@@ -1739,7 +1751,9 @@
       <c r="I18" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="J18" s="26"/>
+      <c r="J18" s="26" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="19" spans="1:18" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="25">
@@ -1769,7 +1783,9 @@
       <c r="I19" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="J19" s="26"/>
+      <c r="J19" s="26" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="20" spans="1:18" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="25">
@@ -1799,7 +1815,9 @@
       <c r="I20" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="J20" s="26"/>
+      <c r="J20" s="26" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="21" spans="1:18" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="25">
@@ -1829,7 +1847,9 @@
       <c r="I21" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="J21" s="26"/>
+      <c r="J21" s="26" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="22" spans="1:18" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="25">
@@ -1859,7 +1879,9 @@
       <c r="I22" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="J22" s="26"/>
+      <c r="J22" s="26" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="23" spans="1:18" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="25">
@@ -1889,7 +1911,9 @@
       <c r="I23" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="J23" s="26"/>
+      <c r="J23" s="26" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="24" spans="1:18" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="25">
@@ -1919,7 +1943,9 @@
       <c r="I24" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="J24" s="26"/>
+      <c r="J24" s="26" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="25" spans="1:18" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="25">
@@ -1947,7 +1973,9 @@
       <c r="I25" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="J25" s="26"/>
+      <c r="J25" s="26" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="26" spans="1:18" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="25">
@@ -1977,7 +2005,9 @@
       <c r="I26" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="J26" s="26"/>
+      <c r="J26" s="26" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="27" spans="1:18" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="25">
@@ -2007,7 +2037,9 @@
       <c r="I27" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="J27" s="26"/>
+      <c r="J27" s="26" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="28" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="25">
@@ -2037,7 +2069,9 @@
       <c r="I28" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="J28" s="26"/>
+      <c r="J28" s="26" t="s">
+        <v>181</v>
+      </c>
       <c r="K28" s="18"/>
       <c r="L28" s="18"/>
       <c r="M28" s="18"/>
@@ -2075,7 +2109,9 @@
       <c r="I29" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="J29" s="26"/>
+      <c r="J29" s="26" t="s">
+        <v>181</v>
+      </c>
       <c r="K29" s="18"/>
       <c r="L29" s="18"/>
       <c r="M29" s="18"/>
@@ -2113,7 +2149,9 @@
       <c r="I30" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="J30" s="26"/>
+      <c r="J30" s="26" t="s">
+        <v>181</v>
+      </c>
       <c r="K30" s="18"/>
       <c r="L30" s="18"/>
       <c r="M30" s="18"/>
@@ -2151,7 +2189,9 @@
       <c r="I31" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="J31" s="26"/>
+      <c r="J31" s="26" t="s">
+        <v>181</v>
+      </c>
       <c r="K31" s="18"/>
       <c r="L31" s="18"/>
       <c r="M31" s="18"/>
@@ -2189,7 +2229,9 @@
       <c r="I32" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="J32" s="26"/>
+      <c r="J32" s="26" t="s">
+        <v>181</v>
+      </c>
       <c r="K32" s="18"/>
       <c r="L32" s="18"/>
       <c r="M32" s="18"/>
@@ -2227,7 +2269,9 @@
       <c r="I33" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="J33" s="26"/>
+      <c r="J33" s="26" t="s">
+        <v>181</v>
+      </c>
       <c r="K33" s="18"/>
       <c r="L33" s="18"/>
       <c r="M33" s="18"/>
@@ -2265,7 +2309,9 @@
       <c r="I34" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="J34" s="26"/>
+      <c r="J34" s="26" t="s">
+        <v>181</v>
+      </c>
       <c r="K34" s="18"/>
       <c r="L34" s="18"/>
       <c r="M34" s="18"/>
@@ -2303,7 +2349,9 @@
       <c r="I35" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="J35" s="26"/>
+      <c r="J35" s="26" t="s">
+        <v>181</v>
+      </c>
       <c r="K35" s="18"/>
       <c r="L35" s="18"/>
       <c r="M35" s="18"/>
@@ -2341,7 +2389,9 @@
       <c r="I36" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="J36" s="26"/>
+      <c r="J36" s="26" t="s">
+        <v>181</v>
+      </c>
       <c r="K36" s="18"/>
       <c r="L36" s="18"/>
       <c r="M36" s="18"/>
@@ -2431,7 +2481,7 @@
       <c r="Q38" s="18"/>
       <c r="R38" s="18"/>
     </row>
-    <row r="39" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="26">
         <v>39</v>
       </c>
@@ -2485,7 +2535,7 @@
       <c r="E40" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="F40" s="32" t="s">
+      <c r="F40" s="27" t="s">
         <v>147</v>
       </c>
       <c r="G40" s="27" t="s">
@@ -2497,7 +2547,9 @@
       <c r="I40" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="J40" s="26"/>
+      <c r="J40" s="26" t="s">
+        <v>181</v>
+      </c>
       <c r="K40" s="18"/>
       <c r="L40" s="18"/>
       <c r="M40" s="18"/>
@@ -2523,7 +2575,7 @@
       <c r="E41" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="F41" s="33" t="s">
+      <c r="F41" s="27" t="s">
         <v>150</v>
       </c>
       <c r="G41" s="27"/>
@@ -2559,7 +2611,7 @@
       <c r="E42" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="F42" s="33" t="s">
+      <c r="F42" s="27" t="s">
         <v>152</v>
       </c>
       <c r="G42" s="27"/>
@@ -2589,7 +2641,7 @@
       </c>
       <c r="D43" s="26"/>
       <c r="E43" s="26"/>
-      <c r="F43" s="33" t="s">
+      <c r="F43" s="27" t="s">
         <v>153</v>
       </c>
       <c r="G43" s="27"/>
@@ -2619,7 +2671,7 @@
       </c>
       <c r="D44" s="26"/>
       <c r="E44" s="26"/>
-      <c r="F44" s="33" t="s">
+      <c r="F44" s="27" t="s">
         <v>154</v>
       </c>
       <c r="G44" s="27"/>
@@ -2725,7 +2777,9 @@
       <c r="I47" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="J47" s="26"/>
+      <c r="J47" s="26" t="s">
+        <v>181</v>
+      </c>
       <c r="K47" s="18"/>
       <c r="L47" s="18"/>
       <c r="M47" s="18"/>
@@ -2763,7 +2817,9 @@
       <c r="I48" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="J48" s="26"/>
+      <c r="J48" s="26" t="s">
+        <v>181</v>
+      </c>
       <c r="K48" s="18"/>
       <c r="L48" s="18"/>
       <c r="M48" s="18"/>
@@ -2845,7 +2901,7 @@
       </c>
       <c r="D51" s="26"/>
       <c r="E51" s="26"/>
-      <c r="F51" s="33" t="s">
+      <c r="F51" s="27" t="s">
         <v>169</v>
       </c>
       <c r="G51" s="27"/>
@@ -2965,7 +3021,7 @@
       </c>
       <c r="D55" s="26"/>
       <c r="E55" s="26"/>
-      <c r="F55" s="33" t="s">
+      <c r="F55" s="27" t="s">
         <v>178</v>
       </c>
       <c r="G55" s="27"/>
@@ -3064,8 +3120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M56"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O48" sqref="O48"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4491,7 +4547,9 @@
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
+      <c r="M39" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="19">
@@ -11984,7 +12042,7 @@
   <dimension ref="C9:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10:F12"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12019,11 +12077,11 @@
       </c>
       <c r="E10" s="4">
         <f>IF(ISERROR(SUMPRODUCT(('Controleur CA'!J:J="fait")*('Controleur CA'!B:B=C10))),"Aucun",SUMPRODUCT(('Controleur CA'!J:J="fait")*('Controleur CA'!B:B=C10)))</f>
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="F10" s="28">
         <f>E10/D10*100</f>
-        <v>8</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.25">
@@ -12036,11 +12094,11 @@
       </c>
       <c r="E11" s="4">
         <f>IF(ISERROR(SUMPRODUCT(('Controleur CA'!J:J="fait")*('Controleur CA'!B:B=C11))),"Aucun",SUMPRODUCT(('Controleur CA'!J:J="fait")*('Controleur CA'!B:B=C11)))</f>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F11" s="28">
         <f>E11/D11*100</f>
-        <v>8.3333333333333321</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="3:6" x14ac:dyDescent="0.25">
@@ -12053,11 +12111,11 @@
       </c>
       <c r="E12" s="4">
         <f>IF(ISERROR(SUMPRODUCT(('Controleur CA'!J:J="fait")*('Controleur CA'!B:B=C12))),"Aucun",SUMPRODUCT(('Controleur CA'!J:J="fait")*('Controleur CA'!B:B=C12)))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F12" s="28">
         <f>E12/D12*100</f>
-        <v>0</v>
+        <v>16.666666666666664</v>
       </c>
     </row>
   </sheetData>
@@ -12066,15 +12124,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document Microsoft Word" ma:contentTypeID="0x01010066910ADB61686C45A75A7A744D7D5C8E0022B63E0AEFBB2040BF2A3B1B4BE32EE5" ma:contentTypeVersion="4" ma:contentTypeDescription="Document Microsoft Word vierge." ma:contentTypeScope="" ma:versionID="0a4943d90c7214e3c95a70ccb3c8346b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c97f8e9-86c7-4e99-9925-cc9540b321fe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eeaa8661ba6ba22f90735bcd04aade41" ns2:_="">
     <xsd:import namespace="9c97f8e9-86c7-4e99-9925-cc9540b321fe"/>
@@ -12277,6 +12326,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -12292,14 +12350,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F02C15CB-09E5-4D58-8C63-77232C75BB18}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8B2112A-C178-4B00-8690-1CA741C188F5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12317,18 +12367,26 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F02C15CB-09E5-4D58-8C63-77232C75BB18}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFD779FF-B039-4DC7-8903-586F168B5B9F}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="9c97f8e9-86c7-4e99-9925-cc9540b321fe"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
- Si la shape n'existe pas, le contrôle de champs de shape gère l'exception d'ouverture et renvoie une erreur pour ce contrôle - Nouvelle version du XML livrables, plus complet et avec un nouveau modèle (par exemple au niveau du nommage) - Ajout du modele cible de CD21 dans le XML et aussi du modèle commun simplifié - Ajout du parseur de XML qui créer les variables à partir du XML, pour l'instant non intégré au programme
</commit_message>
<xml_diff>
--- a/Documentation/Controleur.xlsx
+++ b/Documentation/Controleur.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="315" windowWidth="6915" windowHeight="6540" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="315" windowWidth="6915" windowHeight="6540"/>
   </bookViews>
   <sheets>
     <sheet name="Controleur CA" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1681" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2360" uniqueCount="188">
   <si>
     <t>Famille</t>
   </si>
@@ -1159,8 +1159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R58"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3120,8 +3120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M56" sqref="D2:M56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3325,14 +3325,30 @@
         <f>'Controleur CA'!F6</f>
         <v>vérifier que le couple (id, type) colonne C-D et E-F est cohérent avec la table point_technique</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
+      <c r="D6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="L6" s="4" t="s">
         <v>50</v>
       </c>
@@ -4169,13 +4185,27 @@
         <f>'Controleur CA'!F26</f>
         <v>Vérifier que la liste des champs de la couche point technique correspond aux spécifications QGIS</v>
       </c>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
+      <c r="D26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="K26" s="4" t="s">
         <v>50</v>
       </c>
@@ -4198,13 +4228,27 @@
         <f>'Controleur CA'!F27</f>
         <v>Vérifier que la liste des champs de la couche prises correspond aux spécifications QGIS</v>
       </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
+      <c r="D27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="K27" s="4" t="s">
         <v>50</v>
       </c>
@@ -4227,13 +4271,27 @@
         <f>'Controleur CA'!F28</f>
         <v>Vérifier que la liste des champs de la couche SRO correspond aux spécifications QGIS</v>
       </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
+      <c r="D28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="K28" s="4" t="s">
         <v>50</v>
       </c>
@@ -4256,13 +4314,27 @@
         <f>'Controleur CA'!F29</f>
         <v>Vérifier que la liste des champs de la couche boitiers correspond aux spécifications QGIS</v>
       </c>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
+      <c r="D29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="K29" s="4" t="s">
         <v>50</v>
       </c>
@@ -4285,13 +4357,27 @@
         <f>'Controleur CA'!F30</f>
         <v>Vérifier que la liste des champs de la couche infrastructure correspond aux spécifications QGIS</v>
       </c>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
+      <c r="D30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="K30" s="4" t="s">
         <v>50</v>
       </c>
@@ -4314,13 +4400,27 @@
         <f>'Controleur CA'!F31</f>
         <v>Vérifier que la liste des champs de la couche racco_client correspond aux spécifications QGIS</v>
       </c>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
+      <c r="D31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="K31" s="4" t="s">
         <v>50</v>
       </c>
@@ -4343,13 +4443,27 @@
         <f>'Controleur CA'!F32</f>
         <v>Vérifier que la liste des champs de la couche cable correspond aux spécifications QGIS</v>
       </c>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
+      <c r="D32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="K32" s="4" t="s">
         <v>50</v>
       </c>
@@ -4372,13 +4486,27 @@
         <f>'Controleur CA'!F33</f>
         <v>Vérifier que la liste des champs de la couche ZPBO correspond aux spécifications QGIS</v>
       </c>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
+      <c r="D33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="K33" s="4" t="s">
         <v>50</v>
       </c>
@@ -4401,13 +4529,27 @@
         <f>'Controleur CA'!F34</f>
         <v>Vérifier que la liste des champs de la couche ZSRO correspond aux spécifications QGIS</v>
       </c>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
+      <c r="D34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="K34" s="4" t="s">
         <v>50</v>
       </c>
@@ -4430,18 +4572,36 @@
         <f>'Controleur CA'!F35</f>
         <v>Vérifier que la liste des champs de la couche ZPEC correspond aux spécifications QGIS</v>
       </c>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
+      <c r="D35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="K35" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
+      <c r="L35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M35" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="36" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="19">
@@ -4455,13 +4615,27 @@
         <f>'Controleur CA'!F36</f>
         <v>Vérifier que la liste des champs de la couche ZNRO correspond aux spécifications QGIS</v>
       </c>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
+      <c r="D36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="K36" s="4" t="s">
         <v>50</v>
       </c>
@@ -4484,18 +4658,36 @@
         <f>'Controleur CA'!F37</f>
         <v>Vérifier que la liste des champs de la couche NRO correspond aux spécifications QGIS</v>
       </c>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
+      <c r="D37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="K37" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
+      <c r="L37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M37" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="19">
@@ -4509,13 +4701,27 @@
         <f>'Controleur CA'!F38</f>
         <v>Vérifier que le numéro d'appui dans la C7 est sous la forme insee_identifiant</v>
       </c>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
+      <c r="D38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="K38" s="4" t="s">
         <v>50</v>
       </c>
@@ -4538,15 +4744,33 @@
         <f>'Controleur CA'!F39</f>
         <v>Vérifier que toutes les couches sont présentes selon les spec_QGIS</v>
       </c>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="4"/>
+      <c r="D39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L39" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="M39" s="4" t="s">
         <v>50</v>
       </c>
@@ -4733,9 +4957,7 @@
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
       <c r="L47" s="4"/>
-      <c r="M47" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="M47" s="4"/>
     </row>
     <row r="48" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="19">
@@ -4758,9 +4980,7 @@
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
       <c r="L48" s="4"/>
-      <c r="M48" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="M48" s="4"/>
     </row>
     <row r="49" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="19">
@@ -4956,8 +5176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M56"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:M56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5162,16 +5382,36 @@
         <f>'Controleur CA'!F6</f>
         <v>vérifier que le couple (id, type) colonne C-D et E-F est cohérent avec la table point_technique</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
+      <c r="D6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
@@ -6002,16 +6242,36 @@
         <f>'Controleur CA'!F26</f>
         <v>Vérifier que la liste des champs de la couche point technique correspond aux spécifications QGIS</v>
       </c>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
+      <c r="D26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="27" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
@@ -6025,16 +6285,36 @@
         <f>'Controleur CA'!F27</f>
         <v>Vérifier que la liste des champs de la couche prises correspond aux spécifications QGIS</v>
       </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
+      <c r="D27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M27" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="19">
@@ -6048,16 +6328,36 @@
         <f>'Controleur CA'!F28</f>
         <v>Vérifier que la liste des champs de la couche SRO correspond aux spécifications QGIS</v>
       </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
+      <c r="D28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M28" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="29" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="19">
@@ -6071,16 +6371,36 @@
         <f>'Controleur CA'!F29</f>
         <v>Vérifier que la liste des champs de la couche boitiers correspond aux spécifications QGIS</v>
       </c>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
+      <c r="D29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M29" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="30" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="19">
@@ -6094,16 +6414,36 @@
         <f>'Controleur CA'!F30</f>
         <v>Vérifier que la liste des champs de la couche infrastructure correspond aux spécifications QGIS</v>
       </c>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
+      <c r="D30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M30" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="31" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="19">
@@ -6117,16 +6457,36 @@
         <f>'Controleur CA'!F31</f>
         <v>Vérifier que la liste des champs de la couche racco_client correspond aux spécifications QGIS</v>
       </c>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
+      <c r="D31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M31" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="32" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="19">
@@ -6140,16 +6500,36 @@
         <f>'Controleur CA'!F32</f>
         <v>Vérifier que la liste des champs de la couche cable correspond aux spécifications QGIS</v>
       </c>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
+      <c r="D32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M32" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="33" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="19">
@@ -6163,16 +6543,36 @@
         <f>'Controleur CA'!F33</f>
         <v>Vérifier que la liste des champs de la couche ZPBO correspond aux spécifications QGIS</v>
       </c>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
+      <c r="D33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M33" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="34" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="19">
@@ -6186,16 +6586,36 @@
         <f>'Controleur CA'!F34</f>
         <v>Vérifier que la liste des champs de la couche ZSRO correspond aux spécifications QGIS</v>
       </c>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
+      <c r="D34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M34" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="35" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="19">
@@ -6209,16 +6629,36 @@
         <f>'Controleur CA'!F35</f>
         <v>Vérifier que la liste des champs de la couche ZPEC correspond aux spécifications QGIS</v>
       </c>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
+      <c r="D35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M35" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="36" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="19">
@@ -6232,16 +6672,36 @@
         <f>'Controleur CA'!F36</f>
         <v>Vérifier que la liste des champs de la couche ZNRO correspond aux spécifications QGIS</v>
       </c>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
+      <c r="D36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M36" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="37" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="19">
@@ -6255,16 +6715,36 @@
         <f>'Controleur CA'!F37</f>
         <v>Vérifier que la liste des champs de la couche NRO correspond aux spécifications QGIS</v>
       </c>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
+      <c r="D37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M37" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="19">
@@ -6278,13 +6758,27 @@
         <f>'Controleur CA'!F38</f>
         <v>Vérifier que le numéro d'appui dans la C7 est sous la forme insee_identifiant</v>
       </c>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
+      <c r="D38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="K38" s="4" t="s">
         <v>50</v>
       </c>
@@ -6307,16 +6801,36 @@
         <f>'Controleur CA'!F39</f>
         <v>Vérifier que toutes les couches sont présentes selon les spec_QGIS</v>
       </c>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
+      <c r="D39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M39" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="19">
@@ -6523,9 +7037,7 @@
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
       <c r="L48" s="4"/>
-      <c r="M48" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="M48" s="4"/>
     </row>
     <row r="49" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="19">
@@ -6720,8 +7232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M56"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:C56"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:M56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6926,16 +7438,36 @@
         <f>'Controleur CA'!F6</f>
         <v>vérifier que le couple (id, type) colonne C-D et E-F est cohérent avec la table point_technique</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
+      <c r="D6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
@@ -7766,16 +8298,36 @@
         <f>'Controleur CA'!F26</f>
         <v>Vérifier que la liste des champs de la couche point technique correspond aux spécifications QGIS</v>
       </c>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
+      <c r="D26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="27" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
@@ -7789,16 +8341,36 @@
         <f>'Controleur CA'!F27</f>
         <v>Vérifier que la liste des champs de la couche prises correspond aux spécifications QGIS</v>
       </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
+      <c r="D27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M27" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="19">
@@ -7812,16 +8384,36 @@
         <f>'Controleur CA'!F28</f>
         <v>Vérifier que la liste des champs de la couche SRO correspond aux spécifications QGIS</v>
       </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
+      <c r="D28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M28" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="29" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="19">
@@ -7835,16 +8427,36 @@
         <f>'Controleur CA'!F29</f>
         <v>Vérifier que la liste des champs de la couche boitiers correspond aux spécifications QGIS</v>
       </c>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
+      <c r="D29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M29" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="30" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="19">
@@ -7858,16 +8470,36 @@
         <f>'Controleur CA'!F30</f>
         <v>Vérifier que la liste des champs de la couche infrastructure correspond aux spécifications QGIS</v>
       </c>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
+      <c r="D30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M30" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="31" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="19">
@@ -7881,16 +8513,36 @@
         <f>'Controleur CA'!F31</f>
         <v>Vérifier que la liste des champs de la couche racco_client correspond aux spécifications QGIS</v>
       </c>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
+      <c r="D31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M31" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="32" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="19">
@@ -7904,16 +8556,36 @@
         <f>'Controleur CA'!F32</f>
         <v>Vérifier que la liste des champs de la couche cable correspond aux spécifications QGIS</v>
       </c>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
+      <c r="D32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M32" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="33" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="19">
@@ -7927,16 +8599,36 @@
         <f>'Controleur CA'!F33</f>
         <v>Vérifier que la liste des champs de la couche ZPBO correspond aux spécifications QGIS</v>
       </c>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
+      <c r="D33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M33" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="34" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="19">
@@ -7950,16 +8642,36 @@
         <f>'Controleur CA'!F34</f>
         <v>Vérifier que la liste des champs de la couche ZSRO correspond aux spécifications QGIS</v>
       </c>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
+      <c r="D34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M34" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="35" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="19">
@@ -7973,16 +8685,36 @@
         <f>'Controleur CA'!F35</f>
         <v>Vérifier que la liste des champs de la couche ZPEC correspond aux spécifications QGIS</v>
       </c>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
+      <c r="D35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M35" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="36" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="19">
@@ -7996,16 +8728,36 @@
         <f>'Controleur CA'!F36</f>
         <v>Vérifier que la liste des champs de la couche ZNRO correspond aux spécifications QGIS</v>
       </c>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
+      <c r="D36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M36" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="37" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="19">
@@ -8019,16 +8771,36 @@
         <f>'Controleur CA'!F37</f>
         <v>Vérifier que la liste des champs de la couche NRO correspond aux spécifications QGIS</v>
       </c>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
+      <c r="D37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M37" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="19">
@@ -8042,13 +8814,27 @@
         <f>'Controleur CA'!F38</f>
         <v>Vérifier que le numéro d'appui dans la C7 est sous la forme insee_identifiant</v>
       </c>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
+      <c r="D38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="K38" s="4" t="s">
         <v>50</v>
       </c>
@@ -8071,16 +8857,36 @@
         <f>'Controleur CA'!F39</f>
         <v>Vérifier que toutes les couches sont présentes selon les spec_QGIS</v>
       </c>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
+      <c r="D39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M39" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="19">
@@ -8287,9 +9093,7 @@
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
       <c r="L48" s="4"/>
-      <c r="M48" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="M48" s="4"/>
     </row>
     <row r="49" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="19">
@@ -8484,8 +9288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M56"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:C56"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:M56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8600,9 +9404,7 @@
         <f>'Controleur CA'!F3</f>
         <v>Parcourir la table cable_infra. Pour chaque objet de la table de type infra_orange, vérifier qu'il existe une correspondance dans la C3A</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -8625,9 +9427,7 @@
         <f>'Controleur CA'!F4</f>
         <v>Parcourir la C3A. Pour chaque ligne, vérifier qu'il existe une correspondance dans la table_infra</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -8696,15 +9496,33 @@
       <c r="D6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
@@ -9535,16 +10353,36 @@
         <f>'Controleur CA'!F26</f>
         <v>Vérifier que la liste des champs de la couche point technique correspond aux spécifications QGIS</v>
       </c>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
+      <c r="D26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="27" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
@@ -9558,16 +10396,36 @@
         <f>'Controleur CA'!F27</f>
         <v>Vérifier que la liste des champs de la couche prises correspond aux spécifications QGIS</v>
       </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
+      <c r="D27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M27" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="19">
@@ -9581,16 +10439,36 @@
         <f>'Controleur CA'!F28</f>
         <v>Vérifier que la liste des champs de la couche SRO correspond aux spécifications QGIS</v>
       </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
+      <c r="D28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M28" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="29" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="19">
@@ -9604,16 +10482,36 @@
         <f>'Controleur CA'!F29</f>
         <v>Vérifier que la liste des champs de la couche boitiers correspond aux spécifications QGIS</v>
       </c>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
+      <c r="D29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M29" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="30" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="19">
@@ -9627,16 +10525,36 @@
         <f>'Controleur CA'!F30</f>
         <v>Vérifier que la liste des champs de la couche infrastructure correspond aux spécifications QGIS</v>
       </c>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
+      <c r="D30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M30" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="31" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="19">
@@ -9650,16 +10568,36 @@
         <f>'Controleur CA'!F31</f>
         <v>Vérifier que la liste des champs de la couche racco_client correspond aux spécifications QGIS</v>
       </c>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
+      <c r="D31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M31" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="32" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="19">
@@ -9673,16 +10611,36 @@
         <f>'Controleur CA'!F32</f>
         <v>Vérifier que la liste des champs de la couche cable correspond aux spécifications QGIS</v>
       </c>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
+      <c r="D32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M32" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="33" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="19">
@@ -9696,16 +10654,36 @@
         <f>'Controleur CA'!F33</f>
         <v>Vérifier que la liste des champs de la couche ZPBO correspond aux spécifications QGIS</v>
       </c>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
+      <c r="D33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M33" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="34" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="19">
@@ -9719,16 +10697,36 @@
         <f>'Controleur CA'!F34</f>
         <v>Vérifier que la liste des champs de la couche ZSRO correspond aux spécifications QGIS</v>
       </c>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
+      <c r="D34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M34" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="35" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="19">
@@ -9742,16 +10740,36 @@
         <f>'Controleur CA'!F35</f>
         <v>Vérifier que la liste des champs de la couche ZPEC correspond aux spécifications QGIS</v>
       </c>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
+      <c r="D35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M35" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="36" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="19">
@@ -9765,16 +10783,36 @@
         <f>'Controleur CA'!F36</f>
         <v>Vérifier que la liste des champs de la couche ZNRO correspond aux spécifications QGIS</v>
       </c>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
+      <c r="D36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M36" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="37" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="19">
@@ -9788,16 +10826,36 @@
         <f>'Controleur CA'!F37</f>
         <v>Vérifier que la liste des champs de la couche NRO correspond aux spécifications QGIS</v>
       </c>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
+      <c r="D37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M37" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="19">
@@ -9811,13 +10869,27 @@
         <f>'Controleur CA'!F38</f>
         <v>Vérifier que le numéro d'appui dans la C7 est sous la forme insee_identifiant</v>
       </c>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
+      <c r="D38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="K38" s="4" t="s">
         <v>50</v>
       </c>
@@ -9840,16 +10912,36 @@
         <f>'Controleur CA'!F39</f>
         <v>Vérifier que toutes les couches sont présentes selon les spec_QGIS</v>
       </c>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
+      <c r="D39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M39" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="19">
@@ -10056,9 +11148,7 @@
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
       <c r="L48" s="4"/>
-      <c r="M48" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="M48" s="4"/>
     </row>
     <row r="49" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="19">
@@ -10253,8 +11343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M56"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10459,16 +11549,36 @@
         <f>'Controleur CA'!F6</f>
         <v>vérifier que le couple (id, type) colonne C-D et E-F est cohérent avec la table point_technique</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
+      <c r="D6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
@@ -11299,15 +12409,33 @@
         <f>'Controleur CA'!F26</f>
         <v>Vérifier que la liste des champs de la couche point technique correspond aux spécifications QGIS</v>
       </c>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
+      <c r="D26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="M26" s="4" t="s">
         <v>50</v>
       </c>
@@ -11324,15 +12452,33 @@
         <f>'Controleur CA'!F27</f>
         <v>Vérifier que la liste des champs de la couche prises correspond aux spécifications QGIS</v>
       </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
+      <c r="D27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L27" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="M27" s="4" t="s">
         <v>50</v>
       </c>
@@ -11349,15 +12495,33 @@
         <f>'Controleur CA'!F28</f>
         <v>Vérifier que la liste des champs de la couche SRO correspond aux spécifications QGIS</v>
       </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
+      <c r="D28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="M28" s="4" t="s">
         <v>50</v>
       </c>
@@ -11374,15 +12538,33 @@
         <f>'Controleur CA'!F29</f>
         <v>Vérifier que la liste des champs de la couche boitiers correspond aux spécifications QGIS</v>
       </c>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
+      <c r="D29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="M29" s="4" t="s">
         <v>50</v>
       </c>
@@ -11399,15 +12581,33 @@
         <f>'Controleur CA'!F30</f>
         <v>Vérifier que la liste des champs de la couche infrastructure correspond aux spécifications QGIS</v>
       </c>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
+      <c r="D30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L30" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="M30" s="4" t="s">
         <v>50</v>
       </c>
@@ -11424,15 +12624,33 @@
         <f>'Controleur CA'!F31</f>
         <v>Vérifier que la liste des champs de la couche racco_client correspond aux spécifications QGIS</v>
       </c>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
+      <c r="D31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L31" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="M31" s="4" t="s">
         <v>50</v>
       </c>
@@ -11449,15 +12667,33 @@
         <f>'Controleur CA'!F32</f>
         <v>Vérifier que la liste des champs de la couche cable correspond aux spécifications QGIS</v>
       </c>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
+      <c r="D32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L32" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="M32" s="4" t="s">
         <v>50</v>
       </c>
@@ -11474,15 +12710,33 @@
         <f>'Controleur CA'!F33</f>
         <v>Vérifier que la liste des champs de la couche ZPBO correspond aux spécifications QGIS</v>
       </c>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
+      <c r="D33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L33" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="M33" s="4" t="s">
         <v>50</v>
       </c>
@@ -11499,15 +12753,33 @@
         <f>'Controleur CA'!F34</f>
         <v>Vérifier que la liste des champs de la couche ZSRO correspond aux spécifications QGIS</v>
       </c>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
+      <c r="D34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L34" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="M34" s="4" t="s">
         <v>50</v>
       </c>
@@ -11524,15 +12796,33 @@
         <f>'Controleur CA'!F35</f>
         <v>Vérifier que la liste des champs de la couche ZPEC correspond aux spécifications QGIS</v>
       </c>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
+      <c r="D35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L35" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="M35" s="4" t="s">
         <v>50</v>
       </c>
@@ -11549,15 +12839,33 @@
         <f>'Controleur CA'!F36</f>
         <v>Vérifier que la liste des champs de la couche ZNRO correspond aux spécifications QGIS</v>
       </c>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
+      <c r="D36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K36" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L36" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="M36" s="4" t="s">
         <v>50</v>
       </c>
@@ -11574,15 +12882,33 @@
         <f>'Controleur CA'!F37</f>
         <v>Vérifier que la liste des champs de la couche NRO correspond aux spécifications QGIS</v>
       </c>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
+      <c r="D37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L37" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="M37" s="4" t="s">
         <v>50</v>
       </c>
@@ -11599,13 +12925,27 @@
         <f>'Controleur CA'!F38</f>
         <v>Vérifier que le numéro d'appui dans la C7 est sous la forme insee_identifiant</v>
       </c>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
+      <c r="D38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="K38" s="4" t="s">
         <v>50</v>
       </c>
@@ -11628,16 +12968,36 @@
         <f>'Controleur CA'!F39</f>
         <v>Vérifier que toutes les couches sont présentes selon les spec_QGIS</v>
       </c>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
+      <c r="D39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M39" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="19">
@@ -11844,9 +13204,7 @@
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
       <c r="L48" s="4"/>
-      <c r="M48" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="M48" s="4"/>
     </row>
     <row r="49" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="19">
@@ -12124,6 +13482,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document Microsoft Word" ma:contentTypeID="0x01010066910ADB61686C45A75A7A744D7D5C8E0022B63E0AEFBB2040BF2A3B1B4BE32EE5" ma:contentTypeVersion="4" ma:contentTypeDescription="Document Microsoft Word vierge." ma:contentTypeScope="" ma:versionID="0a4943d90c7214e3c95a70ccb3c8346b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c97f8e9-86c7-4e99-9925-cc9540b321fe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eeaa8661ba6ba22f90735bcd04aade41" ns2:_="">
     <xsd:import namespace="9c97f8e9-86c7-4e99-9925-cc9540b321fe"/>
@@ -12326,15 +13693,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -12350,6 +13708,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F02C15CB-09E5-4D58-8C63-77232C75BB18}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8B2112A-C178-4B00-8690-1CA741C188F5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12363,14 +13729,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F02C15CB-09E5-4D58-8C63-77232C75BB18}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
** Version 8 ** - Refonte de l'arborescence - Formater le chemin affiché du controle 39 - Correction d'un bug du controle 5 - Ajout des contrôles 52,53,54 - Optimisation de code
</commit_message>
<xml_diff>
--- a/Documentation/Controleur.xlsx
+++ b/Documentation/Controleur.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="315" windowWidth="6915" windowHeight="6540"/>
+    <workbookView xWindow="8370" yWindow="1320" windowWidth="6915" windowHeight="6540" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Controleur CA" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2360" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2375" uniqueCount="195">
   <si>
     <t>Famille</t>
   </si>
@@ -587,6 +587,27 @@
   </si>
   <si>
     <t>Le répertoire LAYERS ou le fichier .qgs est introuvable dans le répertoire PROJET_QGIS</t>
+  </si>
+  <si>
+    <t>Le fichier appui est manquant pour ce point technique</t>
+  </si>
+  <si>
+    <t>[nom appui]</t>
+  </si>
+  <si>
+    <t>[Point technique]</t>
+  </si>
+  <si>
+    <t>[Dossier appuis]</t>
+  </si>
+  <si>
+    <t>[Dossier chambres]</t>
+  </si>
+  <si>
+    <t>[nom chambre]</t>
+  </si>
+  <si>
+    <t>Le fichier chambre est manquant pour ce point technique</t>
   </si>
 </sst>
 </file>
@@ -1159,8 +1180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView topLeftCell="G46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J53" sqref="J53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2509,7 +2530,9 @@
       <c r="I39" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="J39" s="26"/>
+      <c r="J39" s="26" t="s">
+        <v>181</v>
+      </c>
       <c r="K39" s="18"/>
       <c r="L39" s="18"/>
       <c r="M39" s="18"/>
@@ -2939,7 +2962,9 @@
       <c r="I52" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="J52" s="26"/>
+      <c r="J52" s="26" t="s">
+        <v>181</v>
+      </c>
       <c r="K52" s="18"/>
       <c r="L52" s="18"/>
       <c r="M52" s="18"/>
@@ -2959,17 +2984,27 @@
       <c r="C53" s="26" t="s">
         <v>173</v>
       </c>
-      <c r="D53" s="26"/>
-      <c r="E53" s="26"/>
+      <c r="D53" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="E53" s="26" t="s">
+        <v>191</v>
+      </c>
       <c r="F53" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="G53" s="27"/>
-      <c r="H53" s="27"/>
+      <c r="G53" s="27" t="s">
+        <v>189</v>
+      </c>
+      <c r="H53" s="27" t="s">
+        <v>188</v>
+      </c>
       <c r="I53" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="J53" s="26"/>
+      <c r="J53" s="26" t="s">
+        <v>181</v>
+      </c>
       <c r="K53" s="18"/>
       <c r="L53" s="18"/>
       <c r="M53" s="18"/>
@@ -2989,17 +3024,27 @@
       <c r="C54" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="D54" s="26"/>
-      <c r="E54" s="26"/>
+      <c r="D54" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="E54" s="26" t="s">
+        <v>192</v>
+      </c>
       <c r="F54" s="27" t="s">
         <v>176</v>
       </c>
-      <c r="G54" s="27"/>
-      <c r="H54" s="27"/>
+      <c r="G54" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="H54" s="27" t="s">
+        <v>194</v>
+      </c>
       <c r="I54" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="J54" s="26"/>
+      <c r="J54" s="26" t="s">
+        <v>181</v>
+      </c>
       <c r="K54" s="18"/>
       <c r="L54" s="18"/>
       <c r="M54" s="18"/>
@@ -3120,8 +3165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M56"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M56" sqref="D2:M56"/>
+    <sheetView topLeftCell="D43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5072,9 +5117,11 @@
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
-      <c r="M52" s="4"/>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M52" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="19">
         <v>53</v>
       </c>
@@ -5095,7 +5142,9 @@
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
-      <c r="M53" s="4"/>
+      <c r="M53" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="19">
@@ -5118,7 +5167,9 @@
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
-      <c r="M54" s="4"/>
+      <c r="M54" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="55" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="19">
@@ -13399,8 +13450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C9:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13469,11 +13520,11 @@
       </c>
       <c r="E12" s="4">
         <f>IF(ISERROR(SUMPRODUCT(('Controleur CA'!J:J="fait")*('Controleur CA'!B:B=C12))),"Aucun",SUMPRODUCT(('Controleur CA'!J:J="fait")*('Controleur CA'!B:B=C12)))</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F12" s="28">
         <f>E12/D12*100</f>
-        <v>16.666666666666664</v>
+        <v>38.888888888888893</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mise à jour des XML d'exemple et modèle selon le nouveau format du XML livrables
</commit_message>
<xml_diff>
--- a/Documentation/Controleur.xlsx
+++ b/Documentation/Controleur.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="8370" yWindow="1320" windowWidth="6915" windowHeight="6540" activeTab="6"/>
+    <workbookView xWindow="8370" yWindow="1320" windowWidth="6915" windowHeight="6540"/>
   </bookViews>
   <sheets>
     <sheet name="Controleur CA" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2375" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2375" uniqueCount="197">
   <si>
     <t>Famille</t>
   </si>
@@ -608,6 +608,12 @@
   </si>
   <si>
     <t>Le fichier chambre est manquant pour ce point technique</t>
+  </si>
+  <si>
+    <t>[Dossier Comac]</t>
+  </si>
+  <si>
+    <t>Il existe des points techniques Enedis mais le dossier Enedic est vide</t>
   </si>
 </sst>
 </file>
@@ -1180,8 +1186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R58"/>
   <sheetViews>
-    <sheetView topLeftCell="G46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J53" sqref="J53"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2952,13 +2958,19 @@
       <c r="C52" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="D52" s="26"/>
-      <c r="E52" s="26"/>
+      <c r="D52" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="E52" s="26" t="s">
+        <v>195</v>
+      </c>
       <c r="F52" s="27" t="s">
         <v>172</v>
       </c>
       <c r="G52" s="27"/>
-      <c r="H52" s="27"/>
+      <c r="H52" s="27" t="s">
+        <v>196</v>
+      </c>
       <c r="I52" s="26" t="s">
         <v>36</v>
       </c>
@@ -3165,8 +3177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M56"/>
   <sheetViews>
-    <sheetView topLeftCell="D43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView topLeftCell="D31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B40" sqref="A40:XFD40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5117,9 +5129,7 @@
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
-      <c r="M52" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="M52" s="4"/>
     </row>
     <row r="53" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="19">
@@ -5142,9 +5152,7 @@
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
-      <c r="M53" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="M53" s="4"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="19">
@@ -5167,9 +5175,7 @@
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
-      <c r="M54" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="M54" s="4"/>
     </row>
     <row r="55" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="19">
@@ -7283,7 +7289,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="D2" sqref="D2:M56"/>
     </sheetView>
   </sheetViews>
@@ -11394,8 +11400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M56"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:M56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13450,8 +13456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C9:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13533,15 +13539,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document Microsoft Word" ma:contentTypeID="0x01010066910ADB61686C45A75A7A744D7D5C8E0022B63E0AEFBB2040BF2A3B1B4BE32EE5" ma:contentTypeVersion="4" ma:contentTypeDescription="Document Microsoft Word vierge." ma:contentTypeScope="" ma:versionID="0a4943d90c7214e3c95a70ccb3c8346b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c97f8e9-86c7-4e99-9925-cc9540b321fe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eeaa8661ba6ba22f90735bcd04aade41" ns2:_="">
     <xsd:import namespace="9c97f8e9-86c7-4e99-9925-cc9540b321fe"/>
@@ -13744,6 +13741,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -13759,14 +13765,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F02C15CB-09E5-4D58-8C63-77232C75BB18}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8B2112A-C178-4B00-8690-1CA741C188F5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13780,6 +13778,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F02C15CB-09E5-4D58-8C63-77232C75BB18}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
- Programme utilisant le XML de configuration pour les chemins selon les départements - Tableau contenant les variables de configuration afin de pouvoir les consulter facilement - Dossier livrable renommé en livrable - Nouvelle version de livrable XML et donc aussi de la DTD - Correction de bug du parseur XML et réorganisation en fonctions et dans une logique de module pour être exploitable - Retirer les "./" des chemins en affichage dans le rapport d'erreurs
</commit_message>
<xml_diff>
--- a/Documentation/Controleur.xlsx
+++ b/Documentation/Controleur.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="8370" yWindow="1320" windowWidth="6915" windowHeight="6540"/>
+    <workbookView xWindow="8370" yWindow="1320" windowWidth="6915" windowHeight="6540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Controleur CA" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2375" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2381" uniqueCount="197">
   <si>
     <t>Famille</t>
   </si>
@@ -1186,8 +1186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView topLeftCell="F16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3177,8 +3177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M56"/>
   <sheetViews>
-    <sheetView topLeftCell="D31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B40" sqref="A40:XFD40"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4853,7 +4853,9 @@
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
-      <c r="M40" s="4"/>
+      <c r="M40" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="41" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="19">
@@ -5014,7 +5016,9 @@
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
       <c r="L47" s="4"/>
-      <c r="M47" s="4"/>
+      <c r="M47" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="48" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="19">
@@ -5037,7 +5041,9 @@
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
       <c r="L48" s="4"/>
-      <c r="M48" s="4"/>
+      <c r="M48" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="49" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="19">
@@ -5129,7 +5135,9 @@
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
-      <c r="M52" s="4"/>
+      <c r="M52" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="53" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="19">
@@ -5152,7 +5160,9 @@
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
-      <c r="M53" s="4"/>
+      <c r="M53" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="19">
@@ -5175,7 +5185,9 @@
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
-      <c r="M54" s="4"/>
+      <c r="M54" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="55" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="19">
@@ -13457,7 +13469,7 @@
   <dimension ref="C9:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C9" sqref="C9:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13539,6 +13551,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document Microsoft Word" ma:contentTypeID="0x01010066910ADB61686C45A75A7A744D7D5C8E0022B63E0AEFBB2040BF2A3B1B4BE32EE5" ma:contentTypeVersion="4" ma:contentTypeDescription="Document Microsoft Word vierge." ma:contentTypeScope="" ma:versionID="0a4943d90c7214e3c95a70ccb3c8346b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c97f8e9-86c7-4e99-9925-cc9540b321fe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eeaa8661ba6ba22f90735bcd04aade41" ns2:_="">
     <xsd:import namespace="9c97f8e9-86c7-4e99-9925-cc9540b321fe"/>
@@ -13741,15 +13762,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -13765,6 +13777,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F02C15CB-09E5-4D58-8C63-77232C75BB18}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8B2112A-C178-4B00-8690-1CA741C188F5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13782,26 +13802,18 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F02C15CB-09E5-4D58-8C63-77232C75BB18}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFD779FF-B039-4DC7-8903-586F168B5B9F}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9c97f8e9-86c7-4e99-9925-cc9540b321fe"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="9c97f8e9-86c7-4e99-9925-cc9540b321fe"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
- Fichier variables de configuration complété avec les autres types de variables - Ajout d'un nouveau contrôle dans la liste Excel - Ajout d'un nouveau contrôle 57 dans le programme - chemin courant et chemin vers le livrable renseignés dans les configurations depuis le parseur XML - Chemin différent selon le département pour gérer les deux types de dossiers - Gestion des listes de formats par fichier (au lieu d'un unique format) - Dépendance totale au fichier de configuration XML - Généralisation de la gestion des formats
</commit_message>
<xml_diff>
--- a/Documentation/Controleur.xlsx
+++ b/Documentation/Controleur.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="8370" yWindow="1320" windowWidth="6915" windowHeight="6540" activeTab="1"/>
+    <workbookView xWindow="8370" yWindow="1320" windowWidth="6915" windowHeight="6540" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Controleur CA" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2381" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2395" uniqueCount="198">
   <si>
     <t>Famille</t>
   </si>
@@ -614,6 +614,9 @@
   </si>
   <si>
     <t>Il existe des points techniques Enedis mais le dossier Enedic est vide</t>
+  </si>
+  <si>
+    <t>Vérifier que le dossier poteaux ne contient que des fichiers dont le format est correct</t>
   </si>
 </sst>
 </file>
@@ -1186,8 +1189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R58"/>
   <sheetViews>
-    <sheetView topLeftCell="F16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3126,25 +3129,35 @@
       <c r="Q56" s="18"/>
       <c r="R56" s="18"/>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A57" s="18"/>
-      <c r="B57" s="18"/>
-      <c r="C57" s="18"/>
-      <c r="D57" s="18"/>
-      <c r="E57" s="18"/>
-      <c r="F57" s="24"/>
-      <c r="G57" s="24"/>
-      <c r="H57" s="24"/>
-      <c r="I57" s="18"/>
-      <c r="J57" s="18"/>
-      <c r="K57" s="18"/>
-      <c r="L57" s="18"/>
-      <c r="M57" s="18"/>
-      <c r="N57" s="18"/>
-      <c r="O57" s="18"/>
-      <c r="P57" s="18"/>
-      <c r="Q57" s="18"/>
-      <c r="R57" s="18"/>
+    <row r="57" spans="1:18" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A57" s="25">
+        <v>57</v>
+      </c>
+      <c r="B57" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" s="26"/>
+      <c r="F57" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="G57" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="H57" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="I57" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="J57" s="26" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="18"/>
@@ -3175,10 +3188,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M56"/>
+  <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M57" sqref="D2:M57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5235,6 +5248,29 @@
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
     </row>
+    <row r="57" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="19">
+        <v>57</v>
+      </c>
+      <c r="B57" s="16" t="str">
+        <f>'Controleur CA'!B57</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C57" s="6" t="str">
+        <f>'Controleur CA'!F57</f>
+        <v>Vérifier que le dossier poteaux ne contient que des fichiers dont le format est correct</v>
+      </c>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="4"/>
+      <c r="L57" s="4"/>
+      <c r="M57" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5243,10 +5279,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M56"/>
+  <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:M56"/>
+    <sheetView tabSelected="1" topLeftCell="F46" workbookViewId="0">
+      <selection activeCell="N68" sqref="N68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6922,7 +6958,9 @@
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
-      <c r="M40" s="4"/>
+      <c r="M40" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="41" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="19">
@@ -7083,7 +7121,9 @@
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
       <c r="L47" s="4"/>
-      <c r="M47" s="4"/>
+      <c r="M47" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="48" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="19">
@@ -7106,7 +7146,9 @@
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
       <c r="L48" s="4"/>
-      <c r="M48" s="4"/>
+      <c r="M48" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="49" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="19">
@@ -7198,7 +7240,9 @@
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
-      <c r="M52" s="4"/>
+      <c r="M52" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="19">
@@ -7221,7 +7265,9 @@
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
-      <c r="M53" s="4"/>
+      <c r="M53" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="19">
@@ -7244,7 +7290,9 @@
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
-      <c r="M54" s="4"/>
+      <c r="M54" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="55" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="19">
@@ -7292,6 +7340,29 @@
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
     </row>
+    <row r="57" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="19">
+        <v>57</v>
+      </c>
+      <c r="B57" s="16" t="str">
+        <f>'Controleur CA'!B57</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C57" s="6" t="str">
+        <f>'Controleur CA'!F57</f>
+        <v>Vérifier que le dossier poteaux ne contient que des fichiers dont le format est correct</v>
+      </c>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="4"/>
+      <c r="L57" s="4"/>
+      <c r="M57" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7299,10 +7370,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M56"/>
+  <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:M56"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57:M57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9348,6 +9419,29 @@
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
     </row>
+    <row r="57" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="19">
+        <v>57</v>
+      </c>
+      <c r="B57" s="16" t="str">
+        <f>'Controleur CA'!B57</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C57" s="6" t="str">
+        <f>'Controleur CA'!F57</f>
+        <v>Vérifier que le dossier poteaux ne contient que des fichiers dont le format est correct</v>
+      </c>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="4"/>
+      <c r="L57" s="4"/>
+      <c r="M57" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9355,10 +9449,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M56"/>
+  <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:M56"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57:M57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11403,6 +11497,29 @@
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
     </row>
+    <row r="57" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="19">
+        <v>57</v>
+      </c>
+      <c r="B57" s="16" t="str">
+        <f>'Controleur CA'!B57</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C57" s="6" t="str">
+        <f>'Controleur CA'!F57</f>
+        <v>Vérifier que le dossier poteaux ne contient que des fichiers dont le format est correct</v>
+      </c>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="4"/>
+      <c r="L57" s="4"/>
+      <c r="M57" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11410,10 +11527,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M56"/>
+  <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:M56"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57:M57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13459,6 +13576,29 @@
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
     </row>
+    <row r="57" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="19">
+        <v>57</v>
+      </c>
+      <c r="B57" s="16" t="str">
+        <f>'Controleur CA'!B57</f>
+        <v>commande d'accès</v>
+      </c>
+      <c r="C57" s="6" t="str">
+        <f>'Controleur CA'!F57</f>
+        <v>Vérifier que le dossier poteaux ne contient que des fichiers dont le format est correct</v>
+      </c>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="4"/>
+      <c r="L57" s="4"/>
+      <c r="M57" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13469,7 +13609,7 @@
   <dimension ref="C9:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:F12"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13500,11 +13640,11 @@
       </c>
       <c r="D10" s="4">
         <f>COUNTIF('Controleur CA'!B:B,Synthèse!C10)</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E10" s="4">
         <f>IF(ISERROR(SUMPRODUCT(('Controleur CA'!J:J="fait")*('Controleur CA'!B:B=C10))),"Aucun",SUMPRODUCT(('Controleur CA'!J:J="fait")*('Controleur CA'!B:B=C10)))</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F10" s="28">
         <f>E10/D10*100</f>
@@ -13551,15 +13691,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document Microsoft Word" ma:contentTypeID="0x01010066910ADB61686C45A75A7A744D7D5C8E0022B63E0AEFBB2040BF2A3B1B4BE32EE5" ma:contentTypeVersion="4" ma:contentTypeDescription="Document Microsoft Word vierge." ma:contentTypeScope="" ma:versionID="0a4943d90c7214e3c95a70ccb3c8346b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c97f8e9-86c7-4e99-9925-cc9540b321fe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eeaa8661ba6ba22f90735bcd04aade41" ns2:_="">
     <xsd:import namespace="9c97f8e9-86c7-4e99-9925-cc9540b321fe"/>
@@ -13762,6 +13893,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -13777,14 +13917,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F02C15CB-09E5-4D58-8C63-77232C75BB18}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8B2112A-C178-4B00-8690-1CA741C188F5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13798,6 +13930,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F02C15CB-09E5-4D58-8C63-77232C75BB18}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
*** Version 9 et correctif ***
- Correction des valeurs de l'XML de configuration
- Dans le parseur XML, dupliquer CDXX dans CD21 si ce n'est pas distribution et EXE
- Fonction de parsing inclus les paramètres de zone livrable et type livrable, et configure différemment selon si distrib EXE et autres
- Stockage dans la variable conf depuis le parseur du chemin courant "app_path" afin de faciliter le changement de definition des chemins lorsqu'on change de liste déroulante
- Gérer le cas où le controle 5 est séléctionné mais que les champs infra sont introuvables et renvoyer une exception gérée
- Ajout des contrôles 46,49,50,56
- Placement plus pratique du code dans definitions pour les étapes d'ajout d'un nouveau contrôle
- Lors du formatage de l'affichage de chemin dans le rapport, mettre la racine ("/") plutôt que vide
- Ajout de la fonction format_inline permettant d'afficher une liste de paramètres en ligne sous forme de chaine de caractère
</commit_message>
<xml_diff>
--- a/Documentation/Controleur.xlsx
+++ b/Documentation/Controleur.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="8370" yWindow="1320" windowWidth="6915" windowHeight="6540" activeTab="2"/>
+    <workbookView xWindow="8370" yWindow="1320" windowWidth="6915" windowHeight="6540"/>
   </bookViews>
   <sheets>
     <sheet name="Controleur CA" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2395" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2420" uniqueCount="208">
   <si>
     <t>Famille</t>
   </si>
@@ -617,6 +617,36 @@
   </si>
   <si>
     <t>Vérifier que le dossier poteaux ne contient que des fichiers dont le format est correct</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>[Dossier racine]</t>
+  </si>
+  <si>
+    <t>Le fichier de synthèse d'étude est introuvable</t>
+  </si>
+  <si>
+    <t>[Dossier Optique]</t>
+  </si>
+  <si>
+    <t>Le fichier synoptique cable est introuvable</t>
+  </si>
+  <si>
+    <t>Le fichier synoptique fibre est introuvable</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>1 contrôle de commande d'accès ajouté à la liste</t>
+  </si>
+  <si>
+    <t>[Dossier Financier]</t>
+  </si>
+  <si>
+    <t>Le fichier BPU est introuvable</t>
   </si>
 </sst>
 </file>
@@ -666,7 +696,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -793,11 +823,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -879,6 +946,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1189,8 +1268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R58"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="F46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2721,7 +2800,7 @@
       <c r="Q44" s="18"/>
       <c r="R44" s="18"/>
     </row>
-    <row r="45" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="26">
         <v>45</v>
       </c>
@@ -2751,7 +2830,7 @@
       <c r="Q45" s="18"/>
       <c r="R45" s="18"/>
     </row>
-    <row r="46" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="26">
         <v>46</v>
       </c>
@@ -2761,17 +2840,27 @@
       <c r="C46" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26"/>
+      <c r="D46" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="E46" s="26" t="s">
+        <v>45</v>
+      </c>
       <c r="F46" s="27" t="s">
         <v>160</v>
       </c>
-      <c r="G46" s="27"/>
-      <c r="H46" s="27"/>
+      <c r="G46" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="H46" s="27" t="s">
+        <v>207</v>
+      </c>
       <c r="I46" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="J46" s="26"/>
+      <c r="J46" s="26" t="s">
+        <v>181</v>
+      </c>
       <c r="K46" s="18"/>
       <c r="L46" s="18"/>
       <c r="M46" s="18"/>
@@ -2871,17 +2960,27 @@
       <c r="C49" s="26" t="s">
         <v>165</v>
       </c>
-      <c r="D49" s="26"/>
-      <c r="E49" s="26"/>
+      <c r="D49" s="26" t="s">
+        <v>201</v>
+      </c>
+      <c r="E49" s="26" t="s">
+        <v>45</v>
+      </c>
       <c r="F49" s="27" t="s">
         <v>167</v>
       </c>
-      <c r="G49" s="27"/>
-      <c r="H49" s="27"/>
+      <c r="G49" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="H49" s="27" t="s">
+        <v>202</v>
+      </c>
       <c r="I49" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="J49" s="26"/>
+      <c r="J49" s="26" t="s">
+        <v>181</v>
+      </c>
       <c r="K49" s="18"/>
       <c r="L49" s="18"/>
       <c r="M49" s="18"/>
@@ -2901,17 +3000,27 @@
       <c r="C50" s="26" t="s">
         <v>166</v>
       </c>
-      <c r="D50" s="26"/>
-      <c r="E50" s="26"/>
+      <c r="D50" s="26" t="s">
+        <v>201</v>
+      </c>
+      <c r="E50" s="26" t="s">
+        <v>45</v>
+      </c>
       <c r="F50" s="27" t="s">
         <v>168</v>
       </c>
-      <c r="G50" s="27"/>
-      <c r="H50" s="27"/>
+      <c r="G50" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="H50" s="27" t="s">
+        <v>203</v>
+      </c>
       <c r="I50" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="J50" s="26"/>
+      <c r="J50" s="26" t="s">
+        <v>181</v>
+      </c>
       <c r="K50" s="18"/>
       <c r="L50" s="18"/>
       <c r="M50" s="18"/>
@@ -2970,7 +3079,9 @@
       <c r="F52" s="27" t="s">
         <v>172</v>
       </c>
-      <c r="G52" s="27"/>
+      <c r="G52" s="26" t="s">
+        <v>45</v>
+      </c>
       <c r="H52" s="27" t="s">
         <v>196</v>
       </c>
@@ -3109,17 +3220,27 @@
       <c r="C56" s="26" t="s">
         <v>179</v>
       </c>
-      <c r="D56" s="26"/>
-      <c r="E56" s="26"/>
+      <c r="D56" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="E56" s="26" t="s">
+        <v>45</v>
+      </c>
       <c r="F56" s="27" t="s">
         <v>180</v>
       </c>
-      <c r="G56" s="27"/>
-      <c r="H56" s="27"/>
+      <c r="G56" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="H56" s="27" t="s">
+        <v>200</v>
+      </c>
       <c r="I56" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="J56" s="26"/>
+        <v>37</v>
+      </c>
+      <c r="J56" s="26" t="s">
+        <v>181</v>
+      </c>
       <c r="K56" s="18"/>
       <c r="L56" s="18"/>
       <c r="M56" s="18"/>
@@ -3142,7 +3263,9 @@
       <c r="D57" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="E57" s="26"/>
+      <c r="E57" s="26" t="s">
+        <v>45</v>
+      </c>
       <c r="F57" s="27" t="s">
         <v>197</v>
       </c>
@@ -3190,8 +3313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M57" sqref="D2:M57"/>
+    <sheetView topLeftCell="D37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M46" sqref="M46:M57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4866,9 +4989,7 @@
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
-      <c r="M40" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="M40" s="4"/>
     </row>
     <row r="41" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="19">
@@ -5006,7 +5127,9 @@
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
       <c r="L46" s="4"/>
-      <c r="M46" s="4"/>
+      <c r="M46" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="47" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="19">
@@ -5029,9 +5152,7 @@
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
       <c r="L47" s="4"/>
-      <c r="M47" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="M47" s="4"/>
     </row>
     <row r="48" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="19">
@@ -5054,9 +5175,7 @@
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
       <c r="L48" s="4"/>
-      <c r="M48" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="M48" s="4"/>
     </row>
     <row r="49" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="19">
@@ -5102,7 +5221,9 @@
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
       <c r="L50" s="4"/>
-      <c r="M50" s="4"/>
+      <c r="M50" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="51" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="19">
@@ -5173,9 +5294,7 @@
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
-      <c r="M53" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="M53" s="4"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="19">
@@ -5246,7 +5365,9 @@
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
       <c r="L56" s="4"/>
-      <c r="M56" s="4"/>
+      <c r="M56" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="57" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="19">
@@ -5269,7 +5390,9 @@
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
       <c r="L57" s="4"/>
-      <c r="M57" s="4"/>
+      <c r="M57" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5281,8 +5404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F46" workbookViewId="0">
-      <selection activeCell="N68" sqref="N68"/>
+    <sheetView topLeftCell="D37" workbookViewId="0">
+      <selection activeCell="N46" sqref="N46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6958,9 +7081,7 @@
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
-      <c r="M40" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="M40" s="4"/>
     </row>
     <row r="41" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="19">
@@ -7098,7 +7219,9 @@
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
       <c r="L46" s="4"/>
-      <c r="M46" s="4"/>
+      <c r="M46" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="47" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="19">
@@ -7121,9 +7244,7 @@
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
       <c r="L47" s="4"/>
-      <c r="M47" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="M47" s="4"/>
     </row>
     <row r="48" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="19">
@@ -7146,9 +7267,7 @@
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
       <c r="L48" s="4"/>
-      <c r="M48" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="M48" s="4"/>
     </row>
     <row r="49" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="19">
@@ -7194,7 +7313,9 @@
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
       <c r="L50" s="4"/>
-      <c r="M50" s="4"/>
+      <c r="M50" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="51" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="19">
@@ -7265,9 +7386,7 @@
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
-      <c r="M53" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="M53" s="4"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="19">
@@ -7338,7 +7457,9 @@
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
       <c r="L56" s="4"/>
-      <c r="M56" s="4"/>
+      <c r="M56" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="57" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="19">
@@ -7361,7 +7482,9 @@
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
       <c r="L57" s="4"/>
-      <c r="M57" s="4"/>
+      <c r="M57" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7372,8 +7495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57:M57"/>
+    <sheetView topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13606,10 +13729,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C9:F12"/>
+  <dimension ref="C9:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="C9" sqref="C9:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13638,11 +13761,11 @@
       <c r="C10" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="19">
         <f>COUNTIF('Controleur CA'!B:B,Synthèse!C10)</f>
         <v>26</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="19">
         <f>IF(ISERROR(SUMPRODUCT(('Controleur CA'!J:J="fait")*('Controleur CA'!B:B=C10))),"Aucun",SUMPRODUCT(('Controleur CA'!J:J="fait")*('Controleur CA'!B:B=C10)))</f>
         <v>26</v>
       </c>
@@ -13655,11 +13778,11 @@
       <c r="C11" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="19">
         <f>COUNTIF('Controleur CA'!B:B,Synthèse!C11)</f>
         <v>12</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="19">
         <f>IF(ISERROR(SUMPRODUCT(('Controleur CA'!J:J="fait")*('Controleur CA'!B:B=C11))),"Aucun",SUMPRODUCT(('Controleur CA'!J:J="fait")*('Controleur CA'!B:B=C11)))</f>
         <v>12</v>
       </c>
@@ -13672,20 +13795,50 @@
       <c r="C12" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="19">
         <f>COUNTIF('Controleur CA'!B:B,Synthèse!C12)</f>
         <v>18</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="19">
         <f>IF(ISERROR(SUMPRODUCT(('Controleur CA'!J:J="fait")*('Controleur CA'!B:B=C12))),"Aucun",SUMPRODUCT(('Controleur CA'!J:J="fait")*('Controleur CA'!B:B=C12)))</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F12" s="28">
         <f>E12/D12*100</f>
-        <v>38.888888888888893</v>
-      </c>
+        <v>61.111111111111114</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C13" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="D13" s="19">
+        <f>D10+D11+D12</f>
+        <v>56</v>
+      </c>
+      <c r="E13" s="19">
+        <f>E10+E11+E12</f>
+        <v>49</v>
+      </c>
+      <c r="F13" s="28">
+        <f>(F10+F11+F12)/3</f>
+        <v>87.037037037037024</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>205</v>
+      </c>
+      <c r="E15" s="33"/>
+      <c r="F15" s="34"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D15:F15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
- Correction des formats dans le XML et regénération du DTD - Adaptation du parseur xml aux nouveaux changements - Finition et correction du contrôle 55 - Ajout du nouveau contrôle de cable infra (2 et 3) par les jointures de couches
</commit_message>
<xml_diff>
--- a/Documentation/Controleur.xlsx
+++ b/Documentation/Controleur.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="8370" yWindow="1320" windowWidth="6915" windowHeight="6540"/>
+    <workbookView xWindow="8370" yWindow="1320" windowWidth="6915" windowHeight="6540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Controleur CA" sheetId="1" r:id="rId1"/>
@@ -19,11 +19,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Controleur CA'!$A$1:$I$24</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2388" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1857" uniqueCount="228">
   <si>
     <t>Famille</t>
   </si>
@@ -634,9 +635,6 @@
     <t>Note</t>
   </si>
   <si>
-    <t>1 contrôle de commande d'accès ajouté à la liste</t>
-  </si>
-  <si>
     <t>[Dossier Financier]</t>
   </si>
   <si>
@@ -685,9 +683,6 @@
     <t>Fiche chambre manquante</t>
   </si>
   <si>
-    <t>A faire 4</t>
-  </si>
-  <si>
     <t>DT manquants pour la commune</t>
   </si>
   <si>
@@ -701,6 +696,18 @@
   </si>
   <si>
     <t>Le fichier PMV aérien est manquant pour la commune</t>
+  </si>
+  <si>
+    <t>L'annexe est manquante pour cette élement</t>
+  </si>
+  <si>
+    <t>[Tronçon / Point technique]</t>
+  </si>
+  <si>
+    <t>[Dossier annexes D15]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Couche Point technique / Couche Infrastructure] </t>
   </si>
 </sst>
 </file>
@@ -1352,8 +1359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E55" sqref="A55:XFD55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1465,9 +1472,7 @@
       <c r="I3" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="28" t="s">
-        <v>180</v>
-      </c>
+      <c r="J3" s="28"/>
     </row>
     <row r="4" spans="1:10" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="30">
@@ -1497,11 +1502,9 @@
       <c r="I4" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="28" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="J4" s="28"/>
+    </row>
+    <row r="5" spans="1:10" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="30">
         <v>4</v>
       </c>
@@ -1597,7 +1600,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="16" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="30">
         <v>7</v>
       </c>
@@ -1885,7 +1888,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="17" spans="1:18" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="30">
         <v>17</v>
       </c>
@@ -1981,7 +1984,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="20" spans="1:18" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="30">
         <v>20</v>
       </c>
@@ -2635,7 +2638,7 @@
       <c r="Q37" s="16"/>
       <c r="R37" s="16"/>
     </row>
-    <row r="38" spans="1:18" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="30">
         <v>38</v>
       </c>
@@ -2775,10 +2778,10 @@
         <v>149</v>
       </c>
       <c r="G41" s="31" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H41" s="35" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="I41" s="28" t="s">
         <v>36</v>
@@ -2795,7 +2798,7 @@
       <c r="Q41" s="16"/>
       <c r="R41" s="16"/>
     </row>
-    <row r="42" spans="1:18" ht="90" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="28">
         <v>42</v>
       </c>
@@ -2806,10 +2809,10 @@
         <v>150</v>
       </c>
       <c r="D42" s="31" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E42" s="28" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F42" s="35" t="s">
         <v>151</v>
@@ -2818,7 +2821,7 @@
         <v>48</v>
       </c>
       <c r="H42" s="35" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I42" s="28" t="s">
         <v>36</v>
@@ -2849,16 +2852,16 @@
         <v>123</v>
       </c>
       <c r="E43" s="28" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F43" s="35" t="s">
         <v>152</v>
       </c>
       <c r="G43" s="31" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H43" s="35" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="I43" s="28" t="s">
         <v>36</v>
@@ -2886,19 +2889,19 @@
         <v>155</v>
       </c>
       <c r="D44" s="31" t="s">
+        <v>215</v>
+      </c>
+      <c r="E44" s="28" t="s">
         <v>216</v>
-      </c>
-      <c r="E44" s="28" t="s">
-        <v>217</v>
       </c>
       <c r="F44" s="35" t="s">
         <v>153</v>
       </c>
       <c r="G44" s="31" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H44" s="35" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I44" s="28" t="s">
         <v>36</v>
@@ -2926,7 +2929,7 @@
         <v>158</v>
       </c>
       <c r="D45" s="31" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E45" s="28" t="s">
         <v>45</v>
@@ -2938,7 +2941,7 @@
         <v>45</v>
       </c>
       <c r="H45" s="35" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I45" s="28" t="s">
         <v>36</v>
@@ -2966,7 +2969,7 @@
         <v>157</v>
       </c>
       <c r="D46" s="31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E46" s="28" t="s">
         <v>45</v>
@@ -2978,7 +2981,7 @@
         <v>45</v>
       </c>
       <c r="H46" s="35" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I46" s="28" t="s">
         <v>36</v>
@@ -2995,7 +2998,7 @@
       <c r="Q46" s="16"/>
       <c r="R46" s="16"/>
     </row>
-    <row r="47" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="28">
         <v>47</v>
       </c>
@@ -3035,7 +3038,7 @@
       <c r="Q47" s="16"/>
       <c r="R47" s="16"/>
     </row>
-    <row r="48" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="28">
         <v>48</v>
       </c>
@@ -3075,7 +3078,7 @@
       <c r="Q48" s="16"/>
       <c r="R48" s="16"/>
     </row>
-    <row r="49" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="28">
         <v>49</v>
       </c>
@@ -3115,7 +3118,7 @@
       <c r="Q49" s="16"/>
       <c r="R49" s="16"/>
     </row>
-    <row r="50" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="28">
         <v>50</v>
       </c>
@@ -3166,19 +3169,19 @@
         <v>169</v>
       </c>
       <c r="D51" s="31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E51" s="28" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F51" s="35" t="s">
         <v>168</v>
       </c>
       <c r="G51" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H51" s="35" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I51" s="28" t="s">
         <v>36</v>
@@ -3206,7 +3209,7 @@
         <v>170</v>
       </c>
       <c r="D52" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E52" s="28" t="s">
         <v>193</v>
@@ -3235,7 +3238,7 @@
       <c r="Q52" s="16"/>
       <c r="R52" s="16"/>
     </row>
-    <row r="53" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="28">
         <v>53</v>
       </c>
@@ -3246,7 +3249,7 @@
         <v>172</v>
       </c>
       <c r="D53" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E53" s="28" t="s">
         <v>189</v>
@@ -3275,7 +3278,7 @@
       <c r="Q53" s="16"/>
       <c r="R53" s="16"/>
     </row>
-    <row r="54" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="28">
         <v>54</v>
       </c>
@@ -3286,7 +3289,7 @@
         <v>174</v>
       </c>
       <c r="D54" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E54" s="28" t="s">
         <v>190</v>
@@ -3315,7 +3318,7 @@
       <c r="Q54" s="16"/>
       <c r="R54" s="16"/>
     </row>
-    <row r="55" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="28">
         <v>55</v>
       </c>
@@ -3325,19 +3328,25 @@
       <c r="C55" s="28" t="s">
         <v>176</v>
       </c>
-      <c r="D55" s="31"/>
-      <c r="E55" s="28"/>
+      <c r="D55" s="31" t="s">
+        <v>227</v>
+      </c>
+      <c r="E55" s="28" t="s">
+        <v>226</v>
+      </c>
       <c r="F55" s="35" t="s">
         <v>177</v>
       </c>
-      <c r="G55" s="31"/>
-      <c r="H55" s="35"/>
+      <c r="G55" s="31" t="s">
+        <v>225</v>
+      </c>
+      <c r="H55" s="35" t="s">
+        <v>224</v>
+      </c>
       <c r="I55" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="J55" s="28" t="s">
-        <v>220</v>
-      </c>
+      <c r="J55" s="28"/>
       <c r="K55" s="16"/>
       <c r="L55" s="16"/>
       <c r="M55" s="16"/>
@@ -3347,7 +3356,7 @@
       <c r="Q55" s="16"/>
       <c r="R55" s="16"/>
     </row>
-    <row r="56" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="28">
         <v>56</v>
       </c>
@@ -3398,7 +3407,7 @@
         <v>15</v>
       </c>
       <c r="D57" s="31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E57" s="28" t="s">
         <v>45</v>
@@ -3419,7 +3428,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="58" spans="1:18" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="30">
         <v>58</v>
       </c>
@@ -3436,13 +3445,13 @@
         <v>190</v>
       </c>
       <c r="F58" s="35" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G58" s="31" t="s">
         <v>61</v>
       </c>
       <c r="H58" s="35" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I58" s="28" t="s">
         <v>9</v>
@@ -3462,8 +3471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView topLeftCell="D25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M47" sqref="M47"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3544,7 +3553,9 @@
       <c r="F2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H2" s="2" t="s">
         <v>50</v>
       </c>
@@ -3560,7 +3571,9 @@
       <c r="L2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M2" s="2"/>
+      <c r="M2" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
@@ -3582,8 +3595,12 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
+      <c r="L3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
@@ -3605,8 +3622,12 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
+      <c r="L4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
@@ -3629,7 +3650,9 @@
       <c r="F5" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H5" s="2" t="s">
         <v>50</v>
       </c>
@@ -3645,7 +3668,9 @@
       <c r="L5" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M5" s="2"/>
+      <c r="M5" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
@@ -3659,31 +3684,15 @@
         <f>'Controleur CA'!F6</f>
         <v>vérifier que le couple (id, type) colonne C-D et E-F est cohérent avec la table point_technique</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
       <c r="M6" s="2"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -3707,7 +3716,9 @@
       <c r="F7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H7" s="2" t="s">
         <v>50</v>
       </c>
@@ -3723,7 +3734,9 @@
       <c r="L7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M7" s="2"/>
+      <c r="M7" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
@@ -3746,7 +3759,9 @@
       <c r="F8" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H8" s="2" t="s">
         <v>50</v>
       </c>
@@ -3762,7 +3777,9 @@
       <c r="L8" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M8" s="2"/>
+      <c r="M8" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -3785,7 +3802,9 @@
       <c r="F9" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H9" s="2" t="s">
         <v>50</v>
       </c>
@@ -3801,7 +3820,9 @@
       <c r="L9" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M9" s="2"/>
+      <c r="M9" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -3824,7 +3845,9 @@
       <c r="F10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H10" s="2" t="s">
         <v>50</v>
       </c>
@@ -3840,7 +3863,9 @@
       <c r="L10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M10" s="2"/>
+      <c r="M10" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
@@ -3863,7 +3888,9 @@
       <c r="F11" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H11" s="2" t="s">
         <v>50</v>
       </c>
@@ -3879,7 +3906,9 @@
       <c r="L11" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M11" s="2"/>
+      <c r="M11" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
@@ -3902,7 +3931,9 @@
       <c r="F12" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H12" s="2" t="s">
         <v>50</v>
       </c>
@@ -3918,7 +3949,9 @@
       <c r="L12" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M12" s="2"/>
+      <c r="M12" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -3941,7 +3974,9 @@
       <c r="F13" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G13" s="2"/>
+      <c r="G13" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H13" s="2" t="s">
         <v>50</v>
       </c>
@@ -3957,7 +3992,9 @@
       <c r="L13" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M13" s="2"/>
+      <c r="M13" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
@@ -3980,7 +4017,9 @@
       <c r="F14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G14" s="2"/>
+      <c r="G14" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H14" s="2" t="s">
         <v>50</v>
       </c>
@@ -3996,7 +4035,9 @@
       <c r="L14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M14" s="2"/>
+      <c r="M14" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -4019,7 +4060,9 @@
       <c r="F15" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G15" s="2"/>
+      <c r="G15" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H15" s="2" t="s">
         <v>50</v>
       </c>
@@ -4035,7 +4078,9 @@
       <c r="L15" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M15" s="2"/>
+      <c r="M15" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -4058,7 +4103,9 @@
       <c r="F16" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="2"/>
+      <c r="G16" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H16" s="2" t="s">
         <v>50</v>
       </c>
@@ -4074,7 +4121,9 @@
       <c r="L16" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M16" s="2"/>
+      <c r="M16" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
@@ -4097,7 +4146,9 @@
       <c r="F17" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G17" s="2"/>
+      <c r="G17" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H17" s="2" t="s">
         <v>50</v>
       </c>
@@ -4113,7 +4164,9 @@
       <c r="L17" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M17" s="2"/>
+      <c r="M17" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
@@ -4136,7 +4189,9 @@
       <c r="F18" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G18" s="2"/>
+      <c r="G18" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H18" s="2" t="s">
         <v>50</v>
       </c>
@@ -4152,7 +4207,9 @@
       <c r="L18" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M18" s="2"/>
+      <c r="M18" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
@@ -4175,7 +4232,9 @@
       <c r="F19" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G19" s="2"/>
+      <c r="G19" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H19" s="2" t="s">
         <v>50</v>
       </c>
@@ -4191,7 +4250,9 @@
       <c r="L19" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M19" s="2"/>
+      <c r="M19" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
@@ -4214,7 +4275,9 @@
       <c r="F20" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G20" s="2"/>
+      <c r="G20" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H20" s="2" t="s">
         <v>50</v>
       </c>
@@ -4230,7 +4293,9 @@
       <c r="L20" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M20" s="2"/>
+      <c r="M20" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
@@ -4253,7 +4318,9 @@
       <c r="F21" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G21" s="2"/>
+      <c r="G21" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H21" s="2" t="s">
         <v>50</v>
       </c>
@@ -4269,7 +4336,9 @@
       <c r="L21" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M21" s="2"/>
+      <c r="M21" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -4292,7 +4361,9 @@
       <c r="F22" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G22" s="2"/>
+      <c r="G22" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H22" s="2" t="s">
         <v>50</v>
       </c>
@@ -4308,7 +4379,9 @@
       <c r="L22" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M22" s="2"/>
+      <c r="M22" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
@@ -4331,7 +4404,9 @@
       <c r="F23" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G23" s="2"/>
+      <c r="G23" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H23" s="2" t="s">
         <v>50</v>
       </c>
@@ -4347,7 +4422,9 @@
       <c r="L23" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M23" s="2"/>
+      <c r="M23" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
@@ -4370,7 +4447,9 @@
       <c r="F24" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G24" s="2"/>
+      <c r="G24" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H24" s="2" t="s">
         <v>50</v>
       </c>
@@ -4386,7 +4465,9 @@
       <c r="L24" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M24" s="2"/>
+      <c r="M24" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
@@ -4409,7 +4490,9 @@
       <c r="F25" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G25" s="2"/>
+      <c r="G25" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H25" s="2" t="s">
         <v>50</v>
       </c>
@@ -4425,7 +4508,9 @@
       <c r="L25" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M25" s="2"/>
+      <c r="M25" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="26" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
@@ -4439,36 +4524,16 @@
         <f>'Controleur CA'!F26</f>
         <v>Vérifier que la liste des champs de la couche point technique correspond aux spécifications QGIS</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L26" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M26" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
     </row>
     <row r="27" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
@@ -4482,36 +4547,16 @@
         <f>'Controleur CA'!F27</f>
         <v>Vérifier que la liste des champs de la couche prises correspond aux spécifications QGIS</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M27" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="17">
@@ -4525,36 +4570,16 @@
         <f>'Controleur CA'!F28</f>
         <v>Vérifier que la liste des champs de la couche SRO correspond aux spécifications QGIS</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K28" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L28" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M28" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
     </row>
     <row r="29" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="17">
@@ -4568,36 +4593,16 @@
         <f>'Controleur CA'!F29</f>
         <v>Vérifier que la liste des champs de la couche boitiers correspond aux spécifications QGIS</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M29" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
     </row>
     <row r="30" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="17">
@@ -4611,36 +4616,16 @@
         <f>'Controleur CA'!F30</f>
         <v>Vérifier que la liste des champs de la couche infrastructure correspond aux spécifications QGIS</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L30" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M30" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
     </row>
     <row r="31" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="17">
@@ -4654,36 +4639,16 @@
         <f>'Controleur CA'!F31</f>
         <v>Vérifier que la liste des champs de la couche racco_client correspond aux spécifications QGIS</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L31" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M31" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
     </row>
     <row r="32" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="17">
@@ -4697,36 +4662,16 @@
         <f>'Controleur CA'!F32</f>
         <v>Vérifier que la liste des champs de la couche cable correspond aux spécifications QGIS</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K32" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L32" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M32" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
     </row>
     <row r="33" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
@@ -4740,36 +4685,16 @@
         <f>'Controleur CA'!F33</f>
         <v>Vérifier que la liste des champs de la couche ZPBO correspond aux spécifications QGIS</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L33" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M33" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
     </row>
     <row r="34" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="17">
@@ -4783,36 +4708,16 @@
         <f>'Controleur CA'!F34</f>
         <v>Vérifier que la liste des champs de la couche ZSRO correspond aux spécifications QGIS</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J34" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K34" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L34" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M34" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
     </row>
     <row r="35" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="17">
@@ -4826,36 +4731,16 @@
         <f>'Controleur CA'!F35</f>
         <v>Vérifier que la liste des champs de la couche ZPEC correspond aux spécifications QGIS</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K35" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L35" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M35" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
     </row>
     <row r="36" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="17">
@@ -4869,36 +4754,16 @@
         <f>'Controleur CA'!F36</f>
         <v>Vérifier que la liste des champs de la couche ZNRO correspond aux spécifications QGIS</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L36" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M36" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
     </row>
     <row r="37" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="17">
@@ -4912,36 +4777,16 @@
         <f>'Controleur CA'!F37</f>
         <v>Vérifier que la liste des champs de la couche NRO correspond aux spécifications QGIS</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L37" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M37" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="17">
@@ -4964,7 +4809,9 @@
       <c r="F38" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G38" s="2"/>
+      <c r="G38" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H38" s="2" t="s">
         <v>50</v>
       </c>
@@ -4980,7 +4827,9 @@
       <c r="L38" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M38" s="2"/>
+      <c r="M38" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="17">
@@ -4994,36 +4843,16 @@
         <f>'Controleur CA'!F39</f>
         <v>Vérifier que toutes les couches sont présentes selon les spec_QGIS</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K39" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L39" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M39" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="17">
@@ -5037,36 +4866,16 @@
         <f>'Controleur CA'!F40</f>
         <v>Vérifier que tous les attributs de chaque couches sont présents selon les spec_QGIS</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K40" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L40" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M40" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
     </row>
     <row r="41" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="17">
@@ -5080,36 +4889,16 @@
         <f>'Controleur CA'!F41</f>
         <v>Vérifier qu'il existe un répertoire au nom de la commune dans 01 - Administratif/1.1 - DT/ lorsque du GC est à faire sur la commune et qu'il est pas vide</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K41" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L41" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M41" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
     </row>
     <row r="42" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="17">
@@ -5123,36 +4912,16 @@
         <f>'Controleur CA'!F42</f>
         <v>Vérifier que s'il y a plus de 1000 m de GC le dossier L49 contient au moins un fichier dont le nom contient dossier et au moins un fichier dont le nom contient recepisse</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I42" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J42" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K42" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L42" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M42" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
     </row>
     <row r="43" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="17">
@@ -5166,36 +4935,16 @@
         <f>'Controleur CA'!F43</f>
         <v>Vérifier s'il exite un fichier nommé [Commune]_aérien s'il y a des poteaux dans la commune à changer ou renforcer</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K43" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L43" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M43" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
     </row>
     <row r="44" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="17">
@@ -5209,36 +4958,16 @@
         <f>'Controleur CA'!F44</f>
         <v>Vérifier s'il exite un fichier nommé [Commune]_conduite s'il y a du GC sur la commune</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I44" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J44" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K44" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L44" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M44" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
     </row>
     <row r="45" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="17">
@@ -5252,36 +4981,16 @@
         <f>'Controleur CA'!F45</f>
         <v>Vérifier que le dossier Conventions contient un fichier contenant "recap_convention"</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I45" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K45" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L45" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M45" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="17">
@@ -5295,36 +5004,16 @@
         <f>'Controleur CA'!F46</f>
         <v>Verifier que le dossier contient un seul fichier qui contient le nom BPU</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I46" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J46" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K46" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L46" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M46" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
     </row>
     <row r="47" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="17">
@@ -5338,36 +5027,16 @@
         <f>'Controleur CA'!F47</f>
         <v>Vérifier que le répertoire PROJET_QGIS contient un répertoire nommé LAYERS et un fichier avec l'extention .qgs</v>
       </c>
-      <c r="D47" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H47" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I47" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J47" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K47" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L47" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M47" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
     </row>
     <row r="48" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="17">
@@ -5381,36 +5050,16 @@
         <f>'Controleur CA'!F48</f>
         <v>Vérifier que le répertoire PROJET_QGIS contient un fichier contenant le nom Plan_tirage au format pdf</v>
       </c>
-      <c r="D48" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I48" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J48" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K48" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L48" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M48" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
     </row>
     <row r="49" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="17">
@@ -5424,36 +5073,16 @@
         <f>'Controleur CA'!F49</f>
         <v>Verifier que le dossier 06 - Dossier Optique contient un fichier contenant "synoptique_cable" au format excel</v>
       </c>
-      <c r="D49" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J49" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K49" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L49" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M49" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
     </row>
     <row r="50" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="17">
@@ -5467,36 +5096,16 @@
         <f>'Controleur CA'!F50</f>
         <v>Verifier que le dossier 06 - Dossier Optique contient un fichier contenant "synoptique_fibre" au format excel</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I50" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J50" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K50" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L50" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M50" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
     </row>
     <row r="51" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="17">
@@ -5510,36 +5119,16 @@
         <f>'Controleur CA'!F51</f>
         <v>Verifier qu'il existe un fichier pour chaque point de QGIS. Le fichier doit être nommé par le bp_etiquet</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I51" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J51" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K51" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L51" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M51" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
     </row>
     <row r="52" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="17">
@@ -5553,36 +5142,16 @@
         <f>'Controleur CA'!F52</f>
         <v>Vérifier que le répertoire n'est pas vide s'il y a des point technique dont Enedis est le propriétaire</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G52" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I52" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J52" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K52" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L52" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M52" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+      <c r="M52" s="2"/>
     </row>
     <row r="53" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="17">
@@ -5596,36 +5165,16 @@
         <f>'Controleur CA'!F53</f>
         <v>Vérifier qu'il existe un fichier par point technique de type Orange Appui</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I53" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J53" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K53" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L53" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M53" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+      <c r="L53" s="2"/>
+      <c r="M53" s="2"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="17">
@@ -5639,36 +5188,16 @@
         <f>'Controleur CA'!F54</f>
         <v>Vérifier qu'il exite un fichier par point technique de type chambre existante</v>
       </c>
-      <c r="D54" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H54" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I54" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J54" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K54" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L54" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M54" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
+      <c r="L54" s="2"/>
+      <c r="M54" s="2"/>
     </row>
     <row r="55" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="17">
@@ -5725,36 +5254,16 @@
         <f>'Controleur CA'!F56</f>
         <v>Vérifier qu'il existe un fichier contenant le nom sythese_etude à la racine du zip</v>
       </c>
-      <c r="D56" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I56" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J56" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K56" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L56" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M56" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="2"/>
+      <c r="L56" s="2"/>
+      <c r="M56" s="2"/>
     </row>
     <row r="57" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="17">
@@ -5777,7 +5286,9 @@
       <c r="F57" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G57" s="2"/>
+      <c r="G57" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H57" s="2" t="s">
         <v>50</v>
       </c>
@@ -5793,7 +5304,9 @@
       <c r="L57" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M57" s="2"/>
+      <c r="M57" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="17">
@@ -5816,7 +5329,9 @@
       <c r="F58" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G58" s="2"/>
+      <c r="G58" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H58" s="2" t="s">
         <v>50</v>
       </c>
@@ -5832,7 +5347,9 @@
       <c r="L58" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M58" s="2"/>
+      <c r="M58" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M59" s="26"/>
@@ -5847,8 +5364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M58"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M58" sqref="M2:M58"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:M58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5948,7 +5465,9 @@
       <c r="L2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M2" s="2"/>
+      <c r="M2" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
@@ -6035,7 +5554,9 @@
       <c r="L5" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M5" s="2"/>
+      <c r="M5" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
@@ -6049,33 +5570,15 @@
         <f>'Controleur CA'!F6</f>
         <v>vérifier que le couple (id, type) colonne C-D et E-F est cohérent avec la table point_technique</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
       <c r="M6" s="2"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -6117,7 +5620,9 @@
       <c r="L7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M7" s="2"/>
+      <c r="M7" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
@@ -6158,7 +5663,9 @@
       <c r="L8" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M8" s="2"/>
+      <c r="M8" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -6199,7 +5706,9 @@
       <c r="L9" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M9" s="2"/>
+      <c r="M9" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -6240,7 +5749,9 @@
       <c r="L10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M10" s="2"/>
+      <c r="M10" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
@@ -6281,7 +5792,9 @@
       <c r="L11" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M11" s="2"/>
+      <c r="M11" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
@@ -6322,7 +5835,9 @@
       <c r="L12" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M12" s="2"/>
+      <c r="M12" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -6363,7 +5878,9 @@
       <c r="L13" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M13" s="2"/>
+      <c r="M13" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
@@ -6404,7 +5921,9 @@
       <c r="L14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M14" s="2"/>
+      <c r="M14" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -6445,7 +5964,9 @@
       <c r="L15" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M15" s="2"/>
+      <c r="M15" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -6486,7 +6007,9 @@
       <c r="L16" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M16" s="2"/>
+      <c r="M16" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
@@ -6527,7 +6050,9 @@
       <c r="L17" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M17" s="2"/>
+      <c r="M17" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
@@ -6568,7 +6093,9 @@
       <c r="L18" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M18" s="2"/>
+      <c r="M18" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
@@ -6609,7 +6136,9 @@
       <c r="L19" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M19" s="2"/>
+      <c r="M19" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
@@ -6650,7 +6179,9 @@
       <c r="L20" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M20" s="2"/>
+      <c r="M20" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
@@ -6691,7 +6222,9 @@
       <c r="L21" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M21" s="2"/>
+      <c r="M21" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -6732,7 +6265,9 @@
       <c r="L22" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M22" s="2"/>
+      <c r="M22" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
@@ -6773,7 +6308,9 @@
       <c r="L23" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M23" s="2"/>
+      <c r="M23" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
@@ -6814,7 +6351,9 @@
       <c r="L24" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M24" s="2"/>
+      <c r="M24" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
@@ -6855,7 +6394,9 @@
       <c r="L25" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M25" s="2"/>
+      <c r="M25" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="26" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
@@ -6869,36 +6410,16 @@
         <f>'Controleur CA'!F26</f>
         <v>Vérifier que la liste des champs de la couche point technique correspond aux spécifications QGIS</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L26" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M26" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
     </row>
     <row r="27" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
@@ -6912,36 +6433,16 @@
         <f>'Controleur CA'!F27</f>
         <v>Vérifier que la liste des champs de la couche prises correspond aux spécifications QGIS</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M27" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="17">
@@ -6955,36 +6456,16 @@
         <f>'Controleur CA'!F28</f>
         <v>Vérifier que la liste des champs de la couche SRO correspond aux spécifications QGIS</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K28" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L28" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M28" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
     </row>
     <row r="29" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="17">
@@ -6998,36 +6479,16 @@
         <f>'Controleur CA'!F29</f>
         <v>Vérifier que la liste des champs de la couche boitiers correspond aux spécifications QGIS</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M29" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
     </row>
     <row r="30" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="17">
@@ -7041,36 +6502,16 @@
         <f>'Controleur CA'!F30</f>
         <v>Vérifier que la liste des champs de la couche infrastructure correspond aux spécifications QGIS</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L30" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M30" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
     </row>
     <row r="31" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="17">
@@ -7084,36 +6525,16 @@
         <f>'Controleur CA'!F31</f>
         <v>Vérifier que la liste des champs de la couche racco_client correspond aux spécifications QGIS</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L31" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M31" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
     </row>
     <row r="32" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="17">
@@ -7127,36 +6548,16 @@
         <f>'Controleur CA'!F32</f>
         <v>Vérifier que la liste des champs de la couche cable correspond aux spécifications QGIS</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K32" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L32" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M32" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
     </row>
     <row r="33" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
@@ -7170,36 +6571,16 @@
         <f>'Controleur CA'!F33</f>
         <v>Vérifier que la liste des champs de la couche ZPBO correspond aux spécifications QGIS</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L33" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M33" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
     </row>
     <row r="34" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="17">
@@ -7213,36 +6594,16 @@
         <f>'Controleur CA'!F34</f>
         <v>Vérifier que la liste des champs de la couche ZSRO correspond aux spécifications QGIS</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J34" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K34" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L34" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M34" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
     </row>
     <row r="35" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="17">
@@ -7256,36 +6617,16 @@
         <f>'Controleur CA'!F35</f>
         <v>Vérifier que la liste des champs de la couche ZPEC correspond aux spécifications QGIS</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K35" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L35" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M35" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
     </row>
     <row r="36" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="17">
@@ -7299,36 +6640,16 @@
         <f>'Controleur CA'!F36</f>
         <v>Vérifier que la liste des champs de la couche ZNRO correspond aux spécifications QGIS</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L36" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M36" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
     </row>
     <row r="37" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="17">
@@ -7342,36 +6663,16 @@
         <f>'Controleur CA'!F37</f>
         <v>Vérifier que la liste des champs de la couche NRO correspond aux spécifications QGIS</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L37" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M37" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="17">
@@ -7412,7 +6713,9 @@
       <c r="L38" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M38" s="2"/>
+      <c r="M38" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="17">
@@ -7426,36 +6729,16 @@
         <f>'Controleur CA'!F39</f>
         <v>Vérifier que toutes les couches sont présentes selon les spec_QGIS</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K39" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L39" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M39" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="17">
@@ -7469,36 +6752,16 @@
         <f>'Controleur CA'!F40</f>
         <v>Vérifier que tous les attributs de chaque couches sont présents selon les spec_QGIS</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K40" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L40" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M40" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
     </row>
     <row r="41" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="17">
@@ -7512,36 +6775,16 @@
         <f>'Controleur CA'!F41</f>
         <v>Vérifier qu'il existe un répertoire au nom de la commune dans 01 - Administratif/1.1 - DT/ lorsque du GC est à faire sur la commune et qu'il est pas vide</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K41" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L41" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M41" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
     </row>
     <row r="42" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="17">
@@ -7555,36 +6798,16 @@
         <f>'Controleur CA'!F42</f>
         <v>Vérifier que s'il y a plus de 1000 m de GC le dossier L49 contient au moins un fichier dont le nom contient dossier et au moins un fichier dont le nom contient recepisse</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I42" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J42" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K42" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L42" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M42" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
     </row>
     <row r="43" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="17">
@@ -7598,36 +6821,16 @@
         <f>'Controleur CA'!F43</f>
         <v>Vérifier s'il exite un fichier nommé [Commune]_aérien s'il y a des poteaux dans la commune à changer ou renforcer</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K43" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L43" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M43" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
     </row>
     <row r="44" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="17">
@@ -7641,36 +6844,16 @@
         <f>'Controleur CA'!F44</f>
         <v>Vérifier s'il exite un fichier nommé [Commune]_conduite s'il y a du GC sur la commune</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I44" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J44" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K44" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L44" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M44" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
     </row>
     <row r="45" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="17">
@@ -7684,36 +6867,16 @@
         <f>'Controleur CA'!F45</f>
         <v>Vérifier que le dossier Conventions contient un fichier contenant "recap_convention"</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I45" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K45" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L45" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M45" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="17">
@@ -7727,36 +6890,16 @@
         <f>'Controleur CA'!F46</f>
         <v>Verifier que le dossier contient un seul fichier qui contient le nom BPU</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I46" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J46" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K46" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L46" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M46" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
     </row>
     <row r="47" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="17">
@@ -7770,36 +6913,16 @@
         <f>'Controleur CA'!F47</f>
         <v>Vérifier que le répertoire PROJET_QGIS contient un répertoire nommé LAYERS et un fichier avec l'extention .qgs</v>
       </c>
-      <c r="D47" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H47" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I47" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J47" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K47" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L47" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M47" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
     </row>
     <row r="48" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="17">
@@ -7813,36 +6936,16 @@
         <f>'Controleur CA'!F48</f>
         <v>Vérifier que le répertoire PROJET_QGIS contient un fichier contenant le nom Plan_tirage au format pdf</v>
       </c>
-      <c r="D48" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I48" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J48" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K48" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L48" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M48" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
     </row>
     <row r="49" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="17">
@@ -7856,36 +6959,16 @@
         <f>'Controleur CA'!F49</f>
         <v>Verifier que le dossier 06 - Dossier Optique contient un fichier contenant "synoptique_cable" au format excel</v>
       </c>
-      <c r="D49" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J49" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K49" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L49" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M49" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
     </row>
     <row r="50" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="17">
@@ -7899,36 +6982,16 @@
         <f>'Controleur CA'!F50</f>
         <v>Verifier que le dossier 06 - Dossier Optique contient un fichier contenant "synoptique_fibre" au format excel</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I50" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J50" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K50" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L50" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M50" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
     </row>
     <row r="51" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="17">
@@ -7942,36 +7005,16 @@
         <f>'Controleur CA'!F51</f>
         <v>Verifier qu'il existe un fichier pour chaque point de QGIS. Le fichier doit être nommé par le bp_etiquet</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I51" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J51" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K51" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L51" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M51" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
     </row>
     <row r="52" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="17">
@@ -7985,36 +7028,16 @@
         <f>'Controleur CA'!F52</f>
         <v>Vérifier que le répertoire n'est pas vide s'il y a des point technique dont Enedis est le propriétaire</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G52" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I52" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J52" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K52" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L52" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M52" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+      <c r="M52" s="2"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="17">
@@ -8028,36 +7051,16 @@
         <f>'Controleur CA'!F53</f>
         <v>Vérifier qu'il existe un fichier par point technique de type Orange Appui</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I53" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J53" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K53" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L53" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M53" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+      <c r="L53" s="2"/>
+      <c r="M53" s="2"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="17">
@@ -8071,36 +7074,16 @@
         <f>'Controleur CA'!F54</f>
         <v>Vérifier qu'il exite un fichier par point technique de type chambre existante</v>
       </c>
-      <c r="D54" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H54" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I54" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J54" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K54" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L54" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M54" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
+      <c r="L54" s="2"/>
+      <c r="M54" s="2"/>
     </row>
     <row r="55" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="17">
@@ -8114,36 +7097,16 @@
         <f>'Controleur CA'!F55</f>
         <v>Vérifier qu'il existe un fichier par point technique problématique et un fichier par tronçon problématique</v>
       </c>
-      <c r="D55" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I55" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J55" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K55" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L55" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M55" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
+      <c r="L55" s="2"/>
+      <c r="M55" s="2"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="17">
@@ -8157,36 +7120,16 @@
         <f>'Controleur CA'!F56</f>
         <v>Vérifier qu'il existe un fichier contenant le nom sythese_etude à la racine du zip</v>
       </c>
-      <c r="D56" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I56" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J56" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K56" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L56" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M56" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="2"/>
+      <c r="L56" s="2"/>
+      <c r="M56" s="2"/>
     </row>
     <row r="57" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="17">
@@ -8227,7 +7170,9 @@
       <c r="L57" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M57" s="2"/>
+      <c r="M57" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="17">
@@ -8268,7 +7213,9 @@
       <c r="L58" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M58" s="2"/>
+      <c r="M58" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12002,7 +10949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D38" workbookViewId="0">
       <selection activeCell="D2" sqref="D2:M58"/>
     </sheetView>
   </sheetViews>
@@ -13865,7 +12812,7 @@
   <dimension ref="C9:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D9" sqref="D9:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13900,11 +12847,11 @@
       </c>
       <c r="E10" s="17">
         <f>IF(ISERROR(SUMPRODUCT(('Controleur CA'!J:J="fait")*('Controleur CA'!B:B=C10))),"Aucun",SUMPRODUCT(('Controleur CA'!J:J="fait")*('Controleur CA'!B:B=C10)))</f>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F10" s="21">
         <f>E10/D10*100</f>
-        <v>100</v>
+        <v>92.592592592592595</v>
       </c>
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.25">
@@ -13951,20 +12898,18 @@
       </c>
       <c r="E13" s="17">
         <f>E10+E11+E12</f>
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F13" s="21">
         <f>(F10+F11+F12)/3</f>
-        <v>98.148148148148152</v>
-      </c>
-    </row>
-    <row r="15" spans="3:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>95.679012345679027</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="25" t="s">
         <v>202</v>
       </c>
-      <c r="D15" s="38" t="s">
-        <v>203</v>
-      </c>
+      <c r="D15" s="38"/>
       <c r="E15" s="39"/>
       <c r="F15" s="40"/>
     </row>
@@ -13977,15 +12922,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document Microsoft Word" ma:contentTypeID="0x01010066910ADB61686C45A75A7A744D7D5C8E0022B63E0AEFBB2040BF2A3B1B4BE32EE5" ma:contentTypeVersion="4" ma:contentTypeDescription="Document Microsoft Word vierge." ma:contentTypeScope="" ma:versionID="0a4943d90c7214e3c95a70ccb3c8346b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c97f8e9-86c7-4e99-9925-cc9540b321fe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eeaa8661ba6ba22f90735bcd04aade41" ns2:_="">
     <xsd:import namespace="9c97f8e9-86c7-4e99-9925-cc9540b321fe"/>
@@ -14188,6 +13124,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -14203,14 +13148,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F02C15CB-09E5-4D58-8C63-77232C75BB18}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8B2112A-C178-4B00-8690-1CA741C188F5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14228,18 +13165,26 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F02C15CB-09E5-4D58-8C63-77232C75BB18}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFD779FF-B039-4DC7-8903-586F168B5B9F}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="9c97f8e9-86c7-4e99-9925-cc9540b321fe"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
- Dans contrôle 5, ne pas envoyer d'erreur si un point technique n'existe pas dans l'un ou l'autre côté, seulement les incohérences de type, ce qui est l'objet de ce contrôle. Les inclusions sont plutôt dans les contrôles 2 et 3 - Gérer les doublons de lignes (normaux) à la dernière étape donc écriture de fichier afin de centraliser le code - Pour contrôles 2 et 3, changement du champ utilisé pour le propriétaire, utilisant les spécifications, même si ce nouveau nom n'est pas dans les shapes de test
</commit_message>
<xml_diff>
--- a/Documentation/Controleur.xlsx
+++ b/Documentation/Controleur.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="8370" yWindow="1320" windowWidth="6915" windowHeight="6540" activeTab="1"/>
+    <workbookView xWindow="8370" yWindow="1320" windowWidth="6915" windowHeight="6540"/>
   </bookViews>
   <sheets>
     <sheet name="Controleur CA" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1857" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1897" uniqueCount="231">
   <si>
     <t>Famille</t>
   </si>
@@ -708,6 +708,15 @@
   </si>
   <si>
     <t xml:space="preserve">[Couche Point technique / Couche Infrastructure] </t>
+  </si>
+  <si>
+    <t>Vérifier que la colonne C et la colonne F contiennent un nom de point technique  respectant les normes Orange</t>
+  </si>
+  <si>
+    <t>Format de nommage du numéro de point technique incorrect</t>
+  </si>
+  <si>
+    <t>J'ai ajouté de nouveaux contrôles après étude des specifications Orange</t>
   </si>
 </sst>
 </file>
@@ -757,7 +766,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -921,22 +930,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1004,9 +1002,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1357,916 +1352,920 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R58"/>
+  <dimension ref="A1:R59"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E55" sqref="A55:XFD55"/>
+    <sheetView tabSelected="1" topLeftCell="F50" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G67" sqref="G67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" style="29" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" style="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" style="29" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" style="32" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.28515625" style="37" customWidth="1"/>
-    <col min="7" max="7" width="33.28515625" style="32" customWidth="1"/>
-    <col min="8" max="8" width="49.7109375" style="37" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" style="29" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" style="29" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" style="28" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" style="28" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="28" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" style="31" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.28515625" style="36" customWidth="1"/>
+    <col min="7" max="7" width="33.28515625" style="31" customWidth="1"/>
+    <col min="8" max="8" width="49.7109375" style="36" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" style="28" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" style="28" customWidth="1"/>
     <col min="11" max="12" width="35.140625" customWidth="1"/>
     <col min="13" max="13" width="23" customWidth="1"/>
     <col min="14" max="14" width="35.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="I1" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="J1" s="33" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="30">
+      <c r="A2" s="29">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="H2" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="27" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="16" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="30">
+      <c r="A3" s="29">
         <v>2</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="31" t="s">
+      <c r="G3" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="35" t="s">
+      <c r="H3" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="I3" s="28" t="s">
+      <c r="I3" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="28"/>
+      <c r="J3" s="27" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="4" spans="1:10" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="30">
+      <c r="A4" s="29">
         <v>3</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="F4" s="35" t="s">
+      <c r="F4" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="31" t="s">
+      <c r="G4" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="35" t="s">
+      <c r="H4" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="I4" s="28" t="s">
+      <c r="I4" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="28"/>
+      <c r="J4" s="27" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="5" spans="1:10" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="30">
+      <c r="A5" s="29">
         <v>4</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="31" t="s">
+      <c r="G5" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="H5" s="35" t="s">
+      <c r="H5" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="I5" s="28" t="s">
+      <c r="I5" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="28" t="s">
+      <c r="J5" s="27" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="30">
+      <c r="A6" s="29">
         <v>5</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="31" t="s">
-        <v>122</v>
-      </c>
-      <c r="E6" s="28" t="s">
+      <c r="D6" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="E6" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="F6" s="35" t="s">
+      <c r="F6" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="31" t="s">
+      <c r="G6" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="H6" s="35" t="s">
+      <c r="H6" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="I6" s="28" t="s">
+      <c r="I6" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J6" s="28" t="s">
+      <c r="J6" s="27" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="30">
+      <c r="A7" s="29">
         <v>6</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="31" t="s">
+      <c r="D7" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="F7" s="35" t="s">
+      <c r="F7" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="31" t="s">
+      <c r="G7" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="H7" s="35" t="s">
+      <c r="H7" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="I7" s="28" t="s">
+      <c r="I7" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="28" t="s">
+      <c r="J7" s="27" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="30">
+      <c r="A8" s="29">
         <v>7</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="F8" s="35" t="s">
+      <c r="F8" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="31" t="s">
+      <c r="G8" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="35" t="s">
+      <c r="H8" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="I8" s="28" t="s">
+      <c r="I8" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J8" s="28" t="s">
+      <c r="J8" s="27" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="30">
+      <c r="A9" s="29">
         <v>8</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="F9" s="35" t="s">
+      <c r="F9" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="31" t="s">
+      <c r="G9" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="H9" s="35" t="s">
+      <c r="H9" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="I9" s="28" t="s">
+      <c r="I9" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="28" t="s">
+      <c r="J9" s="27" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="30">
+      <c r="A10" s="29">
         <v>9</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="31" t="s">
+      <c r="D10" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="35" t="s">
+      <c r="F10" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="31" t="s">
+      <c r="G10" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="H10" s="35" t="s">
+      <c r="H10" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="I10" s="28" t="s">
+      <c r="I10" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="J10" s="28" t="s">
+      <c r="J10" s="27" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="16" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A11" s="30">
+      <c r="A11" s="29">
         <v>10</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="F11" s="35" t="s">
+      <c r="F11" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="31" t="s">
+      <c r="G11" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="H11" s="35" t="s">
+      <c r="H11" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="I11" s="28" t="s">
+      <c r="I11" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J11" s="28" t="s">
+      <c r="J11" s="27" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="16" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A12" s="30">
+      <c r="A12" s="29">
         <v>11</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="28" t="s">
+      <c r="E12" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="35" t="s">
+      <c r="F12" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="31" t="s">
+      <c r="G12" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="H12" s="35" t="s">
+      <c r="H12" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="I12" s="28" t="s">
+      <c r="I12" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J12" s="28" t="s">
+      <c r="J12" s="27" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="16" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="30">
+      <c r="A13" s="29">
         <v>12</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="28" t="s">
+      <c r="E13" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="F13" s="35" t="s">
+      <c r="F13" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="31" t="s">
+      <c r="G13" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="H13" s="35" t="s">
+      <c r="H13" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="I13" s="28" t="s">
+      <c r="I13" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J13" s="28" t="s">
+      <c r="J13" s="27" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="16" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A14" s="30">
+      <c r="A14" s="29">
         <v>13</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="28" t="s">
+      <c r="E14" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="F14" s="35" t="s">
+      <c r="F14" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="31" t="s">
+      <c r="G14" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="H14" s="35" t="s">
+      <c r="H14" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="I14" s="28" t="s">
+      <c r="I14" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="J14" s="28" t="s">
+      <c r="J14" s="27" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="30">
+      <c r="A15" s="29">
         <v>15</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="28" t="s">
+      <c r="E15" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="F15" s="35" t="s">
+      <c r="F15" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="31" t="s">
+      <c r="G15" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="H15" s="35" t="s">
+      <c r="H15" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="I15" s="28" t="s">
+      <c r="I15" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="J15" s="28" t="s">
+      <c r="J15" s="27" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="30">
+      <c r="A16" s="29">
         <v>16</v>
       </c>
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="28" t="s">
+      <c r="E16" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="F16" s="35" t="s">
+      <c r="F16" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="G16" s="31" t="s">
+      <c r="G16" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="I16" s="28" t="s">
+      <c r="I16" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="J16" s="28" t="s">
+      <c r="J16" s="27" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="17" spans="1:18" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="30">
+      <c r="A17" s="29">
         <v>17</v>
       </c>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="28" t="s">
+      <c r="E17" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="F17" s="35" t="s">
+      <c r="F17" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="G17" s="31" t="s">
+      <c r="G17" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="H17" s="35" t="s">
+      <c r="H17" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="I17" s="28" t="s">
+      <c r="I17" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="J17" s="28" t="s">
+      <c r="J17" s="27" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:18" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="30">
+      <c r="A18" s="29">
         <v>18</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="31" t="s">
+      <c r="D18" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="28" t="s">
+      <c r="E18" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="F18" s="35" t="s">
+      <c r="F18" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="G18" s="31" t="s">
+      <c r="G18" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="H18" s="35" t="s">
+      <c r="H18" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="I18" s="28" t="s">
+      <c r="I18" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="J18" s="28" t="s">
+      <c r="J18" s="27" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="19" spans="1:18" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="30">
+      <c r="A19" s="29">
         <v>19</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="31" t="s">
+      <c r="D19" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="28" t="s">
+      <c r="E19" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="F19" s="35" t="s">
+      <c r="F19" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="G19" s="31" t="s">
+      <c r="G19" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="H19" s="36" t="s">
+      <c r="H19" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="I19" s="28" t="s">
+      <c r="I19" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="J19" s="28" t="s">
+      <c r="J19" s="27" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="20" spans="1:18" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="30">
+      <c r="A20" s="29">
         <v>20</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="28" t="s">
+      <c r="C20" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="31" t="s">
+      <c r="D20" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="28" t="s">
+      <c r="E20" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="F20" s="35" t="s">
+      <c r="F20" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="G20" s="31" t="s">
+      <c r="G20" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="H20" s="35" t="s">
+      <c r="H20" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="I20" s="28" t="s">
+      <c r="I20" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="J20" s="28" t="s">
+      <c r="J20" s="27" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:18" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="30">
+      <c r="A21" s="29">
         <v>21</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="31" t="s">
+      <c r="D21" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="28" t="s">
+      <c r="E21" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="F21" s="35" t="s">
+      <c r="F21" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="G21" s="31" t="s">
+      <c r="G21" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="H21" s="35" t="s">
+      <c r="H21" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="I21" s="28" t="s">
+      <c r="I21" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="J21" s="28" t="s">
+      <c r="J21" s="27" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="22" spans="1:18" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="30">
+      <c r="A22" s="29">
         <v>22</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="31" t="s">
+      <c r="D22" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="E22" s="28" t="s">
+      <c r="E22" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="F22" s="35" t="s">
+      <c r="F22" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="G22" s="31" t="s">
+      <c r="G22" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="H22" s="35" t="s">
+      <c r="H22" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="I22" s="28" t="s">
+      <c r="I22" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="J22" s="28" t="s">
+      <c r="J22" s="27" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="23" spans="1:18" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="30">
+      <c r="A23" s="29">
         <v>23</v>
       </c>
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="28" t="s">
+      <c r="C23" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="31" t="s">
+      <c r="D23" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="E23" s="28" t="s">
+      <c r="E23" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="35" t="s">
+      <c r="F23" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="G23" s="31" t="s">
+      <c r="G23" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="H23" s="35" t="s">
+      <c r="H23" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="I23" s="28" t="s">
+      <c r="I23" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="J23" s="28" t="s">
+      <c r="J23" s="27" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="24" spans="1:18" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="30">
+      <c r="A24" s="29">
         <v>24</v>
       </c>
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="28" t="s">
+      <c r="C24" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="31" t="s">
+      <c r="D24" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="E24" s="28" t="s">
+      <c r="E24" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="F24" s="35" t="s">
+      <c r="F24" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="G24" s="31" t="s">
+      <c r="G24" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="H24" s="35" t="s">
+      <c r="H24" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="I24" s="28" t="s">
+      <c r="I24" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="J24" s="28" t="s">
+      <c r="J24" s="27" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="25" spans="1:18" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="30">
+      <c r="A25" s="29">
         <v>25</v>
       </c>
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="28" t="s">
+      <c r="C25" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="31" t="s">
+      <c r="D25" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="28"/>
-      <c r="F25" s="35" t="s">
+      <c r="E25" s="27"/>
+      <c r="F25" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="G25" s="31" t="s">
+      <c r="G25" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="H25" s="35" t="s">
+      <c r="H25" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="I25" s="28" t="s">
+      <c r="I25" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="J25" s="28" t="s">
+      <c r="J25" s="27" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="26" spans="1:18" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="30">
+      <c r="A26" s="29">
         <v>26</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="C26" s="28" t="s">
+      <c r="C26" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="D26" s="31" t="s">
+      <c r="D26" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="E26" s="28" t="s">
+      <c r="E26" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="F26" s="35" t="s">
+      <c r="F26" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="G26" s="31" t="s">
+      <c r="G26" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="H26" s="35" t="s">
+      <c r="H26" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="I26" s="28" t="s">
+      <c r="I26" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J26" s="28" t="s">
+      <c r="J26" s="27" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="27" spans="1:18" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="30">
+      <c r="A27" s="29">
         <v>27</v>
       </c>
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="C27" s="28" t="s">
+      <c r="C27" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="D27" s="31" t="s">
+      <c r="D27" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="E27" s="28" t="s">
+      <c r="E27" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="F27" s="35" t="s">
+      <c r="F27" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="G27" s="31" t="s">
+      <c r="G27" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="H27" s="35" t="s">
+      <c r="H27" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="I27" s="28" t="s">
+      <c r="I27" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J27" s="28" t="s">
+      <c r="J27" s="27" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="30">
+      <c r="A28" s="29">
         <v>28</v>
       </c>
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="C28" s="28" t="s">
+      <c r="C28" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="D28" s="31" t="s">
+      <c r="D28" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="E28" s="28" t="s">
+      <c r="E28" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="F28" s="35" t="s">
+      <c r="F28" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="G28" s="31" t="s">
+      <c r="G28" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="H28" s="35" t="s">
+      <c r="H28" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="I28" s="28" t="s">
+      <c r="I28" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J28" s="28" t="s">
+      <c r="J28" s="27" t="s">
         <v>180</v>
       </c>
       <c r="K28" s="16"/>
@@ -2279,34 +2278,34 @@
       <c r="R28" s="16"/>
     </row>
     <row r="29" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="30">
+      <c r="A29" s="29">
         <v>29</v>
       </c>
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="C29" s="28" t="s">
+      <c r="C29" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="D29" s="31" t="s">
+      <c r="D29" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="E29" s="28" t="s">
+      <c r="E29" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="F29" s="35" t="s">
+      <c r="F29" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="G29" s="31" t="s">
+      <c r="G29" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="H29" s="35" t="s">
+      <c r="H29" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="I29" s="28" t="s">
+      <c r="I29" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J29" s="28" t="s">
+      <c r="J29" s="27" t="s">
         <v>180</v>
       </c>
       <c r="K29" s="16"/>
@@ -2319,34 +2318,34 @@
       <c r="R29" s="16"/>
     </row>
     <row r="30" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="30">
+      <c r="A30" s="29">
         <v>30</v>
       </c>
-      <c r="B30" s="28" t="s">
+      <c r="B30" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="C30" s="28" t="s">
+      <c r="C30" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="D30" s="31" t="s">
+      <c r="D30" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="E30" s="28" t="s">
+      <c r="E30" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="F30" s="35" t="s">
+      <c r="F30" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="G30" s="31" t="s">
+      <c r="G30" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="H30" s="35" t="s">
+      <c r="H30" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="I30" s="28" t="s">
+      <c r="I30" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J30" s="28" t="s">
+      <c r="J30" s="27" t="s">
         <v>180</v>
       </c>
       <c r="K30" s="16"/>
@@ -2359,34 +2358,34 @@
       <c r="R30" s="16"/>
     </row>
     <row r="31" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="30">
+      <c r="A31" s="29">
         <v>31</v>
       </c>
-      <c r="B31" s="28" t="s">
+      <c r="B31" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="C31" s="28" t="s">
+      <c r="C31" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="D31" s="31" t="s">
+      <c r="D31" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="F31" s="35" t="s">
+      <c r="F31" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="G31" s="31" t="s">
+      <c r="G31" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="H31" s="35" t="s">
+      <c r="H31" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="I31" s="28" t="s">
+      <c r="I31" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J31" s="28" t="s">
+      <c r="J31" s="27" t="s">
         <v>180</v>
       </c>
       <c r="K31" s="16"/>
@@ -2399,34 +2398,34 @@
       <c r="R31" s="16"/>
     </row>
     <row r="32" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="30">
+      <c r="A32" s="29">
         <v>32</v>
       </c>
-      <c r="B32" s="28" t="s">
+      <c r="B32" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="C32" s="28" t="s">
+      <c r="C32" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="D32" s="31" t="s">
+      <c r="D32" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="E32" s="28" t="s">
+      <c r="E32" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="F32" s="35" t="s">
+      <c r="F32" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="G32" s="31" t="s">
+      <c r="G32" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="H32" s="35" t="s">
+      <c r="H32" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="I32" s="28" t="s">
+      <c r="I32" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J32" s="28" t="s">
+      <c r="J32" s="27" t="s">
         <v>180</v>
       </c>
       <c r="K32" s="16"/>
@@ -2439,34 +2438,34 @@
       <c r="R32" s="16"/>
     </row>
     <row r="33" spans="1:18" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="30">
+      <c r="A33" s="29">
         <v>33</v>
       </c>
-      <c r="B33" s="28" t="s">
+      <c r="B33" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="C33" s="28" t="s">
+      <c r="C33" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="D33" s="31" t="s">
+      <c r="D33" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="E33" s="28" t="s">
+      <c r="E33" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="F33" s="35" t="s">
+      <c r="F33" s="34" t="s">
         <v>116</v>
       </c>
-      <c r="G33" s="31" t="s">
+      <c r="G33" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="H33" s="35" t="s">
+      <c r="H33" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="I33" s="28" t="s">
+      <c r="I33" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J33" s="28" t="s">
+      <c r="J33" s="27" t="s">
         <v>180</v>
       </c>
       <c r="K33" s="16"/>
@@ -2479,34 +2478,34 @@
       <c r="R33" s="16"/>
     </row>
     <row r="34" spans="1:18" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="30">
+      <c r="A34" s="29">
         <v>34</v>
       </c>
-      <c r="B34" s="28" t="s">
+      <c r="B34" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="C34" s="28" t="s">
+      <c r="C34" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="D34" s="31" t="s">
+      <c r="D34" s="30" t="s">
         <v>131</v>
       </c>
-      <c r="E34" s="28" t="s">
+      <c r="E34" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="F34" s="35" t="s">
+      <c r="F34" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="G34" s="31" t="s">
+      <c r="G34" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="H34" s="35" t="s">
+      <c r="H34" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="I34" s="28" t="s">
+      <c r="I34" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J34" s="28" t="s">
+      <c r="J34" s="27" t="s">
         <v>180</v>
       </c>
       <c r="K34" s="16"/>
@@ -2519,34 +2518,34 @@
       <c r="R34" s="16"/>
     </row>
     <row r="35" spans="1:18" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="30">
+      <c r="A35" s="29">
         <v>35</v>
       </c>
-      <c r="B35" s="28" t="s">
+      <c r="B35" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="C35" s="28" t="s">
+      <c r="C35" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="D35" s="31" t="s">
+      <c r="D35" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="E35" s="28" t="s">
+      <c r="E35" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="F35" s="35" t="s">
+      <c r="F35" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="G35" s="31" t="s">
+      <c r="G35" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="H35" s="35" t="s">
+      <c r="H35" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="I35" s="28" t="s">
+      <c r="I35" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J35" s="28" t="s">
+      <c r="J35" s="27" t="s">
         <v>180</v>
       </c>
       <c r="K35" s="16"/>
@@ -2559,34 +2558,34 @@
       <c r="R35" s="16"/>
     </row>
     <row r="36" spans="1:18" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="30">
+      <c r="A36" s="29">
         <v>36</v>
       </c>
-      <c r="B36" s="28" t="s">
+      <c r="B36" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="C36" s="28" t="s">
+      <c r="C36" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="D36" s="31" t="s">
+      <c r="D36" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="E36" s="28" t="s">
+      <c r="E36" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="F36" s="35" t="s">
+      <c r="F36" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="G36" s="31" t="s">
+      <c r="G36" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="H36" s="35" t="s">
+      <c r="H36" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="I36" s="28" t="s">
+      <c r="I36" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J36" s="28" t="s">
+      <c r="J36" s="27" t="s">
         <v>180</v>
       </c>
       <c r="K36" s="16"/>
@@ -2599,34 +2598,34 @@
       <c r="R36" s="16"/>
     </row>
     <row r="37" spans="1:18" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="30">
+      <c r="A37" s="29">
         <v>37</v>
       </c>
-      <c r="B37" s="28" t="s">
+      <c r="B37" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="C37" s="28" t="s">
+      <c r="C37" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="D37" s="31" t="s">
+      <c r="D37" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="E37" s="28" t="s">
+      <c r="E37" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="F37" s="35" t="s">
+      <c r="F37" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="G37" s="31" t="s">
+      <c r="G37" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="H37" s="35" t="s">
+      <c r="H37" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="I37" s="28" t="s">
+      <c r="I37" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J37" s="28" t="s">
+      <c r="J37" s="27" t="s">
         <v>180</v>
       </c>
       <c r="K37" s="16"/>
@@ -2639,34 +2638,34 @@
       <c r="R37" s="16"/>
     </row>
     <row r="38" spans="1:18" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="30">
+      <c r="A38" s="29">
         <v>38</v>
       </c>
-      <c r="B38" s="28" t="s">
+      <c r="B38" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C38" s="28" t="s">
+      <c r="C38" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D38" s="31" t="s">
+      <c r="D38" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="E38" s="31" t="s">
+      <c r="E38" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="F38" s="35" t="s">
+      <c r="F38" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="G38" s="31" t="s">
+      <c r="G38" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="H38" s="36" t="s">
+      <c r="H38" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="I38" s="28" t="s">
+      <c r="I38" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="J38" s="28" t="s">
+      <c r="J38" s="27" t="s">
         <v>180</v>
       </c>
       <c r="K38" s="16"/>
@@ -2679,34 +2678,34 @@
       <c r="R38" s="16"/>
     </row>
     <row r="39" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="28">
+      <c r="A39" s="27">
         <v>39</v>
       </c>
-      <c r="B39" s="28" t="s">
+      <c r="B39" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="C39" s="28" t="s">
+      <c r="C39" s="27" t="s">
         <v>140</v>
       </c>
-      <c r="D39" s="31" t="s">
+      <c r="D39" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="E39" s="31" t="s">
+      <c r="E39" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="F39" s="35" t="s">
+      <c r="F39" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="G39" s="31" t="s">
+      <c r="G39" s="30" t="s">
         <v>143</v>
       </c>
-      <c r="H39" s="35" t="s">
+      <c r="H39" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="I39" s="28" t="s">
+      <c r="I39" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J39" s="28" t="s">
+      <c r="J39" s="27" t="s">
         <v>180</v>
       </c>
       <c r="K39" s="16"/>
@@ -2719,34 +2718,34 @@
       <c r="R39" s="16"/>
     </row>
     <row r="40" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="28">
+      <c r="A40" s="27">
         <v>40</v>
       </c>
-      <c r="B40" s="28" t="s">
+      <c r="B40" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="C40" s="28" t="s">
+      <c r="C40" s="27" t="s">
         <v>140</v>
       </c>
-      <c r="D40" s="31" t="s">
+      <c r="D40" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="E40" s="31" t="s">
+      <c r="E40" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="F40" s="35" t="s">
+      <c r="F40" s="34" t="s">
         <v>147</v>
       </c>
-      <c r="G40" s="31" t="s">
+      <c r="G40" s="30" t="s">
         <v>145</v>
       </c>
-      <c r="H40" s="35" t="s">
+      <c r="H40" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="I40" s="28" t="s">
+      <c r="I40" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J40" s="28" t="s">
+      <c r="J40" s="27" t="s">
         <v>180</v>
       </c>
       <c r="K40" s="16"/>
@@ -2759,34 +2758,34 @@
       <c r="R40" s="16"/>
     </row>
     <row r="41" spans="1:18" ht="75" x14ac:dyDescent="0.25">
-      <c r="A41" s="28">
+      <c r="A41" s="27">
         <v>41</v>
       </c>
-      <c r="B41" s="28" t="s">
+      <c r="B41" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="C41" s="28" t="s">
+      <c r="C41" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="D41" s="31" t="s">
+      <c r="D41" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="E41" s="28" t="s">
+      <c r="E41" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="F41" s="35" t="s">
+      <c r="F41" s="34" t="s">
         <v>149</v>
       </c>
-      <c r="G41" s="31" t="s">
+      <c r="G41" s="30" t="s">
         <v>214</v>
       </c>
-      <c r="H41" s="35" t="s">
+      <c r="H41" s="34" t="s">
         <v>219</v>
       </c>
-      <c r="I41" s="28" t="s">
+      <c r="I41" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J41" s="28" t="s">
+      <c r="J41" s="27" t="s">
         <v>180</v>
       </c>
       <c r="K41" s="16"/>
@@ -2799,34 +2798,34 @@
       <c r="R41" s="16"/>
     </row>
     <row r="42" spans="1:18" ht="75" x14ac:dyDescent="0.25">
-      <c r="A42" s="28">
+      <c r="A42" s="27">
         <v>42</v>
       </c>
-      <c r="B42" s="28" t="s">
+      <c r="B42" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="C42" s="28" t="s">
+      <c r="C42" s="27" t="s">
         <v>150</v>
       </c>
-      <c r="D42" s="31" t="s">
+      <c r="D42" s="30" t="s">
         <v>220</v>
       </c>
-      <c r="E42" s="28" t="s">
+      <c r="E42" s="27" t="s">
         <v>221</v>
       </c>
-      <c r="F42" s="35" t="s">
+      <c r="F42" s="34" t="s">
         <v>151</v>
       </c>
-      <c r="G42" s="31" t="s">
+      <c r="G42" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="H42" s="35" t="s">
+      <c r="H42" s="34" t="s">
         <v>222</v>
       </c>
-      <c r="I42" s="28" t="s">
+      <c r="I42" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J42" s="28" t="s">
+      <c r="J42" s="27" t="s">
         <v>180</v>
       </c>
       <c r="K42" s="16"/>
@@ -2839,34 +2838,34 @@
       <c r="R42" s="16"/>
     </row>
     <row r="43" spans="1:18" ht="60" x14ac:dyDescent="0.25">
-      <c r="A43" s="28">
+      <c r="A43" s="27">
         <v>43</v>
       </c>
-      <c r="B43" s="28" t="s">
+      <c r="B43" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="C43" s="28" t="s">
+      <c r="C43" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="D43" s="31" t="s">
+      <c r="D43" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="E43" s="28" t="s">
+      <c r="E43" s="27" t="s">
         <v>216</v>
       </c>
-      <c r="F43" s="35" t="s">
+      <c r="F43" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="G43" s="31" t="s">
+      <c r="G43" s="30" t="s">
         <v>214</v>
       </c>
-      <c r="H43" s="35" t="s">
+      <c r="H43" s="34" t="s">
         <v>223</v>
       </c>
-      <c r="I43" s="28" t="s">
+      <c r="I43" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J43" s="28" t="s">
+      <c r="J43" s="27" t="s">
         <v>180</v>
       </c>
       <c r="K43" s="16"/>
@@ -2879,34 +2878,34 @@
       <c r="R43" s="16"/>
     </row>
     <row r="44" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="28">
+      <c r="A44" s="27">
         <v>44</v>
       </c>
-      <c r="B44" s="28" t="s">
+      <c r="B44" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="C44" s="28" t="s">
+      <c r="C44" s="27" t="s">
         <v>155</v>
       </c>
-      <c r="D44" s="31" t="s">
+      <c r="D44" s="30" t="s">
         <v>215</v>
       </c>
-      <c r="E44" s="28" t="s">
+      <c r="E44" s="27" t="s">
         <v>216</v>
       </c>
-      <c r="F44" s="35" t="s">
+      <c r="F44" s="34" t="s">
         <v>153</v>
       </c>
-      <c r="G44" s="31" t="s">
+      <c r="G44" s="30" t="s">
         <v>214</v>
       </c>
-      <c r="H44" s="35" t="s">
+      <c r="H44" s="34" t="s">
         <v>213</v>
       </c>
-      <c r="I44" s="28" t="s">
+      <c r="I44" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J44" s="28" t="s">
+      <c r="J44" s="27" t="s">
         <v>180</v>
       </c>
       <c r="K44" s="16"/>
@@ -2919,34 +2918,34 @@
       <c r="R44" s="16"/>
     </row>
     <row r="45" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="28">
+      <c r="A45" s="27">
         <v>45</v>
       </c>
-      <c r="B45" s="28" t="s">
+      <c r="B45" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="C45" s="28" t="s">
+      <c r="C45" s="27" t="s">
         <v>158</v>
       </c>
-      <c r="D45" s="31" t="s">
+      <c r="D45" s="30" t="s">
         <v>206</v>
       </c>
-      <c r="E45" s="28" t="s">
+      <c r="E45" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="F45" s="35" t="s">
+      <c r="F45" s="34" t="s">
         <v>154</v>
       </c>
-      <c r="G45" s="31" t="s">
+      <c r="G45" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="34" t="s">
         <v>205</v>
       </c>
-      <c r="I45" s="28" t="s">
+      <c r="I45" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J45" s="28" t="s">
+      <c r="J45" s="27" t="s">
         <v>180</v>
       </c>
       <c r="K45" s="16"/>
@@ -2959,34 +2958,34 @@
       <c r="R45" s="16"/>
     </row>
     <row r="46" spans="1:18" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="28">
+      <c r="A46" s="27">
         <v>46</v>
       </c>
-      <c r="B46" s="28" t="s">
+      <c r="B46" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="C46" s="28" t="s">
+      <c r="C46" s="27" t="s">
         <v>157</v>
       </c>
-      <c r="D46" s="31" t="s">
+      <c r="D46" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="E46" s="28" t="s">
+      <c r="E46" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="F46" s="35" t="s">
+      <c r="F46" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="G46" s="31" t="s">
+      <c r="G46" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="34" t="s">
         <v>204</v>
       </c>
-      <c r="I46" s="28" t="s">
+      <c r="I46" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J46" s="28" t="s">
+      <c r="J46" s="27" t="s">
         <v>180</v>
       </c>
       <c r="K46" s="16"/>
@@ -2999,34 +2998,34 @@
       <c r="R46" s="16"/>
     </row>
     <row r="47" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A47" s="28">
+      <c r="A47" s="27">
         <v>47</v>
       </c>
-      <c r="B47" s="28" t="s">
+      <c r="B47" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="C47" s="28" t="s">
+      <c r="C47" s="27" t="s">
         <v>160</v>
       </c>
-      <c r="D47" s="31" t="s">
+      <c r="D47" s="30" t="s">
         <v>185</v>
       </c>
-      <c r="E47" s="28" t="s">
+      <c r="E47" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="F47" s="35" t="s">
+      <c r="F47" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="G47" s="31" t="s">
+      <c r="G47" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="H47" s="35" t="s">
+      <c r="H47" s="34" t="s">
         <v>186</v>
       </c>
-      <c r="I47" s="28" t="s">
+      <c r="I47" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J47" s="28" t="s">
+      <c r="J47" s="27" t="s">
         <v>180</v>
       </c>
       <c r="K47" s="16"/>
@@ -3039,34 +3038,34 @@
       <c r="R47" s="16"/>
     </row>
     <row r="48" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="28">
+      <c r="A48" s="27">
         <v>48</v>
       </c>
-      <c r="B48" s="28" t="s">
+      <c r="B48" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="C48" s="28" t="s">
+      <c r="C48" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="D48" s="31" t="s">
+      <c r="D48" s="30" t="s">
         <v>185</v>
       </c>
-      <c r="E48" s="28" t="s">
+      <c r="E48" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="F48" s="35" t="s">
+      <c r="F48" s="34" t="s">
         <v>163</v>
       </c>
-      <c r="G48" s="31" t="s">
+      <c r="G48" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="H48" s="35" t="s">
+      <c r="H48" s="34" t="s">
         <v>184</v>
       </c>
-      <c r="I48" s="28" t="s">
+      <c r="I48" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J48" s="28" t="s">
+      <c r="J48" s="27" t="s">
         <v>180</v>
       </c>
       <c r="K48" s="16"/>
@@ -3079,34 +3078,34 @@
       <c r="R48" s="16"/>
     </row>
     <row r="49" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A49" s="28">
+      <c r="A49" s="27">
         <v>49</v>
       </c>
-      <c r="B49" s="28" t="s">
+      <c r="B49" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="C49" s="28" t="s">
+      <c r="C49" s="27" t="s">
         <v>164</v>
       </c>
-      <c r="D49" s="31" t="s">
+      <c r="D49" s="30" t="s">
         <v>199</v>
       </c>
-      <c r="E49" s="28" t="s">
+      <c r="E49" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="F49" s="35" t="s">
+      <c r="F49" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="G49" s="28" t="s">
+      <c r="G49" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="H49" s="35" t="s">
+      <c r="H49" s="34" t="s">
         <v>200</v>
       </c>
-      <c r="I49" s="28" t="s">
+      <c r="I49" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J49" s="28" t="s">
+      <c r="J49" s="27" t="s">
         <v>180</v>
       </c>
       <c r="K49" s="16"/>
@@ -3119,34 +3118,34 @@
       <c r="R49" s="16"/>
     </row>
     <row r="50" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A50" s="28">
-        <v>50</v>
-      </c>
-      <c r="B50" s="28" t="s">
+      <c r="A50" s="27">
+        <v>50</v>
+      </c>
+      <c r="B50" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="C50" s="28" t="s">
+      <c r="C50" s="27" t="s">
         <v>165</v>
       </c>
-      <c r="D50" s="31" t="s">
+      <c r="D50" s="30" t="s">
         <v>199</v>
       </c>
-      <c r="E50" s="28" t="s">
+      <c r="E50" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="F50" s="35" t="s">
+      <c r="F50" s="34" t="s">
         <v>167</v>
       </c>
-      <c r="G50" s="28" t="s">
+      <c r="G50" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="H50" s="35" t="s">
+      <c r="H50" s="34" t="s">
         <v>201</v>
       </c>
-      <c r="I50" s="28" t="s">
+      <c r="I50" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J50" s="28" t="s">
+      <c r="J50" s="27" t="s">
         <v>180</v>
       </c>
       <c r="K50" s="16"/>
@@ -3159,34 +3158,34 @@
       <c r="R50" s="16"/>
     </row>
     <row r="51" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A51" s="28">
+      <c r="A51" s="27">
         <v>51</v>
       </c>
-      <c r="B51" s="28" t="s">
+      <c r="B51" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="C51" s="28" t="s">
+      <c r="C51" s="27" t="s">
         <v>169</v>
       </c>
-      <c r="D51" s="31" t="s">
+      <c r="D51" s="30" t="s">
         <v>210</v>
       </c>
-      <c r="E51" s="28" t="s">
+      <c r="E51" s="27" t="s">
         <v>207</v>
       </c>
-      <c r="F51" s="35" t="s">
+      <c r="F51" s="34" t="s">
         <v>168</v>
       </c>
-      <c r="G51" s="31" t="s">
+      <c r="G51" s="30" t="s">
         <v>209</v>
       </c>
-      <c r="H51" s="35" t="s">
+      <c r="H51" s="34" t="s">
         <v>208</v>
       </c>
-      <c r="I51" s="28" t="s">
+      <c r="I51" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J51" s="28" t="s">
+      <c r="J51" s="27" t="s">
         <v>180</v>
       </c>
       <c r="K51" s="16"/>
@@ -3199,34 +3198,34 @@
       <c r="R51" s="16"/>
     </row>
     <row r="52" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A52" s="28">
+      <c r="A52" s="27">
         <v>52</v>
       </c>
-      <c r="B52" s="28" t="s">
+      <c r="B52" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="C52" s="28" t="s">
+      <c r="C52" s="27" t="s">
         <v>170</v>
       </c>
-      <c r="D52" s="31" t="s">
+      <c r="D52" s="30" t="s">
         <v>211</v>
       </c>
-      <c r="E52" s="28" t="s">
+      <c r="E52" s="27" t="s">
         <v>193</v>
       </c>
-      <c r="F52" s="35" t="s">
+      <c r="F52" s="34" t="s">
         <v>171</v>
       </c>
-      <c r="G52" s="28" t="s">
+      <c r="G52" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="H52" s="35" t="s">
+      <c r="H52" s="34" t="s">
         <v>194</v>
       </c>
-      <c r="I52" s="28" t="s">
+      <c r="I52" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J52" s="28" t="s">
+      <c r="J52" s="27" t="s">
         <v>180</v>
       </c>
       <c r="K52" s="16"/>
@@ -3239,34 +3238,34 @@
       <c r="R52" s="16"/>
     </row>
     <row r="53" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="28">
+      <c r="A53" s="27">
         <v>53</v>
       </c>
-      <c r="B53" s="28" t="s">
+      <c r="B53" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="C53" s="28" t="s">
+      <c r="C53" s="27" t="s">
         <v>172</v>
       </c>
-      <c r="D53" s="31" t="s">
+      <c r="D53" s="30" t="s">
         <v>211</v>
       </c>
-      <c r="E53" s="28" t="s">
+      <c r="E53" s="27" t="s">
         <v>189</v>
       </c>
-      <c r="F53" s="35" t="s">
+      <c r="F53" s="34" t="s">
         <v>173</v>
       </c>
-      <c r="G53" s="31" t="s">
+      <c r="G53" s="30" t="s">
         <v>188</v>
       </c>
-      <c r="H53" s="35" t="s">
+      <c r="H53" s="34" t="s">
         <v>187</v>
       </c>
-      <c r="I53" s="28" t="s">
+      <c r="I53" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J53" s="28" t="s">
+      <c r="J53" s="27" t="s">
         <v>180</v>
       </c>
       <c r="K53" s="16"/>
@@ -3279,34 +3278,34 @@
       <c r="R53" s="16"/>
     </row>
     <row r="54" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="28">
+      <c r="A54" s="27">
         <v>54</v>
       </c>
-      <c r="B54" s="28" t="s">
+      <c r="B54" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="C54" s="28" t="s">
+      <c r="C54" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="D54" s="31" t="s">
+      <c r="D54" s="30" t="s">
         <v>211</v>
       </c>
-      <c r="E54" s="28" t="s">
+      <c r="E54" s="27" t="s">
         <v>190</v>
       </c>
-      <c r="F54" s="35" t="s">
+      <c r="F54" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="G54" s="31" t="s">
+      <c r="G54" s="30" t="s">
         <v>191</v>
       </c>
-      <c r="H54" s="35" t="s">
+      <c r="H54" s="34" t="s">
         <v>192</v>
       </c>
-      <c r="I54" s="28" t="s">
+      <c r="I54" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J54" s="28" t="s">
+      <c r="J54" s="27" t="s">
         <v>180</v>
       </c>
       <c r="K54" s="16"/>
@@ -3319,34 +3318,36 @@
       <c r="R54" s="16"/>
     </row>
     <row r="55" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A55" s="28">
+      <c r="A55" s="27">
         <v>55</v>
       </c>
-      <c r="B55" s="28" t="s">
+      <c r="B55" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="C55" s="28" t="s">
+      <c r="C55" s="27" t="s">
         <v>176</v>
       </c>
-      <c r="D55" s="31" t="s">
+      <c r="D55" s="30" t="s">
         <v>227</v>
       </c>
-      <c r="E55" s="28" t="s">
+      <c r="E55" s="27" t="s">
         <v>226</v>
       </c>
-      <c r="F55" s="35" t="s">
+      <c r="F55" s="34" t="s">
         <v>177</v>
       </c>
-      <c r="G55" s="31" t="s">
+      <c r="G55" s="30" t="s">
         <v>225</v>
       </c>
-      <c r="H55" s="35" t="s">
+      <c r="H55" s="34" t="s">
         <v>224</v>
       </c>
-      <c r="I55" s="28" t="s">
+      <c r="I55" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="J55" s="28"/>
+      <c r="J55" s="27" t="s">
+        <v>180</v>
+      </c>
       <c r="K55" s="16"/>
       <c r="L55" s="16"/>
       <c r="M55" s="16"/>
@@ -3357,34 +3358,34 @@
       <c r="R55" s="16"/>
     </row>
     <row r="56" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="28">
+      <c r="A56" s="27">
         <v>56</v>
       </c>
-      <c r="B56" s="28" t="s">
+      <c r="B56" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="C56" s="28" t="s">
+      <c r="C56" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="D56" s="31" t="s">
+      <c r="D56" s="30" t="s">
         <v>197</v>
       </c>
-      <c r="E56" s="28" t="s">
+      <c r="E56" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="F56" s="35" t="s">
+      <c r="F56" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="G56" s="28" t="s">
+      <c r="G56" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="H56" s="35" t="s">
+      <c r="H56" s="34" t="s">
         <v>198</v>
       </c>
-      <c r="I56" s="28" t="s">
+      <c r="I56" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="J56" s="28" t="s">
+      <c r="J56" s="27" t="s">
         <v>180</v>
       </c>
       <c r="K56" s="16"/>
@@ -3397,68 +3398,98 @@
       <c r="R56" s="16"/>
     </row>
     <row r="57" spans="1:18" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A57" s="30">
+      <c r="A57" s="29">
         <v>57</v>
       </c>
-      <c r="B57" s="28" t="s">
+      <c r="B57" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C57" s="28" t="s">
+      <c r="C57" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D57" s="31" t="s">
+      <c r="D57" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="E57" s="28" t="s">
+      <c r="E57" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="F57" s="35" t="s">
+      <c r="F57" s="34" t="s">
         <v>195</v>
       </c>
-      <c r="G57" s="31" t="s">
+      <c r="G57" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="H57" s="35" t="s">
+      <c r="H57" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="I57" s="28" t="s">
+      <c r="I57" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="J57" s="28" t="s">
+      <c r="J57" s="27" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="58" spans="1:18" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="30">
+      <c r="A58" s="29">
         <v>58</v>
       </c>
-      <c r="B58" s="28" t="s">
+      <c r="B58" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C58" s="28" t="s">
+      <c r="C58" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D58" s="31" t="s">
+      <c r="D58" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="E58" s="28" t="s">
+      <c r="E58" s="27" t="s">
         <v>190</v>
       </c>
-      <c r="F58" s="35" t="s">
+      <c r="F58" s="34" t="s">
         <v>217</v>
       </c>
-      <c r="G58" s="31" t="s">
+      <c r="G58" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="H58" s="35" t="s">
+      <c r="H58" s="34" t="s">
         <v>218</v>
       </c>
-      <c r="I58" s="28" t="s">
+      <c r="I58" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="J58" s="28" t="s">
+      <c r="J58" s="27" t="s">
         <v>180</v>
       </c>
+    </row>
+    <row r="59" spans="1:18" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A59" s="29">
+        <v>59</v>
+      </c>
+      <c r="B59" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D59" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="E59" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="F59" s="34" t="s">
+        <v>228</v>
+      </c>
+      <c r="G59" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="H59" s="34" t="s">
+        <v>229</v>
+      </c>
+      <c r="I59" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="J59" s="27"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I24"/>
@@ -3469,10 +3500,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M59"/>
+  <dimension ref="A1:M58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3595,9 +3626,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="L3" s="2"/>
       <c r="M3" s="2" t="s">
         <v>50</v>
       </c>
@@ -3622,9 +3651,7 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="L4" s="2"/>
       <c r="M4" s="2" t="s">
         <v>50</v>
       </c>
@@ -3693,7 +3720,9 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
+      <c r="M6" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
@@ -4533,7 +4562,9 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
+      <c r="M26" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="27" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
@@ -4556,7 +4587,9 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
+      <c r="M27" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="17">
@@ -4579,7 +4612,9 @@
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
+      <c r="M28" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="29" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="17">
@@ -4602,7 +4637,9 @@
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
+      <c r="M29" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="30" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="17">
@@ -4625,7 +4662,9 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
+      <c r="M30" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="31" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="17">
@@ -4648,7 +4687,9 @@
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
+      <c r="M31" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="32" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="17">
@@ -4671,7 +4712,9 @@
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
+      <c r="M32" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="33" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
@@ -4694,7 +4737,9 @@
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
+      <c r="M33" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="34" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="17">
@@ -4717,7 +4762,9 @@
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
+      <c r="M34" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="35" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="17">
@@ -4740,7 +4787,9 @@
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
+      <c r="M35" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="36" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="17">
@@ -4763,7 +4812,9 @@
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
+      <c r="M36" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="37" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="17">
@@ -4786,7 +4837,9 @@
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
+      <c r="M37" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="17">
@@ -4852,7 +4905,9 @@
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
+      <c r="M39" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="17">
@@ -4875,7 +4930,9 @@
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
-      <c r="M40" s="2"/>
+      <c r="M40" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="41" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="17">
@@ -4898,7 +4955,9 @@
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
+      <c r="M41" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="42" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="17">
@@ -4921,7 +4980,9 @@
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
-      <c r="M42" s="2"/>
+      <c r="M42" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="43" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="17">
@@ -4944,7 +5005,9 @@
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
-      <c r="M43" s="2"/>
+      <c r="M43" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="44" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="17">
@@ -4967,7 +5030,9 @@
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
-      <c r="M44" s="2"/>
+      <c r="M44" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="45" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="17">
@@ -4990,7 +5055,9 @@
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
-      <c r="M45" s="2"/>
+      <c r="M45" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="17">
@@ -5013,7 +5080,9 @@
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
-      <c r="M46" s="2"/>
+      <c r="M46" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="47" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="17">
@@ -5036,7 +5105,9 @@
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
-      <c r="M47" s="2"/>
+      <c r="M47" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="48" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="17">
@@ -5059,7 +5130,9 @@
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
-      <c r="M48" s="2"/>
+      <c r="M48" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="49" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="17">
@@ -5082,7 +5155,9 @@
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
-      <c r="M49" s="2"/>
+      <c r="M49" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="50" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="17">
@@ -5105,7 +5180,9 @@
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
-      <c r="M50" s="2"/>
+      <c r="M50" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="51" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="17">
@@ -5128,7 +5205,9 @@
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
-      <c r="M51" s="2"/>
+      <c r="M51" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="52" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="17">
@@ -5151,7 +5230,9 @@
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
-      <c r="M52" s="2"/>
+      <c r="M52" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="53" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="17">
@@ -5174,7 +5255,9 @@
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
-      <c r="M53" s="2"/>
+      <c r="M53" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="17">
@@ -5197,7 +5280,9 @@
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
-      <c r="M54" s="2"/>
+      <c r="M54" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="55" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="17">
@@ -5263,7 +5348,9 @@
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
-      <c r="M56" s="2"/>
+      <c r="M56" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="57" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="17">
@@ -5350,9 +5437,6 @@
       <c r="M58" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="M59" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10949,8 +11033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M58"/>
   <sheetViews>
-    <sheetView topLeftCell="D38" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:M58"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12812,7 +12896,7 @@
   <dimension ref="C9:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:F9"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12843,15 +12927,15 @@
       </c>
       <c r="D10" s="17">
         <f>COUNTIF('Controleur CA'!B:B,Synthèse!C10)</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E10" s="17">
         <f>IF(ISERROR(SUMPRODUCT(('Controleur CA'!J:J="fait")*('Controleur CA'!B:B=C10))),"Aucun",SUMPRODUCT(('Controleur CA'!J:J="fait")*('Controleur CA'!B:B=C10)))</f>
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F10" s="21">
         <f>E10/D10*100</f>
-        <v>92.592592592592595</v>
+        <v>96.428571428571431</v>
       </c>
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.25">
@@ -12881,11 +12965,11 @@
       </c>
       <c r="E12" s="17">
         <f>IF(ISERROR(SUMPRODUCT(('Controleur CA'!J:J="fait")*('Controleur CA'!B:B=C12))),"Aucun",SUMPRODUCT(('Controleur CA'!J:J="fait")*('Controleur CA'!B:B=C12)))</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F12" s="21">
         <f>E12/D12*100</f>
-        <v>94.444444444444443</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="3:6" x14ac:dyDescent="0.25">
@@ -12894,24 +12978,26 @@
       </c>
       <c r="D13" s="17">
         <f>D10+D11+D12</f>
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E13" s="17">
         <f>E10+E11+E12</f>
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F13" s="21">
         <f>(F10+F11+F12)/3</f>
-        <v>95.679012345679027</v>
+        <v>98.80952380952381</v>
       </c>
     </row>
     <row r="15" spans="3:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="25" t="s">
         <v>202</v>
       </c>
-      <c r="D15" s="38"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="40"/>
+      <c r="D15" s="37" t="s">
+        <v>230</v>
+      </c>
+      <c r="E15" s="38"/>
+      <c r="F15" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
*** Version v 1.9 *** - Ajout du contrôle 40 et mutualistion avec les contrôles de structuration des couches - Correction des contrôles de structuration des couches
</commit_message>
<xml_diff>
--- a/Documentation/Controleur.xlsx
+++ b/Documentation/Controleur.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="8370" yWindow="1320" windowWidth="6915" windowHeight="6540"/>
+    <workbookView xWindow="8370" yWindow="1320" windowWidth="6915" windowHeight="6540" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Controleur CA" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Controleur CA'!$A$1:$I$24</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1897" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1904" uniqueCount="233">
   <si>
     <t>Famille</t>
   </si>
@@ -455,15 +454,9 @@
     <t>Vérifier que toutes les couches sont présentes selon les spec_QGIS</t>
   </si>
   <si>
-    <t>[couches]</t>
-  </si>
-  <si>
     <t>La couche est manquante</t>
   </si>
   <si>
-    <t>[Attribut]</t>
-  </si>
-  <si>
     <t>L'attribut est manquant</t>
   </si>
   <si>
@@ -716,14 +709,26 @@
     <t>Format de nommage du numéro de point technique incorrect</t>
   </si>
   <si>
-    <t>J'ai ajouté de nouveaux contrôles après étude des specifications Orange</t>
+    <t>Refonte</t>
+  </si>
+  <si>
+    <t>Refonte de contrôles</t>
+  </si>
+  <si>
+    <t>Nb refonte</t>
+  </si>
+  <si>
+    <t>[Couche]</t>
+  </si>
+  <si>
+    <t>J'ai ajouté de nouveaux contrôles à réaliser après étude des specifications Orange + refonte prévue des contrôles + gestion des cas particuliers + stabilité programme (optimisation, commentaires,…?) + nouveau système de gestion et affichage des erreurs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -739,8 +744,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -765,8 +786,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -894,10 +927,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
-      </left>
-      <right/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -907,9 +940,147 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
-      <right/>
-      <top style="thin">
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -925,16 +1096,149 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -984,13 +1288,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -999,9 +1296,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1036,23 +1330,92 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="5" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFCC66"/>
       <color rgb="FFFFFFCC"/>
       <color rgb="FFFFCC99"/>
     </mruColors>
@@ -1354,921 +1717,960 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F50" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G67" sqref="G67"/>
+    <sheetView topLeftCell="E7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" style="28" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" style="28" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" style="28" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" style="31" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" style="28" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.28515625" style="36" customWidth="1"/>
-    <col min="7" max="7" width="33.28515625" style="31" customWidth="1"/>
-    <col min="8" max="8" width="49.7109375" style="36" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" style="28" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" style="28" customWidth="1"/>
-    <col min="11" max="12" width="35.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" style="24" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" style="24" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="24" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" style="27" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.28515625" style="32" customWidth="1"/>
+    <col min="7" max="7" width="33.28515625" style="27" customWidth="1"/>
+    <col min="8" max="8" width="49.7109375" style="32" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" style="24" customWidth="1"/>
+    <col min="10" max="11" width="17.85546875" style="24" customWidth="1"/>
+    <col min="12" max="12" width="35.140625" customWidth="1"/>
     <col min="13" max="13" width="23" customWidth="1"/>
     <col min="14" max="14" width="35.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="I1" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="33" t="s">
+      <c r="J1" s="29" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="29">
+      <c r="K1" s="29" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="25">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="34" t="s">
+      <c r="F2" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="G2" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="H2" s="34" t="s">
+      <c r="H2" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="I2" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="27" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="16" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="29">
+      <c r="J2" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K2" s="23"/>
+    </row>
+    <row r="3" spans="1:11" s="16" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="25">
         <v>2</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="34" t="s">
+      <c r="F3" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="34" t="s">
+      <c r="H3" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="I3" s="27" t="s">
+      <c r="I3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="27" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="29">
+      <c r="J3" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K3" s="23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="25">
         <v>3</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="F4" s="34" t="s">
+      <c r="F4" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="G4" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="34" t="s">
+      <c r="H4" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="I4" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="27" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="29">
+      <c r="J4" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K4" s="23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="25">
         <v>4</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="34" t="s">
+      <c r="F5" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="30" t="s">
+      <c r="G5" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="H5" s="34" t="s">
+      <c r="H5" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="I5" s="27" t="s">
+      <c r="I5" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="27" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="29">
+      <c r="J5" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K5" s="23"/>
+    </row>
+    <row r="6" spans="1:11" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="25">
         <v>5</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="F6" s="34" t="s">
+      <c r="F6" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="30" t="s">
+      <c r="G6" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="H6" s="34" t="s">
+      <c r="H6" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="I6" s="27" t="s">
+      <c r="I6" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J6" s="27" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="29">
+      <c r="J6" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K6" s="23"/>
+    </row>
+    <row r="7" spans="1:11" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="25">
         <v>6</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="F7" s="34" t="s">
+      <c r="F7" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="30" t="s">
+      <c r="G7" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="H7" s="34" t="s">
+      <c r="H7" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="I7" s="27" t="s">
+      <c r="I7" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="27" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="29">
+      <c r="J7" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K7" s="23"/>
+    </row>
+    <row r="8" spans="1:11" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="25">
         <v>7</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="F8" s="34" t="s">
+      <c r="F8" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="30" t="s">
+      <c r="G8" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="34" t="s">
+      <c r="H8" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="I8" s="27" t="s">
+      <c r="I8" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J8" s="27" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="29">
+      <c r="J8" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K8" s="23"/>
+    </row>
+    <row r="9" spans="1:11" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="25">
         <v>8</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="F9" s="34" t="s">
+      <c r="F9" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="30" t="s">
+      <c r="G9" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="H9" s="34" t="s">
+      <c r="H9" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="I9" s="27" t="s">
+      <c r="I9" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="27" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="29">
+      <c r="J9" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K9" s="23"/>
+    </row>
+    <row r="10" spans="1:11" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="25">
         <v>9</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="E10" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="34" t="s">
+      <c r="F10" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="30" t="s">
+      <c r="G10" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="H10" s="34" t="s">
+      <c r="H10" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="I10" s="27" t="s">
+      <c r="I10" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="J10" s="27" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="16" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A11" s="29">
+      <c r="J10" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K10" s="23"/>
+    </row>
+    <row r="11" spans="1:11" s="16" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="25">
         <v>10</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="E11" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="F11" s="34" t="s">
+      <c r="F11" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="30" t="s">
+      <c r="G11" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="H11" s="34" t="s">
+      <c r="H11" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="I11" s="27" t="s">
+      <c r="I11" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J11" s="27" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="16" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A12" s="29">
+      <c r="J11" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K11" s="23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="16" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="25">
         <v>11</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="34" t="s">
+      <c r="F12" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="30" t="s">
+      <c r="G12" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="H12" s="34" t="s">
+      <c r="H12" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="I12" s="27" t="s">
+      <c r="I12" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J12" s="27" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="16" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="29">
+      <c r="J12" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K12" s="23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="16" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="25">
         <v>12</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="30" t="s">
+      <c r="D13" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="27" t="s">
+      <c r="E13" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="F13" s="34" t="s">
+      <c r="F13" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="30" t="s">
+      <c r="G13" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="H13" s="34" t="s">
+      <c r="H13" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="I13" s="27" t="s">
+      <c r="I13" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J13" s="27" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="16" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A14" s="29">
+      <c r="J13" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K13" s="23"/>
+    </row>
+    <row r="14" spans="1:11" s="16" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14" s="25">
         <v>13</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="27" t="s">
+      <c r="E14" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="F14" s="34" t="s">
+      <c r="F14" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="30" t="s">
+      <c r="G14" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="H14" s="34" t="s">
+      <c r="H14" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="I14" s="27" t="s">
+      <c r="I14" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="J14" s="27" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="29">
+      <c r="J14" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K14" s="23"/>
+    </row>
+    <row r="15" spans="1:11" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="25">
         <v>15</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="30" t="s">
+      <c r="D15" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="27" t="s">
+      <c r="E15" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="F15" s="34" t="s">
+      <c r="F15" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="30" t="s">
+      <c r="G15" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="H15" s="34" t="s">
+      <c r="H15" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="I15" s="27" t="s">
+      <c r="I15" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="J15" s="27" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="29">
+      <c r="J15" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K15" s="23"/>
+    </row>
+    <row r="16" spans="1:11" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="25">
         <v>16</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="30" t="s">
+      <c r="D16" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="27" t="s">
+      <c r="E16" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="F16" s="34" t="s">
+      <c r="F16" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="G16" s="30" t="s">
+      <c r="G16" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="H16" s="34" t="s">
+      <c r="H16" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="I16" s="27" t="s">
+      <c r="I16" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="J16" s="27" t="s">
-        <v>180</v>
-      </c>
+      <c r="J16" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K16" s="23"/>
     </row>
     <row r="17" spans="1:18" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="29">
+      <c r="A17" s="25">
         <v>17</v>
       </c>
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="30" t="s">
+      <c r="D17" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="27" t="s">
+      <c r="E17" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="F17" s="34" t="s">
+      <c r="F17" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="G17" s="30" t="s">
+      <c r="G17" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="H17" s="34" t="s">
+      <c r="H17" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="I17" s="27" t="s">
+      <c r="I17" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="J17" s="27" t="s">
-        <v>180</v>
-      </c>
+      <c r="J17" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K17" s="23"/>
     </row>
     <row r="18" spans="1:18" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="29">
+      <c r="A18" s="25">
         <v>18</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="C18" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="30" t="s">
+      <c r="D18" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="27" t="s">
+      <c r="E18" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="F18" s="34" t="s">
+      <c r="F18" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="G18" s="30" t="s">
+      <c r="G18" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="H18" s="34" t="s">
+      <c r="H18" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="I18" s="27" t="s">
+      <c r="I18" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="J18" s="27" t="s">
-        <v>180</v>
-      </c>
+      <c r="J18" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K18" s="23"/>
     </row>
     <row r="19" spans="1:18" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="29">
+      <c r="A19" s="25">
         <v>19</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C19" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="30" t="s">
+      <c r="D19" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="27" t="s">
+      <c r="E19" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="F19" s="34" t="s">
+      <c r="F19" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="G19" s="30" t="s">
+      <c r="G19" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="H19" s="35" t="s">
+      <c r="H19" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="I19" s="27" t="s">
+      <c r="I19" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="J19" s="27" t="s">
-        <v>180</v>
-      </c>
+      <c r="J19" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K19" s="23"/>
     </row>
     <row r="20" spans="1:18" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="29">
+      <c r="A20" s="25">
         <v>20</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="27" t="s">
+      <c r="C20" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="30" t="s">
+      <c r="D20" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="27" t="s">
+      <c r="E20" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="F20" s="34" t="s">
+      <c r="F20" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="G20" s="30" t="s">
+      <c r="G20" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="H20" s="34" t="s">
+      <c r="H20" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="I20" s="27" t="s">
+      <c r="I20" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="J20" s="27" t="s">
-        <v>180</v>
-      </c>
+      <c r="J20" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K20" s="23"/>
     </row>
     <row r="21" spans="1:18" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="29">
+      <c r="A21" s="25">
         <v>21</v>
       </c>
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="27" t="s">
+      <c r="C21" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="30" t="s">
+      <c r="D21" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="27" t="s">
+      <c r="E21" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="F21" s="34" t="s">
+      <c r="F21" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="G21" s="30" t="s">
+      <c r="G21" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="H21" s="34" t="s">
+      <c r="H21" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="I21" s="27" t="s">
+      <c r="I21" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="J21" s="27" t="s">
-        <v>180</v>
-      </c>
+      <c r="J21" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K21" s="23"/>
     </row>
     <row r="22" spans="1:18" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="29">
+      <c r="A22" s="25">
         <v>22</v>
       </c>
-      <c r="B22" s="27" t="s">
+      <c r="B22" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="27" t="s">
+      <c r="C22" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="30" t="s">
+      <c r="D22" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="E22" s="27" t="s">
+      <c r="E22" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="F22" s="34" t="s">
+      <c r="F22" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="G22" s="30" t="s">
+      <c r="G22" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="H22" s="34" t="s">
+      <c r="H22" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="I22" s="27" t="s">
+      <c r="I22" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="J22" s="27" t="s">
-        <v>180</v>
-      </c>
+      <c r="J22" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K22" s="23"/>
     </row>
     <row r="23" spans="1:18" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="29">
+      <c r="A23" s="25">
         <v>23</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="27" t="s">
+      <c r="C23" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="30" t="s">
+      <c r="D23" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="E23" s="27" t="s">
+      <c r="E23" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="34" t="s">
+      <c r="F23" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="G23" s="30" t="s">
+      <c r="G23" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="H23" s="34" t="s">
+      <c r="H23" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="I23" s="27" t="s">
+      <c r="I23" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="J23" s="27" t="s">
-        <v>180</v>
-      </c>
+      <c r="J23" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K23" s="23"/>
     </row>
     <row r="24" spans="1:18" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="29">
+      <c r="A24" s="25">
         <v>24</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="30" t="s">
+      <c r="D24" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="E24" s="27" t="s">
+      <c r="E24" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="F24" s="34" t="s">
+      <c r="F24" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="G24" s="30" t="s">
+      <c r="G24" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="H24" s="34" t="s">
+      <c r="H24" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="I24" s="27" t="s">
+      <c r="I24" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="J24" s="27" t="s">
-        <v>180</v>
-      </c>
+      <c r="J24" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K24" s="23"/>
     </row>
     <row r="25" spans="1:18" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="29">
+      <c r="A25" s="25">
         <v>25</v>
       </c>
-      <c r="B25" s="27" t="s">
+      <c r="B25" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="27" t="s">
+      <c r="C25" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="30" t="s">
+      <c r="D25" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="27"/>
-      <c r="F25" s="34" t="s">
+      <c r="E25" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="F25" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="G25" s="30" t="s">
+      <c r="G25" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="H25" s="34" t="s">
+      <c r="H25" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="I25" s="27" t="s">
+      <c r="I25" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="J25" s="27" t="s">
-        <v>180</v>
-      </c>
+      <c r="J25" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K25" s="23"/>
     </row>
     <row r="26" spans="1:18" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="29">
+      <c r="A26" s="25">
         <v>26</v>
       </c>
-      <c r="B26" s="27" t="s">
+      <c r="B26" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="C26" s="27" t="s">
+      <c r="C26" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="D26" s="30" t="s">
+      <c r="D26" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="E26" s="27" t="s">
+      <c r="E26" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="F26" s="34" t="s">
+      <c r="F26" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="G26" s="30" t="s">
+      <c r="G26" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="H26" s="34" t="s">
+      <c r="H26" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="I26" s="27" t="s">
+      <c r="I26" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J26" s="27" t="s">
-        <v>180</v>
-      </c>
+      <c r="J26" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K26" s="23"/>
     </row>
     <row r="27" spans="1:18" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="29">
+      <c r="A27" s="25">
         <v>27</v>
       </c>
-      <c r="B27" s="27" t="s">
+      <c r="B27" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="C27" s="27" t="s">
+      <c r="C27" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="D27" s="30" t="s">
+      <c r="D27" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="E27" s="27" t="s">
+      <c r="E27" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="F27" s="34" t="s">
+      <c r="F27" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="G27" s="30" t="s">
+      <c r="G27" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="H27" s="34" t="s">
+      <c r="H27" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="I27" s="27" t="s">
+      <c r="I27" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J27" s="27" t="s">
-        <v>180</v>
-      </c>
+      <c r="J27" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K27" s="23"/>
     </row>
     <row r="28" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="29">
+      <c r="A28" s="25">
         <v>28</v>
       </c>
-      <c r="B28" s="27" t="s">
+      <c r="B28" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="D28" s="30" t="s">
+      <c r="D28" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="E28" s="27" t="s">
+      <c r="E28" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="F28" s="34" t="s">
+      <c r="F28" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="G28" s="30" t="s">
+      <c r="G28" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="H28" s="34" t="s">
+      <c r="H28" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="I28" s="27" t="s">
+      <c r="I28" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J28" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="K28" s="16"/>
+      <c r="J28" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K28" s="23"/>
       <c r="L28" s="16"/>
       <c r="M28" s="16"/>
       <c r="N28" s="16"/>
@@ -2278,37 +2680,37 @@
       <c r="R28" s="16"/>
     </row>
     <row r="29" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="29">
+      <c r="A29" s="25">
         <v>29</v>
       </c>
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="C29" s="27" t="s">
+      <c r="C29" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="D29" s="30" t="s">
+      <c r="D29" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="E29" s="27" t="s">
+      <c r="E29" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="F29" s="34" t="s">
+      <c r="F29" s="30" t="s">
         <v>120</v>
       </c>
-      <c r="G29" s="30" t="s">
+      <c r="G29" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="H29" s="34" t="s">
+      <c r="H29" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="I29" s="27" t="s">
+      <c r="I29" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J29" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="K29" s="16"/>
+      <c r="J29" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K29" s="23"/>
       <c r="L29" s="16"/>
       <c r="M29" s="16"/>
       <c r="N29" s="16"/>
@@ -2318,37 +2720,37 @@
       <c r="R29" s="16"/>
     </row>
     <row r="30" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="29">
+      <c r="A30" s="25">
         <v>30</v>
       </c>
-      <c r="B30" s="27" t="s">
+      <c r="B30" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="C30" s="27" t="s">
+      <c r="C30" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="D30" s="30" t="s">
+      <c r="D30" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="E30" s="27" t="s">
+      <c r="E30" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="F30" s="34" t="s">
+      <c r="F30" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="G30" s="30" t="s">
+      <c r="G30" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="H30" s="34" t="s">
+      <c r="H30" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="I30" s="27" t="s">
+      <c r="I30" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J30" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="K30" s="16"/>
+      <c r="J30" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K30" s="23"/>
       <c r="L30" s="16"/>
       <c r="M30" s="16"/>
       <c r="N30" s="16"/>
@@ -2358,37 +2760,37 @@
       <c r="R30" s="16"/>
     </row>
     <row r="31" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="29">
+      <c r="A31" s="25">
         <v>31</v>
       </c>
-      <c r="B31" s="27" t="s">
+      <c r="B31" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="C31" s="27" t="s">
+      <c r="C31" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="D31" s="30" t="s">
+      <c r="D31" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="E31" s="27" t="s">
+      <c r="E31" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="F31" s="34" t="s">
+      <c r="F31" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="G31" s="30" t="s">
+      <c r="G31" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="H31" s="34" t="s">
+      <c r="H31" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="I31" s="27" t="s">
+      <c r="I31" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J31" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="K31" s="16"/>
+      <c r="J31" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K31" s="23"/>
       <c r="L31" s="16"/>
       <c r="M31" s="16"/>
       <c r="N31" s="16"/>
@@ -2398,37 +2800,37 @@
       <c r="R31" s="16"/>
     </row>
     <row r="32" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="29">
+      <c r="A32" s="25">
         <v>32</v>
       </c>
-      <c r="B32" s="27" t="s">
+      <c r="B32" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="C32" s="27" t="s">
+      <c r="C32" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="D32" s="30" t="s">
+      <c r="D32" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="E32" s="27" t="s">
+      <c r="E32" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="F32" s="34" t="s">
+      <c r="F32" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="G32" s="30" t="s">
+      <c r="G32" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="H32" s="34" t="s">
+      <c r="H32" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="I32" s="27" t="s">
+      <c r="I32" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J32" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="K32" s="16"/>
+      <c r="J32" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K32" s="23"/>
       <c r="L32" s="16"/>
       <c r="M32" s="16"/>
       <c r="N32" s="16"/>
@@ -2438,37 +2840,37 @@
       <c r="R32" s="16"/>
     </row>
     <row r="33" spans="1:18" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="29">
+      <c r="A33" s="25">
         <v>33</v>
       </c>
-      <c r="B33" s="27" t="s">
+      <c r="B33" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="C33" s="27" t="s">
+      <c r="C33" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="D33" s="30" t="s">
+      <c r="D33" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="E33" s="27" t="s">
+      <c r="E33" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="F33" s="34" t="s">
+      <c r="F33" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="G33" s="30" t="s">
+      <c r="G33" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="H33" s="34" t="s">
+      <c r="H33" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="I33" s="27" t="s">
+      <c r="I33" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J33" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="K33" s="16"/>
+      <c r="J33" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K33" s="23"/>
       <c r="L33" s="16"/>
       <c r="M33" s="16"/>
       <c r="N33" s="16"/>
@@ -2478,37 +2880,37 @@
       <c r="R33" s="16"/>
     </row>
     <row r="34" spans="1:18" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="29">
+      <c r="A34" s="25">
         <v>34</v>
       </c>
-      <c r="B34" s="27" t="s">
+      <c r="B34" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="C34" s="27" t="s">
+      <c r="C34" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="D34" s="30" t="s">
+      <c r="D34" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="E34" s="27" t="s">
+      <c r="E34" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="F34" s="34" t="s">
+      <c r="F34" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="G34" s="30" t="s">
+      <c r="G34" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="H34" s="34" t="s">
+      <c r="H34" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="I34" s="27" t="s">
+      <c r="I34" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J34" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="K34" s="16"/>
+      <c r="J34" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K34" s="23"/>
       <c r="L34" s="16"/>
       <c r="M34" s="16"/>
       <c r="N34" s="16"/>
@@ -2518,37 +2920,37 @@
       <c r="R34" s="16"/>
     </row>
     <row r="35" spans="1:18" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="29">
+      <c r="A35" s="25">
         <v>35</v>
       </c>
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="C35" s="27" t="s">
+      <c r="C35" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="D35" s="30" t="s">
+      <c r="D35" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="E35" s="27" t="s">
+      <c r="E35" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="F35" s="34" t="s">
+      <c r="F35" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="G35" s="30" t="s">
+      <c r="G35" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="H35" s="34" t="s">
+      <c r="H35" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="I35" s="27" t="s">
+      <c r="I35" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J35" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="K35" s="16"/>
+      <c r="J35" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K35" s="23"/>
       <c r="L35" s="16"/>
       <c r="M35" s="16"/>
       <c r="N35" s="16"/>
@@ -2558,37 +2960,37 @@
       <c r="R35" s="16"/>
     </row>
     <row r="36" spans="1:18" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="29">
+      <c r="A36" s="25">
         <v>36</v>
       </c>
-      <c r="B36" s="27" t="s">
+      <c r="B36" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="C36" s="27" t="s">
+      <c r="C36" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="D36" s="30" t="s">
+      <c r="D36" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="E36" s="27" t="s">
+      <c r="E36" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="F36" s="34" t="s">
+      <c r="F36" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="G36" s="30" t="s">
+      <c r="G36" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="H36" s="34" t="s">
+      <c r="H36" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="I36" s="27" t="s">
+      <c r="I36" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J36" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="K36" s="16"/>
+      <c r="J36" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K36" s="23"/>
       <c r="L36" s="16"/>
       <c r="M36" s="16"/>
       <c r="N36" s="16"/>
@@ -2598,37 +3000,37 @@
       <c r="R36" s="16"/>
     </row>
     <row r="37" spans="1:18" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="29">
+      <c r="A37" s="25">
         <v>37</v>
       </c>
-      <c r="B37" s="27" t="s">
+      <c r="B37" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="C37" s="27" t="s">
+      <c r="C37" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="D37" s="30" t="s">
+      <c r="D37" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="E37" s="27" t="s">
+      <c r="E37" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="F37" s="34" t="s">
+      <c r="F37" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="G37" s="30" t="s">
+      <c r="G37" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="H37" s="34" t="s">
+      <c r="H37" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="I37" s="27" t="s">
+      <c r="I37" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J37" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="K37" s="16"/>
+      <c r="J37" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K37" s="23"/>
       <c r="L37" s="16"/>
       <c r="M37" s="16"/>
       <c r="N37" s="16"/>
@@ -2638,37 +3040,37 @@
       <c r="R37" s="16"/>
     </row>
     <row r="38" spans="1:18" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="29">
+      <c r="A38" s="25">
         <v>38</v>
       </c>
-      <c r="B38" s="27" t="s">
+      <c r="B38" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C38" s="27" t="s">
+      <c r="C38" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D38" s="30" t="s">
+      <c r="D38" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="E38" s="30" t="s">
+      <c r="E38" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="F38" s="34" t="s">
+      <c r="F38" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="G38" s="30" t="s">
+      <c r="G38" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="H38" s="35" t="s">
+      <c r="H38" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="I38" s="27" t="s">
+      <c r="I38" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="J38" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="K38" s="16"/>
+      <c r="J38" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K38" s="23"/>
       <c r="L38" s="16"/>
       <c r="M38" s="16"/>
       <c r="N38" s="16"/>
@@ -2678,37 +3080,37 @@
       <c r="R38" s="16"/>
     </row>
     <row r="39" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="27">
+      <c r="A39" s="23">
         <v>39</v>
       </c>
-      <c r="B39" s="27" t="s">
+      <c r="B39" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="C39" s="27" t="s">
+      <c r="C39" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="D39" s="30" t="s">
+      <c r="D39" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="E39" s="30" t="s">
+      <c r="E39" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="F39" s="34" t="s">
+      <c r="F39" s="30" t="s">
         <v>142</v>
       </c>
-      <c r="G39" s="30" t="s">
+      <c r="G39" s="26" t="s">
+        <v>231</v>
+      </c>
+      <c r="H39" s="30" t="s">
         <v>143</v>
       </c>
-      <c r="H39" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="I39" s="27" t="s">
+      <c r="I39" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J39" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="K39" s="16"/>
+      <c r="J39" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K39" s="23"/>
       <c r="L39" s="16"/>
       <c r="M39" s="16"/>
       <c r="N39" s="16"/>
@@ -2718,37 +3120,37 @@
       <c r="R39" s="16"/>
     </row>
     <row r="40" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="27">
+      <c r="A40" s="23">
         <v>40</v>
       </c>
-      <c r="B40" s="27" t="s">
+      <c r="B40" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="C40" s="27" t="s">
+      <c r="C40" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="D40" s="30" t="s">
+      <c r="D40" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="E40" s="30" t="s">
+      <c r="E40" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="F40" s="34" t="s">
-        <v>147</v>
+      <c r="F40" s="30" t="s">
+        <v>145</v>
       </c>
       <c r="G40" s="30" t="s">
-        <v>145</v>
-      </c>
-      <c r="H40" s="34" t="s">
-        <v>146</v>
-      </c>
-      <c r="I40" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="H40" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="I40" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J40" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="K40" s="16"/>
+      <c r="J40" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K40" s="23"/>
       <c r="L40" s="16"/>
       <c r="M40" s="16"/>
       <c r="N40" s="16"/>
@@ -2758,37 +3160,37 @@
       <c r="R40" s="16"/>
     </row>
     <row r="41" spans="1:18" ht="75" x14ac:dyDescent="0.25">
-      <c r="A41" s="27">
+      <c r="A41" s="23">
         <v>41</v>
       </c>
-      <c r="B41" s="27" t="s">
+      <c r="B41" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="C41" s="27" t="s">
-        <v>148</v>
-      </c>
-      <c r="D41" s="30" t="s">
+      <c r="C41" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="D41" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="E41" s="27" t="s">
-        <v>148</v>
-      </c>
-      <c r="F41" s="34" t="s">
-        <v>149</v>
-      </c>
-      <c r="G41" s="30" t="s">
-        <v>214</v>
-      </c>
-      <c r="H41" s="34" t="s">
-        <v>219</v>
-      </c>
-      <c r="I41" s="27" t="s">
+      <c r="E41" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="F41" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="G41" s="26" t="s">
+        <v>212</v>
+      </c>
+      <c r="H41" s="30" t="s">
+        <v>217</v>
+      </c>
+      <c r="I41" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J41" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="K41" s="16"/>
+      <c r="J41" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K41" s="23"/>
       <c r="L41" s="16"/>
       <c r="M41" s="16"/>
       <c r="N41" s="16"/>
@@ -2798,37 +3200,37 @@
       <c r="R41" s="16"/>
     </row>
     <row r="42" spans="1:18" ht="75" x14ac:dyDescent="0.25">
-      <c r="A42" s="27">
+      <c r="A42" s="23">
         <v>42</v>
       </c>
-      <c r="B42" s="27" t="s">
+      <c r="B42" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="C42" s="27" t="s">
-        <v>150</v>
-      </c>
-      <c r="D42" s="30" t="s">
+      <c r="C42" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="D42" s="26" t="s">
+        <v>218</v>
+      </c>
+      <c r="E42" s="23" t="s">
+        <v>219</v>
+      </c>
+      <c r="F42" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="G42" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="H42" s="30" t="s">
         <v>220</v>
       </c>
-      <c r="E42" s="27" t="s">
-        <v>221</v>
-      </c>
-      <c r="F42" s="34" t="s">
-        <v>151</v>
-      </c>
-      <c r="G42" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="H42" s="34" t="s">
-        <v>222</v>
-      </c>
-      <c r="I42" s="27" t="s">
+      <c r="I42" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J42" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="K42" s="16"/>
+      <c r="J42" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K42" s="23"/>
       <c r="L42" s="16"/>
       <c r="M42" s="16"/>
       <c r="N42" s="16"/>
@@ -2838,37 +3240,37 @@
       <c r="R42" s="16"/>
     </row>
     <row r="43" spans="1:18" ht="60" x14ac:dyDescent="0.25">
-      <c r="A43" s="27">
+      <c r="A43" s="23">
         <v>43</v>
       </c>
-      <c r="B43" s="27" t="s">
+      <c r="B43" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="C43" s="27" t="s">
-        <v>156</v>
-      </c>
-      <c r="D43" s="30" t="s">
+      <c r="C43" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="D43" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="E43" s="27" t="s">
-        <v>216</v>
-      </c>
-      <c r="F43" s="34" t="s">
-        <v>152</v>
-      </c>
-      <c r="G43" s="30" t="s">
+      <c r="E43" s="23" t="s">
         <v>214</v>
       </c>
-      <c r="H43" s="34" t="s">
-        <v>223</v>
-      </c>
-      <c r="I43" s="27" t="s">
+      <c r="F43" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="G43" s="26" t="s">
+        <v>212</v>
+      </c>
+      <c r="H43" s="30" t="s">
+        <v>221</v>
+      </c>
+      <c r="I43" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J43" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="K43" s="16"/>
+      <c r="J43" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K43" s="23"/>
       <c r="L43" s="16"/>
       <c r="M43" s="16"/>
       <c r="N43" s="16"/>
@@ -2878,37 +3280,37 @@
       <c r="R43" s="16"/>
     </row>
     <row r="44" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="27">
+      <c r="A44" s="23">
         <v>44</v>
       </c>
-      <c r="B44" s="27" t="s">
+      <c r="B44" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="C44" s="27" t="s">
-        <v>155</v>
-      </c>
-      <c r="D44" s="30" t="s">
-        <v>215</v>
-      </c>
-      <c r="E44" s="27" t="s">
-        <v>216</v>
-      </c>
-      <c r="F44" s="34" t="s">
+      <c r="C44" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="G44" s="30" t="s">
+      <c r="D44" s="26" t="s">
+        <v>213</v>
+      </c>
+      <c r="E44" s="23" t="s">
         <v>214</v>
       </c>
-      <c r="H44" s="34" t="s">
-        <v>213</v>
-      </c>
-      <c r="I44" s="27" t="s">
+      <c r="F44" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="G44" s="26" t="s">
+        <v>212</v>
+      </c>
+      <c r="H44" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="I44" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J44" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="K44" s="16"/>
+      <c r="J44" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K44" s="23"/>
       <c r="L44" s="16"/>
       <c r="M44" s="16"/>
       <c r="N44" s="16"/>
@@ -2918,37 +3320,37 @@
       <c r="R44" s="16"/>
     </row>
     <row r="45" spans="1:18" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="27">
+      <c r="A45" s="23">
         <v>45</v>
       </c>
-      <c r="B45" s="27" t="s">
+      <c r="B45" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="C45" s="27" t="s">
-        <v>158</v>
-      </c>
-      <c r="D45" s="30" t="s">
-        <v>206</v>
-      </c>
-      <c r="E45" s="27" t="s">
+      <c r="C45" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="D45" s="26" t="s">
+        <v>204</v>
+      </c>
+      <c r="E45" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="F45" s="34" t="s">
-        <v>154</v>
-      </c>
-      <c r="G45" s="30" t="s">
+      <c r="F45" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="G45" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="H45" s="34" t="s">
-        <v>205</v>
-      </c>
-      <c r="I45" s="27" t="s">
+      <c r="H45" s="30" t="s">
+        <v>203</v>
+      </c>
+      <c r="I45" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J45" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="K45" s="16"/>
+      <c r="J45" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K45" s="23"/>
       <c r="L45" s="16"/>
       <c r="M45" s="16"/>
       <c r="N45" s="16"/>
@@ -2958,37 +3360,37 @@
       <c r="R45" s="16"/>
     </row>
     <row r="46" spans="1:18" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="27">
+      <c r="A46" s="23">
         <v>46</v>
       </c>
-      <c r="B46" s="27" t="s">
+      <c r="B46" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="C46" s="27" t="s">
+      <c r="C46" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="D46" s="26" t="s">
+        <v>201</v>
+      </c>
+      <c r="E46" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="F46" s="30" t="s">
         <v>157</v>
       </c>
-      <c r="D46" s="30" t="s">
-        <v>203</v>
-      </c>
-      <c r="E46" s="27" t="s">
+      <c r="G46" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="F46" s="34" t="s">
-        <v>159</v>
-      </c>
-      <c r="G46" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="H46" s="34" t="s">
-        <v>204</v>
-      </c>
-      <c r="I46" s="27" t="s">
+      <c r="H46" s="30" t="s">
+        <v>202</v>
+      </c>
+      <c r="I46" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J46" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="K46" s="16"/>
+      <c r="J46" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K46" s="23"/>
       <c r="L46" s="16"/>
       <c r="M46" s="16"/>
       <c r="N46" s="16"/>
@@ -2998,37 +3400,37 @@
       <c r="R46" s="16"/>
     </row>
     <row r="47" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A47" s="27">
+      <c r="A47" s="23">
         <v>47</v>
       </c>
-      <c r="B47" s="27" t="s">
+      <c r="B47" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="C47" s="27" t="s">
-        <v>160</v>
-      </c>
-      <c r="D47" s="30" t="s">
-        <v>185</v>
-      </c>
-      <c r="E47" s="27" t="s">
+      <c r="C47" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="D47" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="E47" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="F47" s="34" t="s">
-        <v>161</v>
-      </c>
-      <c r="G47" s="30" t="s">
+      <c r="F47" s="30" t="s">
+        <v>159</v>
+      </c>
+      <c r="G47" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="H47" s="34" t="s">
-        <v>186</v>
-      </c>
-      <c r="I47" s="27" t="s">
+      <c r="H47" s="30" t="s">
+        <v>184</v>
+      </c>
+      <c r="I47" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J47" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="K47" s="16"/>
+      <c r="J47" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K47" s="23"/>
       <c r="L47" s="16"/>
       <c r="M47" s="16"/>
       <c r="N47" s="16"/>
@@ -3038,37 +3440,37 @@
       <c r="R47" s="16"/>
     </row>
     <row r="48" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="27">
+      <c r="A48" s="23">
         <v>48</v>
       </c>
-      <c r="B48" s="27" t="s">
+      <c r="B48" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="C48" s="27" t="s">
-        <v>162</v>
-      </c>
-      <c r="D48" s="30" t="s">
-        <v>185</v>
-      </c>
-      <c r="E48" s="27" t="s">
+      <c r="C48" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="D48" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="E48" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="F48" s="34" t="s">
-        <v>163</v>
-      </c>
-      <c r="G48" s="30" t="s">
+      <c r="F48" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="G48" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="H48" s="34" t="s">
-        <v>184</v>
-      </c>
-      <c r="I48" s="27" t="s">
+      <c r="H48" s="30" t="s">
+        <v>182</v>
+      </c>
+      <c r="I48" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J48" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="K48" s="16"/>
+      <c r="J48" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K48" s="23"/>
       <c r="L48" s="16"/>
       <c r="M48" s="16"/>
       <c r="N48" s="16"/>
@@ -3078,37 +3480,37 @@
       <c r="R48" s="16"/>
     </row>
     <row r="49" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A49" s="27">
+      <c r="A49" s="23">
         <v>49</v>
       </c>
-      <c r="B49" s="27" t="s">
+      <c r="B49" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="C49" s="27" t="s">
+      <c r="C49" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="D49" s="26" t="s">
+        <v>197</v>
+      </c>
+      <c r="E49" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="F49" s="30" t="s">
         <v>164</v>
       </c>
-      <c r="D49" s="30" t="s">
-        <v>199</v>
-      </c>
-      <c r="E49" s="27" t="s">
+      <c r="G49" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="F49" s="34" t="s">
-        <v>166</v>
-      </c>
-      <c r="G49" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="H49" s="34" t="s">
-        <v>200</v>
-      </c>
-      <c r="I49" s="27" t="s">
+      <c r="H49" s="30" t="s">
+        <v>198</v>
+      </c>
+      <c r="I49" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J49" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="K49" s="16"/>
+      <c r="J49" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K49" s="23"/>
       <c r="L49" s="16"/>
       <c r="M49" s="16"/>
       <c r="N49" s="16"/>
@@ -3118,37 +3520,37 @@
       <c r="R49" s="16"/>
     </row>
     <row r="50" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A50" s="27">
-        <v>50</v>
-      </c>
-      <c r="B50" s="27" t="s">
+      <c r="A50" s="23">
+        <v>50</v>
+      </c>
+      <c r="B50" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="C50" s="27" t="s">
+      <c r="C50" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="D50" s="26" t="s">
+        <v>197</v>
+      </c>
+      <c r="E50" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="F50" s="30" t="s">
         <v>165</v>
       </c>
-      <c r="D50" s="30" t="s">
+      <c r="G50" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="H50" s="30" t="s">
         <v>199</v>
       </c>
-      <c r="E50" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="F50" s="34" t="s">
-        <v>167</v>
-      </c>
-      <c r="G50" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="H50" s="34" t="s">
-        <v>201</v>
-      </c>
-      <c r="I50" s="27" t="s">
+      <c r="I50" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J50" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="K50" s="16"/>
+      <c r="J50" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K50" s="23"/>
       <c r="L50" s="16"/>
       <c r="M50" s="16"/>
       <c r="N50" s="16"/>
@@ -3158,37 +3560,37 @@
       <c r="R50" s="16"/>
     </row>
     <row r="51" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A51" s="27">
+      <c r="A51" s="23">
         <v>51</v>
       </c>
-      <c r="B51" s="27" t="s">
+      <c r="B51" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="C51" s="27" t="s">
-        <v>169</v>
-      </c>
-      <c r="D51" s="30" t="s">
-        <v>210</v>
-      </c>
-      <c r="E51" s="27" t="s">
+      <c r="C51" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="D51" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="E51" s="23" t="s">
+        <v>205</v>
+      </c>
+      <c r="F51" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="G51" s="26" t="s">
         <v>207</v>
       </c>
-      <c r="F51" s="34" t="s">
-        <v>168</v>
-      </c>
-      <c r="G51" s="30" t="s">
-        <v>209</v>
-      </c>
-      <c r="H51" s="34" t="s">
-        <v>208</v>
-      </c>
-      <c r="I51" s="27" t="s">
+      <c r="H51" s="30" t="s">
+        <v>206</v>
+      </c>
+      <c r="I51" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J51" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="K51" s="16"/>
+      <c r="J51" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K51" s="23"/>
       <c r="L51" s="16"/>
       <c r="M51" s="16"/>
       <c r="N51" s="16"/>
@@ -3198,37 +3600,37 @@
       <c r="R51" s="16"/>
     </row>
     <row r="52" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A52" s="27">
+      <c r="A52" s="23">
         <v>52</v>
       </c>
-      <c r="B52" s="27" t="s">
+      <c r="B52" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="C52" s="27" t="s">
-        <v>170</v>
-      </c>
-      <c r="D52" s="30" t="s">
-        <v>211</v>
-      </c>
-      <c r="E52" s="27" t="s">
-        <v>193</v>
-      </c>
-      <c r="F52" s="34" t="s">
-        <v>171</v>
-      </c>
-      <c r="G52" s="27" t="s">
+      <c r="C52" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="D52" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="E52" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="F52" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="G52" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="H52" s="34" t="s">
-        <v>194</v>
-      </c>
-      <c r="I52" s="27" t="s">
+      <c r="H52" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="I52" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J52" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="K52" s="16"/>
+      <c r="J52" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K52" s="23"/>
       <c r="L52" s="16"/>
       <c r="M52" s="16"/>
       <c r="N52" s="16"/>
@@ -3238,37 +3640,37 @@
       <c r="R52" s="16"/>
     </row>
     <row r="53" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="27">
+      <c r="A53" s="23">
         <v>53</v>
       </c>
-      <c r="B53" s="27" t="s">
+      <c r="B53" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="C53" s="27" t="s">
-        <v>172</v>
-      </c>
-      <c r="D53" s="30" t="s">
-        <v>211</v>
-      </c>
-      <c r="E53" s="27" t="s">
-        <v>189</v>
-      </c>
-      <c r="F53" s="34" t="s">
-        <v>173</v>
-      </c>
-      <c r="G53" s="30" t="s">
-        <v>188</v>
-      </c>
-      <c r="H53" s="34" t="s">
+      <c r="C53" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="D53" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="E53" s="23" t="s">
         <v>187</v>
       </c>
-      <c r="I53" s="27" t="s">
+      <c r="F53" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="G53" s="26" t="s">
+        <v>186</v>
+      </c>
+      <c r="H53" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="I53" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J53" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="K53" s="16"/>
+      <c r="J53" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K53" s="23"/>
       <c r="L53" s="16"/>
       <c r="M53" s="16"/>
       <c r="N53" s="16"/>
@@ -3278,37 +3680,37 @@
       <c r="R53" s="16"/>
     </row>
     <row r="54" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="27">
+      <c r="A54" s="23">
         <v>54</v>
       </c>
-      <c r="B54" s="27" t="s">
+      <c r="B54" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="C54" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="D54" s="30" t="s">
-        <v>211</v>
-      </c>
-      <c r="E54" s="27" t="s">
+      <c r="C54" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="D54" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="E54" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="F54" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="G54" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="H54" s="30" t="s">
         <v>190</v>
       </c>
-      <c r="F54" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="G54" s="30" t="s">
-        <v>191</v>
-      </c>
-      <c r="H54" s="34" t="s">
-        <v>192</v>
-      </c>
-      <c r="I54" s="27" t="s">
+      <c r="I54" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J54" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="K54" s="16"/>
+      <c r="J54" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K54" s="23"/>
       <c r="L54" s="16"/>
       <c r="M54" s="16"/>
       <c r="N54" s="16"/>
@@ -3318,37 +3720,37 @@
       <c r="R54" s="16"/>
     </row>
     <row r="55" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="A55" s="27">
+      <c r="A55" s="23">
         <v>55</v>
       </c>
-      <c r="B55" s="27" t="s">
+      <c r="B55" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="C55" s="27" t="s">
-        <v>176</v>
-      </c>
-      <c r="D55" s="30" t="s">
-        <v>227</v>
-      </c>
-      <c r="E55" s="27" t="s">
-        <v>226</v>
-      </c>
-      <c r="F55" s="34" t="s">
-        <v>177</v>
-      </c>
-      <c r="G55" s="30" t="s">
+      <c r="C55" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="D55" s="26" t="s">
         <v>225</v>
       </c>
-      <c r="H55" s="34" t="s">
+      <c r="E55" s="23" t="s">
         <v>224</v>
       </c>
-      <c r="I55" s="27" t="s">
+      <c r="F55" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="G55" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="H55" s="30" t="s">
+        <v>222</v>
+      </c>
+      <c r="I55" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J55" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="K55" s="16"/>
+      <c r="J55" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K55" s="23"/>
       <c r="L55" s="16"/>
       <c r="M55" s="16"/>
       <c r="N55" s="16"/>
@@ -3358,37 +3760,37 @@
       <c r="R55" s="16"/>
     </row>
     <row r="56" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="27">
+      <c r="A56" s="23">
         <v>56</v>
       </c>
-      <c r="B56" s="27" t="s">
+      <c r="B56" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="C56" s="27" t="s">
+      <c r="C56" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="D56" s="26" t="s">
+        <v>195</v>
+      </c>
+      <c r="E56" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="F56" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="G56" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="H56" s="30" t="s">
+        <v>196</v>
+      </c>
+      <c r="I56" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="J56" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="D56" s="30" t="s">
-        <v>197</v>
-      </c>
-      <c r="E56" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="F56" s="34" t="s">
-        <v>179</v>
-      </c>
-      <c r="G56" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="H56" s="34" t="s">
-        <v>198</v>
-      </c>
-      <c r="I56" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="J56" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="K56" s="16"/>
+      <c r="K56" s="23"/>
       <c r="L56" s="16"/>
       <c r="M56" s="16"/>
       <c r="N56" s="16"/>
@@ -3398,98 +3800,101 @@
       <c r="R56" s="16"/>
     </row>
     <row r="57" spans="1:18" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A57" s="29">
+      <c r="A57" s="25">
         <v>57</v>
       </c>
-      <c r="B57" s="27" t="s">
+      <c r="B57" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C57" s="27" t="s">
+      <c r="C57" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D57" s="30" t="s">
-        <v>212</v>
-      </c>
-      <c r="E57" s="27" t="s">
+      <c r="D57" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="E57" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="F57" s="34" t="s">
-        <v>195</v>
-      </c>
-      <c r="G57" s="30" t="s">
+      <c r="F57" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="G57" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="H57" s="34" t="s">
+      <c r="H57" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="I57" s="27" t="s">
+      <c r="I57" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="J57" s="27" t="s">
-        <v>180</v>
-      </c>
+      <c r="J57" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K57" s="23"/>
     </row>
     <row r="58" spans="1:18" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="29">
+      <c r="A58" s="25">
         <v>58</v>
       </c>
-      <c r="B58" s="27" t="s">
+      <c r="B58" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C58" s="27" t="s">
+      <c r="C58" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D58" s="30" t="s">
+      <c r="D58" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="E58" s="27" t="s">
-        <v>190</v>
-      </c>
-      <c r="F58" s="34" t="s">
-        <v>217</v>
-      </c>
-      <c r="G58" s="30" t="s">
+      <c r="E58" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="F58" s="30" t="s">
+        <v>215</v>
+      </c>
+      <c r="G58" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="H58" s="34" t="s">
-        <v>218</v>
-      </c>
-      <c r="I58" s="27" t="s">
+      <c r="H58" s="30" t="s">
+        <v>216</v>
+      </c>
+      <c r="I58" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="J58" s="27" t="s">
-        <v>180</v>
-      </c>
+      <c r="J58" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="K58" s="23"/>
     </row>
     <row r="59" spans="1:18" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A59" s="29">
+      <c r="A59" s="25">
         <v>59</v>
       </c>
-      <c r="B59" s="27" t="s">
+      <c r="B59" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C59" s="27" t="s">
+      <c r="C59" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D59" s="30" t="s">
+      <c r="D59" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="E59" s="27" t="s">
+      <c r="E59" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="F59" s="34" t="s">
-        <v>228</v>
-      </c>
-      <c r="G59" s="30" t="s">
+      <c r="F59" s="30" t="s">
+        <v>226</v>
+      </c>
+      <c r="G59" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="H59" s="34" t="s">
-        <v>229</v>
-      </c>
-      <c r="I59" s="27" t="s">
+      <c r="H59" s="30" t="s">
+        <v>227</v>
+      </c>
+      <c r="I59" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="J59" s="27"/>
+      <c r="J59" s="23"/>
+      <c r="K59" s="23"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I24"/>
@@ -3503,12 +3908,12 @@
   <dimension ref="A1:M58"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19" style="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19" style="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="77.140625" style="1" customWidth="1"/>
     <col min="4" max="5" width="9.140625" bestFit="1" customWidth="1"/>
@@ -3627,9 +4032,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
-      <c r="M3" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="M3" s="2"/>
     </row>
     <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
@@ -3652,9 +4055,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
-      <c r="M4" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
@@ -5117,7 +5518,7 @@
         <f>'Controleur CA'!B48</f>
         <v>Complétude</v>
       </c>
-      <c r="C48" s="23" t="str">
+      <c r="C48" s="20" t="str">
         <f>'Controleur CA'!F48</f>
         <v>Vérifier que le répertoire PROJET_QGIS contient un fichier contenant le nom Plan_tirage au format pdf</v>
       </c>
@@ -5217,7 +5618,7 @@
         <f>'Controleur CA'!B52</f>
         <v>Complétude</v>
       </c>
-      <c r="C52" s="24" t="str">
+      <c r="C52" s="21" t="str">
         <f>'Controleur CA'!F52</f>
         <v>Vérifier que le répertoire n'est pas vide s'il y a des point technique dont Enedis est le propriétaire</v>
       </c>
@@ -7016,7 +7417,7 @@
         <f>'Controleur CA'!B48</f>
         <v>Complétude</v>
       </c>
-      <c r="C48" s="23" t="str">
+      <c r="C48" s="20" t="str">
         <f>'Controleur CA'!F48</f>
         <v>Vérifier que le répertoire PROJET_QGIS contient un fichier contenant le nom Plan_tirage au format pdf</v>
       </c>
@@ -7108,7 +7509,7 @@
         <f>'Controleur CA'!B52</f>
         <v>Complétude</v>
       </c>
-      <c r="C52" s="24" t="str">
+      <c r="C52" s="21" t="str">
         <f>'Controleur CA'!F52</f>
         <v>Vérifier que le répertoire n'est pas vide s'il y a des point technique dont Enedis est le propriétaire</v>
       </c>
@@ -8878,7 +9279,7 @@
         <f>'Controleur CA'!B48</f>
         <v>Complétude</v>
       </c>
-      <c r="C48" s="23" t="str">
+      <c r="C48" s="20" t="str">
         <f>'Controleur CA'!F48</f>
         <v>Vérifier que le répertoire PROJET_QGIS contient un fichier contenant le nom Plan_tirage au format pdf</v>
       </c>
@@ -8970,7 +9371,7 @@
         <f>'Controleur CA'!B52</f>
         <v>Complétude</v>
       </c>
-      <c r="C52" s="24" t="str">
+      <c r="C52" s="21" t="str">
         <f>'Controleur CA'!F52</f>
         <v>Vérifier que le répertoire n'est pas vide s'il y a des point technique dont Enedis est le propriétaire</v>
       </c>
@@ -10739,7 +11140,7 @@
         <f>'Controleur CA'!B48</f>
         <v>Complétude</v>
       </c>
-      <c r="C48" s="23" t="str">
+      <c r="C48" s="20" t="str">
         <f>'Controleur CA'!F48</f>
         <v>Vérifier que le répertoire PROJET_QGIS contient un fichier contenant le nom Plan_tirage au format pdf</v>
       </c>
@@ -10831,7 +11232,7 @@
         <f>'Controleur CA'!B52</f>
         <v>Complétude</v>
       </c>
-      <c r="C52" s="24" t="str">
+      <c r="C52" s="21" t="str">
         <f>'Controleur CA'!F52</f>
         <v>Vérifier que le répertoire n'est pas vide s'il y a des point technique dont Enedis est le propriétaire</v>
       </c>
@@ -12601,7 +13002,7 @@
         <f>'Controleur CA'!B48</f>
         <v>Complétude</v>
       </c>
-      <c r="C48" s="23" t="str">
+      <c r="C48" s="20" t="str">
         <f>'Controleur CA'!F48</f>
         <v>Vérifier que le répertoire PROJET_QGIS contient un fichier contenant le nom Plan_tirage au format pdf</v>
       </c>
@@ -12693,7 +13094,7 @@
         <f>'Controleur CA'!B52</f>
         <v>Complétude</v>
       </c>
-      <c r="C52" s="24" t="str">
+      <c r="C52" s="21" t="str">
         <f>'Controleur CA'!F52</f>
         <v>Vérifier que le répertoire n'est pas vide s'il y a des point technique dont Enedis est le propriétaire</v>
       </c>
@@ -12893,10 +13294,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C9:F15"/>
+  <dimension ref="C8:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12904,45 +13305,54 @@
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C9" s="20" t="s">
+    <row r="8" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="3:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>182</v>
-      </c>
-      <c r="F9" s="20" t="s">
+      <c r="D9" s="39" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C10" s="19" t="s">
+      <c r="E9" s="37" t="s">
+        <v>180</v>
+      </c>
+      <c r="F9" s="37" t="s">
+        <v>230</v>
+      </c>
+      <c r="G9" s="38" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="40">
         <f>COUNTIF('Controleur CA'!B:B,Synthèse!C10)</f>
         <v>28</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="35">
         <f>IF(ISERROR(SUMPRODUCT(('Controleur CA'!J:J="fait")*('Controleur CA'!B:B=C10))),"Aucun",SUMPRODUCT(('Controleur CA'!J:J="fait")*('Controleur CA'!B:B=C10)))</f>
         <v>27</v>
       </c>
-      <c r="F10" s="21">
-        <f>E10/D10*100</f>
-        <v>96.428571428571431</v>
-      </c>
-    </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C11" s="19" t="s">
+      <c r="F10" s="35">
+        <f>IF(ISERROR(SUMPRODUCT(('Controleur CA'!K:K="x")*('Controleur CA'!B:B=D10))),"Aucun",SUMPRODUCT(('Controleur CA'!K:K="x")*('Controleur CA'!B:B=C10)))</f>
+        <v>4</v>
+      </c>
+      <c r="G10" s="55">
+        <f>E10/D10</f>
+        <v>0.9642857142857143</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C11" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="41">
         <f>COUNTIF('Controleur CA'!B:B,Synthèse!C11)</f>
         <v>12</v>
       </c>
@@ -12950,64 +13360,138 @@
         <f>IF(ISERROR(SUMPRODUCT(('Controleur CA'!J:J="fait")*('Controleur CA'!B:B=C11))),"Aucun",SUMPRODUCT(('Controleur CA'!J:J="fait")*('Controleur CA'!B:B=C11)))</f>
         <v>12</v>
       </c>
-      <c r="F11" s="21">
-        <f>E11/D11*100</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C12" s="19" t="s">
+      <c r="F11" s="17">
+        <f>IF(ISERROR(SUMPRODUCT(('Controleur CA'!K:K="x")*('Controleur CA'!B:B=D11))),"Aucun",SUMPRODUCT(('Controleur CA'!K:K="x")*('Controleur CA'!B:B=C11)))</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="56">
+        <f>E11/D11</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="48" t="s">
         <v>139</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="42">
         <f>COUNTIF('Controleur CA'!B:B,Synthèse!C12)</f>
         <v>18</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="36">
         <f>IF(ISERROR(SUMPRODUCT(('Controleur CA'!J:J="fait")*('Controleur CA'!B:B=C12))),"Aucun",SUMPRODUCT(('Controleur CA'!J:J="fait")*('Controleur CA'!B:B=C12)))</f>
         <v>18</v>
       </c>
-      <c r="F12" s="21">
-        <f>E12/D12*100</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C13" s="19" t="s">
-        <v>196</v>
-      </c>
-      <c r="D13" s="17">
+      <c r="F12" s="36">
+        <f>IF(ISERROR(SUMPRODUCT(('Controleur CA'!K:K="x")*('Controleur CA'!B:B=D12))),"Aucun",SUMPRODUCT(('Controleur CA'!K:K="x")*('Controleur CA'!B:B=C12)))</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="57">
+        <f>E12/D12</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="49"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="58"/>
+    </row>
+    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C14" s="50" t="s">
+        <v>194</v>
+      </c>
+      <c r="D14" s="40">
         <f>D10+D11+D12</f>
         <v>58</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E14" s="35">
         <f>E10+E11+E12</f>
         <v>57</v>
       </c>
-      <c r="F13" s="21">
-        <f>(F10+F11+F12)/3</f>
-        <v>98.80952380952381</v>
-      </c>
-    </row>
-    <row r="15" spans="3:6" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="25" t="s">
-        <v>202</v>
-      </c>
-      <c r="D15" s="37" t="s">
-        <v>230</v>
-      </c>
-      <c r="E15" s="38"/>
-      <c r="F15" s="39"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="55">
+        <f>(G10+G11+G12)/3</f>
+        <v>0.98809523809523814</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="51" t="s">
+        <v>229</v>
+      </c>
+      <c r="D15" s="42">
+        <f>D14</f>
+        <v>58</v>
+      </c>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36">
+        <f>F12+F11+F10</f>
+        <v>4</v>
+      </c>
+      <c r="G15" s="57">
+        <f>(E14-F15)/E14</f>
+        <v>0.92982456140350878</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="49"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="58"/>
+    </row>
+    <row r="17" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="52" t="s">
+        <v>194</v>
+      </c>
+      <c r="D17" s="44">
+        <f>D14</f>
+        <v>58</v>
+      </c>
+      <c r="E17" s="33">
+        <f>E14</f>
+        <v>57</v>
+      </c>
+      <c r="F17" s="54">
+        <f>F15</f>
+        <v>4</v>
+      </c>
+      <c r="G17" s="59">
+        <f>(G14+G15)/2</f>
+        <v>0.95895989974937346</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="3:7" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="53" t="s">
+        <v>200</v>
+      </c>
+      <c r="D19" s="60" t="s">
+        <v>232</v>
+      </c>
+      <c r="E19" s="61"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D19:G19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document Microsoft Word" ma:contentTypeID="0x01010066910ADB61686C45A75A7A744D7D5C8E0022B63E0AEFBB2040BF2A3B1B4BE32EE5" ma:contentTypeVersion="4" ma:contentTypeDescription="Document Microsoft Word vierge." ma:contentTypeScope="" ma:versionID="0a4943d90c7214e3c95a70ccb3c8346b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c97f8e9-86c7-4e99-9925-cc9540b321fe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eeaa8661ba6ba22f90735bcd04aade41" ns2:_="">
     <xsd:import namespace="9c97f8e9-86c7-4e99-9925-cc9540b321fe"/>
@@ -13210,15 +13694,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -13234,6 +13709,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F02C15CB-09E5-4D58-8C63-77232C75BB18}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8B2112A-C178-4B00-8690-1CA741C188F5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13247,14 +13730,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F02C15CB-09E5-4D58-8C63-77232C75BB18}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
- Ajout du fichier python contenant la nouvelle classe InternalException
- Ajout d'une exception custom "InternalException" permettant de créer une alerte d'erreur dans des sous fonctions puis provoquer cette exception qui sera catchée au plus haut, donc dans controleur_param.py afin de stopper les controles ET ne pas déclancher des erreurs en chaine

- Suppression de code inutilisé

- Création de "find_fichier_format" créée à partir de tous les contrôles qui cherches un fichier ou dossier par le format et chemin du xml selon des conditions mutualisables
Ainsi, toutes ces fonctions appellent une unique fonction paramétrable permettant de convenir à tous les tests et donc centraliser le code, et permettre plus facilement l'ajout de nouvelles fonctions

- Gestion de l'exception pour les contrôles 2 et 3, dans le cas où des champs sont manquants, en passant par le novueau système de l'exception InternalException après avoir lancé la fonction log.
</commit_message>
<xml_diff>
--- a/Documentation/Controleur.xlsx
+++ b/Documentation/Controleur.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="8370" yWindow="1320" windowWidth="6915" windowHeight="6540" activeTab="6"/>
+    <workbookView xWindow="8370" yWindow="1320" windowWidth="6915" windowHeight="6540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Controleur CA" sheetId="1" r:id="rId1"/>
@@ -703,9 +703,6 @@
     <t xml:space="preserve">[Couche Point technique / Couche Infrastructure] </t>
   </si>
   <si>
-    <t>Vérifier que la colonne C et la colonne F contiennent un nom de point technique  respectant les normes Orange</t>
-  </si>
-  <si>
     <t>Format de nommage du numéro de point technique incorrect</t>
   </si>
   <si>
@@ -722,6 +719,9 @@
   </si>
   <si>
     <t>J'ai ajouté de nouveaux contrôles à réaliser après étude des specifications Orange + refonte prévue des contrôles + gestion des cas particuliers + stabilité programme (optimisation, commentaires,…?) + nouveau système de gestion et affichage des erreurs</t>
+  </si>
+  <si>
+    <t>Vérifier que la colonne C et la colonne F contiennent un nom de point technique  respectant les normes Orange (numerique ou FT / AE)</t>
   </si>
 </sst>
 </file>
@@ -1717,8 +1717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R59"/>
   <sheetViews>
-    <sheetView topLeftCell="E7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1770,7 +1770,7 @@
         <v>138</v>
       </c>
       <c r="K1" s="29" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3099,7 +3099,7 @@
         <v>142</v>
       </c>
       <c r="G39" s="26" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H39" s="30" t="s">
         <v>143</v>
@@ -3865,7 +3865,7 @@
       </c>
       <c r="K58" s="23"/>
     </row>
-    <row r="59" spans="1:18" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" s="16" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" s="25">
         <v>59</v>
       </c>
@@ -3882,13 +3882,13 @@
         <v>57</v>
       </c>
       <c r="F59" s="30" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="G59" s="26" t="s">
         <v>53</v>
       </c>
       <c r="H59" s="30" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I59" s="23" t="s">
         <v>36</v>
@@ -3907,8 +3907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M58"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13296,7 +13296,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C8:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -13321,7 +13321,7 @@
         <v>180</v>
       </c>
       <c r="F9" s="37" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G9" s="38" t="s">
         <v>179</v>
@@ -13417,7 +13417,7 @@
     </row>
     <row r="15" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="51" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D15" s="42">
         <f>D14</f>
@@ -13467,7 +13467,7 @@
         <v>200</v>
       </c>
       <c r="D19" s="60" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E19" s="61"/>
       <c r="F19" s="61"/>
@@ -13483,15 +13483,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document Microsoft Word" ma:contentTypeID="0x01010066910ADB61686C45A75A7A744D7D5C8E0022B63E0AEFBB2040BF2A3B1B4BE32EE5" ma:contentTypeVersion="4" ma:contentTypeDescription="Document Microsoft Word vierge." ma:contentTypeScope="" ma:versionID="0a4943d90c7214e3c95a70ccb3c8346b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c97f8e9-86c7-4e99-9925-cc9540b321fe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eeaa8661ba6ba22f90735bcd04aade41" ns2:_="">
     <xsd:import namespace="9c97f8e9-86c7-4e99-9925-cc9540b321fe"/>
@@ -13694,6 +13685,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -13709,14 +13709,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F02C15CB-09E5-4D58-8C63-77232C75BB18}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8B2112A-C178-4B00-8690-1CA741C188F5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13730,6 +13722,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F02C15CB-09E5-4D58-8C63-77232C75BB18}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
- Ajout du chemin de la dll du module unrar dans la configuration.txt qui s'ajoute dans les variables d'environnement (dans le cas où on est amené à utiliser la lib, car sinon, plantage...) - Constatation que pour utiliser unrar, il faut donc la variable d'environnement dans le PC qui execute le programme (car fonction de verification dans une lib, lancé à l'execution) et avoir le fichier dll dans son PC - Retrait de la fonctionnalité de decompression de fichiers rar, trop compliquer à déployer en logiciel, à voir plus tard eventuellement si important - Correction du bug de "modele_erreur" qui récupérait pas les infos sous force de tableau - Passer les variables concernant la génération de l'erreur en tableaux et dictionnaires, avec simplification des étapes pour avoir le moins de traitement possible
</commit_message>
<xml_diff>
--- a/Documentation/Controleur.xlsx
+++ b/Documentation/Controleur.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="8370" yWindow="1320" windowWidth="6915" windowHeight="6540" activeTab="1"/>
+    <workbookView xWindow="8370" yWindow="1320" windowWidth="6915" windowHeight="6540" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Controleur CA" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1904" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1907" uniqueCount="237">
   <si>
     <t>Famille</t>
   </si>
@@ -718,17 +718,29 @@
     <t>[Couche]</t>
   </si>
   <si>
-    <t>J'ai ajouté de nouveaux contrôles à réaliser après étude des specifications Orange + refonte prévue des contrôles + gestion des cas particuliers + stabilité programme (optimisation, commentaires,…?) + nouveau système de gestion et affichage des erreurs</t>
-  </si>
-  <si>
     <t>Vérifier que la colonne C et la colonne F contiennent un nom de point technique  respectant les normes Orange (numerique ou FT / AE)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nb maintenances evolutives / correctives </t>
+  </si>
+  <si>
+    <t>Nb</t>
+  </si>
+  <si>
+    <t>Controles</t>
+  </si>
+  <si>
+    <t>Général</t>
+  </si>
+  <si>
+    <t>J'ai restructuré ce planning enfin de donner + de visibilité</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -760,8 +772,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -798,8 +817,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="33">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -1233,12 +1258,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1405,6 +1456,45 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="7" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1717,8 +1807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R59"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView topLeftCell="E40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K60" sqref="K60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1837,9 +1927,7 @@
       <c r="J3" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="K3" s="23" t="s">
-        <v>50</v>
-      </c>
+      <c r="K3" s="23"/>
     </row>
     <row r="4" spans="1:11" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="25">
@@ -1872,9 +1960,7 @@
       <c r="J4" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="K4" s="23" t="s">
-        <v>50</v>
-      </c>
+      <c r="K4" s="23"/>
     </row>
     <row r="5" spans="1:11" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="25">
@@ -2105,9 +2191,7 @@
       <c r="J11" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="K11" s="23" t="s">
-        <v>50</v>
-      </c>
+      <c r="K11" s="23"/>
     </row>
     <row r="12" spans="1:11" s="16" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="25">
@@ -2140,9 +2224,7 @@
       <c r="J12" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="K12" s="23" t="s">
-        <v>50</v>
-      </c>
+      <c r="K12" s="23"/>
     </row>
     <row r="13" spans="1:11" s="16" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="25">
@@ -3882,7 +3964,7 @@
         <v>57</v>
       </c>
       <c r="F59" s="30" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G59" s="26" t="s">
         <v>53</v>
@@ -3894,7 +3976,9 @@
         <v>36</v>
       </c>
       <c r="J59" s="23"/>
-      <c r="K59" s="23"/>
+      <c r="K59" s="23" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:I24"/>
@@ -3907,7 +3991,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
@@ -13294,23 +13378,30 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C8:G19"/>
+  <dimension ref="B8:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" customWidth="1"/>
+    <col min="3" max="3" width="39.85546875" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" customWidth="1"/>
+    <col min="9" max="9" width="40.42578125" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="3:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="2:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="69" t="s">
+        <v>234</v>
+      </c>
       <c r="C9" s="45" t="s">
         <v>0</v>
       </c>
@@ -13327,7 +13418,8 @@
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="70"/>
       <c r="C10" s="46" t="s">
         <v>7</v>
       </c>
@@ -13341,14 +13433,15 @@
       </c>
       <c r="F10" s="35">
         <f>IF(ISERROR(SUMPRODUCT(('Controleur CA'!K:K="x")*('Controleur CA'!B:B=D10))),"Aucun",SUMPRODUCT(('Controleur CA'!K:K="x")*('Controleur CA'!B:B=C10)))</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G10" s="55">
         <f>E10/D10</f>
         <v>0.9642857142857143</v>
       </c>
     </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="70"/>
       <c r="C11" s="47" t="s">
         <v>94</v>
       </c>
@@ -13369,7 +13462,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="70"/>
       <c r="C12" s="48" t="s">
         <v>139</v>
       </c>
@@ -13390,14 +13484,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="70"/>
       <c r="C13" s="49"/>
       <c r="D13" s="43"/>
       <c r="E13" s="34"/>
       <c r="F13" s="34"/>
       <c r="G13" s="58"/>
     </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="70"/>
       <c r="C14" s="50" t="s">
         <v>194</v>
       </c>
@@ -13415,7 +13511,8 @@
         <v>0.98809523809523814</v>
       </c>
     </row>
-    <row r="15" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="70"/>
       <c r="C15" s="51" t="s">
         <v>228</v>
       </c>
@@ -13426,21 +13523,23 @@
       <c r="E15" s="36"/>
       <c r="F15" s="36">
         <f>F12+F11+F10</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G15" s="57">
         <f>(E14-F15)/E14</f>
-        <v>0.92982456140350878</v>
-      </c>
-    </row>
-    <row r="16" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.98245614035087714</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="70"/>
       <c r="C16" s="49"/>
       <c r="D16" s="43"/>
       <c r="E16" s="34"/>
       <c r="F16" s="34"/>
       <c r="G16" s="58"/>
     </row>
-    <row r="17" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="71"/>
       <c r="C17" s="52" t="s">
         <v>194</v>
       </c>
@@ -13454,28 +13553,71 @@
       </c>
       <c r="F17" s="54">
         <f>F15</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G17" s="59">
         <f>(G14+G15)/2</f>
-        <v>0.95895989974937346</v>
-      </c>
-    </row>
-    <row r="18" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="3:7" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="53" t="s">
+        <v>0.98527568922305764</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="63"/>
+      <c r="D18" s="63"/>
+      <c r="E18" s="63"/>
+      <c r="F18" s="63"/>
+      <c r="G18" s="63"/>
+    </row>
+    <row r="19" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="2:7" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="69" t="s">
+        <v>235</v>
+      </c>
+      <c r="C20" s="65" t="s">
+        <v>232</v>
+      </c>
+      <c r="D20" s="66" t="s">
+        <v>233</v>
+      </c>
+      <c r="E20" s="67" t="s">
+        <v>180</v>
+      </c>
+      <c r="F20" s="75"/>
+      <c r="G20" s="72" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="71"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="33">
+        <v>48</v>
+      </c>
+      <c r="E21" s="73">
+        <v>19</v>
+      </c>
+      <c r="F21" s="74"/>
+      <c r="G21" s="68">
+        <f>E21/D21</f>
+        <v>0.39583333333333331</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="53" t="s">
         <v>200</v>
       </c>
-      <c r="D19" s="60" t="s">
-        <v>231</v>
-      </c>
-      <c r="E19" s="61"/>
-      <c r="F19" s="61"/>
-      <c r="G19" s="62"/>
+      <c r="D23" s="60" t="s">
+        <v>236</v>
+      </c>
+      <c r="E23" s="61"/>
+      <c r="F23" s="61"/>
+      <c r="G23" s="62"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D19:G19"/>
+  <mergeCells count="3">
+    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B9:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
** Controleur v1.10.3 **
- Indépendance des contrôles 10,11,38
- Modification de la lecture des C7 suite à la demande de Claude
</commit_message>
<xml_diff>
--- a/Documentation/Controleur.xlsx
+++ b/Documentation/Controleur.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="8370" yWindow="1320" windowWidth="6915" windowHeight="6540"/>
+    <workbookView xWindow="8370" yWindow="1320" windowWidth="6915" windowHeight="6540" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Controleur CA" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1907" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1877" uniqueCount="238">
   <si>
     <t>Famille</t>
   </si>
@@ -1481,6 +1481,9 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1498,9 +1501,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1814,8 +1814,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:R59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K59" sqref="A1:K59"/>
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1913,7 +1913,7 @@
       <c r="C3" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="76" t="s">
+      <c r="D3" s="70" t="s">
         <v>119</v>
       </c>
       <c r="E3" s="23" t="s">
@@ -1946,7 +1946,7 @@
       <c r="C4" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="76" t="s">
+      <c r="D4" s="70" t="s">
         <v>45</v>
       </c>
       <c r="E4" s="23" t="s">
@@ -2012,7 +2012,7 @@
       <c r="C6" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="76" t="s">
+      <c r="D6" s="70" t="s">
         <v>120</v>
       </c>
       <c r="E6" s="23" t="s">
@@ -9670,8 +9670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:M58"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25:M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10113,36 +10113,16 @@
         <f>'Controleur CA'!F12</f>
         <v>Vérifier que l'appui est présent dans la C7 si la colonne M ou N contient l'une des valeurs suivantes "oui remplacement appui" ou "oui renforcement appui avec commande d'appui"</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>48</v>
-      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
     </row>
     <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -10672,36 +10652,16 @@
         <f>'Controleur CA'!F25</f>
         <v>Vérifier que le nom des fiches poteau sont au format insee_nom</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="L25" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="M25" s="2" t="s">
-        <v>48</v>
-      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
     </row>
     <row r="26" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
@@ -10991,36 +10951,16 @@
         <f>'Controleur CA'!F38</f>
         <v>Vérifier que le numéro d'appui dans la C7 est sous la forme insee_identifiant</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="L38" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="M38" s="2" t="s">
-        <v>48</v>
-      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="17">
@@ -13412,7 +13352,7 @@
   <sheetData>
     <row r="8" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="2:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="73" t="s">
+      <c r="B9" s="74" t="s">
         <v>231</v>
       </c>
       <c r="C9" s="45" t="s">
@@ -13432,7 +13372,7 @@
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="75"/>
+      <c r="B10" s="76"/>
       <c r="C10" s="46" t="s">
         <v>7</v>
       </c>
@@ -13454,7 +13394,7 @@
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="75"/>
+      <c r="B11" s="76"/>
       <c r="C11" s="47" t="s">
         <v>91</v>
       </c>
@@ -13476,7 +13416,7 @@
       </c>
     </row>
     <row r="12" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="75"/>
+      <c r="B12" s="76"/>
       <c r="C12" s="48" t="s">
         <v>136</v>
       </c>
@@ -13498,7 +13438,7 @@
       </c>
     </row>
     <row r="13" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="75"/>
+      <c r="B13" s="76"/>
       <c r="C13" s="49"/>
       <c r="D13" s="43"/>
       <c r="E13" s="34"/>
@@ -13506,7 +13446,7 @@
       <c r="G13" s="58"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="75"/>
+      <c r="B14" s="76"/>
       <c r="C14" s="50" t="s">
         <v>191</v>
       </c>
@@ -13525,7 +13465,7 @@
       </c>
     </row>
     <row r="15" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="75"/>
+      <c r="B15" s="76"/>
       <c r="C15" s="51" t="s">
         <v>225</v>
       </c>
@@ -13544,7 +13484,7 @@
       </c>
     </row>
     <row r="16" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="75"/>
+      <c r="B16" s="76"/>
       <c r="C16" s="49"/>
       <c r="D16" s="43"/>
       <c r="E16" s="34"/>
@@ -13552,7 +13492,7 @@
       <c r="G16" s="58"/>
     </row>
     <row r="17" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="74"/>
+      <c r="B17" s="75"/>
       <c r="C17" s="52" t="s">
         <v>191</v>
       </c>
@@ -13582,7 +13522,7 @@
     </row>
     <row r="19" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="2:7" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="73" t="s">
+      <c r="B20" s="74" t="s">
         <v>232</v>
       </c>
       <c r="C20" s="62" t="s">
@@ -13600,7 +13540,7 @@
       </c>
     </row>
     <row r="21" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="74"/>
+      <c r="B21" s="75"/>
       <c r="C21" s="61"/>
       <c r="D21" s="33">
         <v>48</v>
@@ -13619,12 +13559,12 @@
       <c r="C23" s="53" t="s">
         <v>197</v>
       </c>
-      <c r="D23" s="70" t="s">
+      <c r="D23" s="71" t="s">
         <v>233</v>
       </c>
-      <c r="E23" s="71"/>
-      <c r="F23" s="71"/>
-      <c r="G23" s="72"/>
+      <c r="E23" s="72"/>
+      <c r="F23" s="72"/>
+      <c r="G23" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>